<commit_message>
agregado de etiqueta 121 tapa bife block jabat
</commit_message>
<xml_diff>
--- a/Copia de Copia de Codigos CHABAT NICO.xlsx
+++ b/Copia de Copia de Codigos CHABAT NICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{337A8B92-5B3A-4E8C-B8CE-5D0F1831432B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B3042DA-0A71-4B0A-BF1F-FF6CC22F8494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="196">
   <si>
     <t>לשון בקר קפוא</t>
   </si>
@@ -1552,8 +1552,8 @@
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N23" sqref="N23"/>
+      <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2662,8 +2662,12 @@
       <c r="L27" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="M27" s="78"/>
-      <c r="N27" s="78"/>
+      <c r="M27" s="78">
+        <v>121</v>
+      </c>
+      <c r="N27" s="78" t="s">
+        <v>195</v>
+      </c>
       <c r="O27" s="76"/>
     </row>
     <row r="28" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3187,6 +3191,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="מסמך" ma:contentTypeID="0x010100E111FB68E4AB3A458E6F1E68F8888CED" ma:contentTypeVersion="13" ma:contentTypeDescription="צור מסמך חדש." ma:contentTypeScope="" ma:versionID="bfe1cfa8ea064de69b4e2203b8e1e509">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4613b05c-4671-4207-a6b8-e30994dce502" xmlns:ns3="ae89acfa-0242-4570-84ca-e3aafb74daca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b8d078cf0bd54969afc6a4d318ee940" ns2:_="" ns3:_="">
     <xsd:import namespace="4613b05c-4671-4207-a6b8-e30994dce502"/>
@@ -3409,15 +3422,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3430,6 +3434,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A9BCE7-9EE4-4695-9AF6-872741DC1E3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3448,14 +3460,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
agregado de etiqueta 120 TAPA DE AGUJA jabat. FALTA TRADUCCION
</commit_message>
<xml_diff>
--- a/Copia de Copia de Codigos CHABAT NICO.xlsx
+++ b/Copia de Copia de Codigos CHABAT NICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B3042DA-0A71-4B0A-BF1F-FF6CC22F8494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3409C3BF-4ECF-4032-99B3-4F99BF6CBA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="196">
   <si>
     <t>לשון בקר קפוא</t>
   </si>
@@ -1552,8 +1552,8 @@
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N28" sqref="N28"/>
+      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2418,8 +2418,12 @@
       <c r="L21" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="M21" s="78"/>
-      <c r="N21" s="78"/>
+      <c r="M21" s="78">
+        <v>120</v>
+      </c>
+      <c r="N21" s="78" t="s">
+        <v>190</v>
+      </c>
       <c r="O21" s="76"/>
     </row>
     <row r="22" spans="1:15" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3191,15 +3195,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="מסמך" ma:contentTypeID="0x010100E111FB68E4AB3A458E6F1E68F8888CED" ma:contentTypeVersion="13" ma:contentTypeDescription="צור מסמך חדש." ma:contentTypeScope="" ma:versionID="bfe1cfa8ea064de69b4e2203b8e1e509">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4613b05c-4671-4207-a6b8-e30994dce502" xmlns:ns3="ae89acfa-0242-4570-84ca-e3aafb74daca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b8d078cf0bd54969afc6a4d318ee940" ns2:_="" ns3:_="">
     <xsd:import namespace="4613b05c-4671-4207-a6b8-e30994dce502"/>
@@ -3422,6 +3417,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3434,14 +3438,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A9BCE7-9EE4-4695-9AF6-872741DC1E3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3460,6 +3456,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
agregado de etiqueta 110 GRASA jabat
</commit_message>
<xml_diff>
--- a/Copia de Copia de Codigos CHABAT NICO.xlsx
+++ b/Copia de Copia de Codigos CHABAT NICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3409C3BF-4ECF-4032-99B3-4F99BF6CBA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4F4F6A-C2CE-41A0-8E3B-B8C35D05C280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="196">
   <si>
     <t>לשון בקר קפוא</t>
   </si>
@@ -1552,8 +1552,8 @@
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K21" sqref="K21"/>
+      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2824,8 +2824,12 @@
       <c r="L31" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="M31" s="78"/>
-      <c r="N31" s="78"/>
+      <c r="M31" s="78">
+        <v>110</v>
+      </c>
+      <c r="N31" s="78" t="s">
+        <v>195</v>
+      </c>
       <c r="O31" s="76"/>
     </row>
     <row r="32" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3195,6 +3199,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="מסמך" ma:contentTypeID="0x010100E111FB68E4AB3A458E6F1E68F8888CED" ma:contentTypeVersion="13" ma:contentTypeDescription="צור מסמך חדש." ma:contentTypeScope="" ma:versionID="bfe1cfa8ea064de69b4e2203b8e1e509">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4613b05c-4671-4207-a6b8-e30994dce502" xmlns:ns3="ae89acfa-0242-4570-84ca-e3aafb74daca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b8d078cf0bd54969afc6a4d318ee940" ns2:_="" ns3:_="">
     <xsd:import namespace="4613b05c-4671-4207-a6b8-e30994dce502"/>
@@ -3417,15 +3430,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3438,6 +3442,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A9BCE7-9EE4-4695-9AF6-872741DC1E3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3456,14 +3468,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
agregado de etiqueta 111 PALETA 4 JABAT - FALTA TRADUCCION
</commit_message>
<xml_diff>
--- a/Copia de Copia de Codigos CHABAT NICO.xlsx
+++ b/Copia de Copia de Codigos CHABAT NICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4F4F6A-C2CE-41A0-8E3B-B8C35D05C280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9314569C-11A9-4E2A-9306-90FDD203CB4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="196">
   <si>
     <t>לשון בקר קפוא</t>
   </si>
@@ -1552,8 +1552,8 @@
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N31" sqref="N31"/>
+      <pane ySplit="3" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2252,8 +2252,12 @@
       <c r="L17" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="M17" s="78"/>
-      <c r="N17" s="78"/>
+      <c r="M17" s="78">
+        <v>111</v>
+      </c>
+      <c r="N17" s="78" t="s">
+        <v>190</v>
+      </c>
       <c r="O17" s="76"/>
     </row>
     <row r="18" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3199,15 +3203,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="מסמך" ma:contentTypeID="0x010100E111FB68E4AB3A458E6F1E68F8888CED" ma:contentTypeVersion="13" ma:contentTypeDescription="צור מסמך חדש." ma:contentTypeScope="" ma:versionID="bfe1cfa8ea064de69b4e2203b8e1e509">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4613b05c-4671-4207-a6b8-e30994dce502" xmlns:ns3="ae89acfa-0242-4570-84ca-e3aafb74daca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b8d078cf0bd54969afc6a4d318ee940" ns2:_="" ns3:_="">
     <xsd:import namespace="4613b05c-4671-4207-a6b8-e30994dce502"/>
@@ -3430,6 +3425,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3442,14 +3446,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A9BCE7-9EE4-4695-9AF6-872741DC1E3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3468,6 +3464,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
REVISION de etiqueta 100 AGUJA JABAT - FALTA TRADUCCION
</commit_message>
<xml_diff>
--- a/Copia de Copia de Codigos CHABAT NICO.xlsx
+++ b/Copia de Copia de Codigos CHABAT NICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9314569C-11A9-4E2A-9306-90FDD203CB4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{528B91EB-1C21-46A5-97A9-8171FDE2A9A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="196">
   <si>
     <t>לשון בקר קפוא</t>
   </si>
@@ -1553,7 +1553,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M18" sqref="M18"/>
+      <selection pane="bottomLeft" activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1870,7 +1870,9 @@
       <c r="M8" s="78">
         <v>100</v>
       </c>
-      <c r="N8" s="78"/>
+      <c r="N8" s="78" t="s">
+        <v>190</v>
+      </c>
       <c r="O8" s="76" t="s">
         <v>190</v>
       </c>
@@ -3203,6 +3205,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="מסמך" ma:contentTypeID="0x010100E111FB68E4AB3A458E6F1E68F8888CED" ma:contentTypeVersion="13" ma:contentTypeDescription="צור מסמך חדש." ma:contentTypeScope="" ma:versionID="bfe1cfa8ea064de69b4e2203b8e1e509">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4613b05c-4671-4207-a6b8-e30994dce502" xmlns:ns3="ae89acfa-0242-4570-84ca-e3aafb74daca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b8d078cf0bd54969afc6a4d318ee940" ns2:_="" ns3:_="">
     <xsd:import namespace="4613b05c-4671-4207-a6b8-e30994dce502"/>
@@ -3425,15 +3436,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3446,6 +3448,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A9BCE7-9EE4-4695-9AF6-872741DC1E3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3464,14 +3474,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
REVISION de etiqueta 103 BRAZUELO JABAT OK
</commit_message>
<xml_diff>
--- a/Copia de Copia de Codigos CHABAT NICO.xlsx
+++ b/Copia de Copia de Codigos CHABAT NICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{528B91EB-1C21-46A5-97A9-8171FDE2A9A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C25583-19C6-418C-99AE-71AA902C4A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1553,7 +1553,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N8" sqref="N8"/>
+      <selection pane="bottomLeft" activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -3205,15 +3205,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="מסמך" ma:contentTypeID="0x010100E111FB68E4AB3A458E6F1E68F8888CED" ma:contentTypeVersion="13" ma:contentTypeDescription="צור מסמך חדש." ma:contentTypeScope="" ma:versionID="bfe1cfa8ea064de69b4e2203b8e1e509">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4613b05c-4671-4207-a6b8-e30994dce502" xmlns:ns3="ae89acfa-0242-4570-84ca-e3aafb74daca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b8d078cf0bd54969afc6a4d318ee940" ns2:_="" ns3:_="">
     <xsd:import namespace="4613b05c-4671-4207-a6b8-e30994dce502"/>
@@ -3436,6 +3427,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3448,14 +3448,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A9BCE7-9EE4-4695-9AF6-872741DC1E3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3474,6 +3466,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
agregado de etiqueta 112 COGOTE BLOKE 10B JABAT - FALTA TRADUCCION
</commit_message>
<xml_diff>
--- a/Copia de Copia de Codigos CHABAT NICO.xlsx
+++ b/Copia de Copia de Codigos CHABAT NICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C25583-19C6-418C-99AE-71AA902C4A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E51E9433-6192-4E12-869A-2EB1EBB7A2D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="196">
   <si>
     <t>לשון בקר קפוא</t>
   </si>
@@ -1552,8 +1552,8 @@
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K22" sqref="K22"/>
+      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1565,7 +1565,7 @@
     <col min="5" max="5" width="39.5703125" style="44" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="12.85546875" style="5" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.85546875" style="5" customWidth="1"/>
     <col min="9" max="9" width="16.7109375" style="4" customWidth="1"/>
     <col min="10" max="10" width="11" style="61" customWidth="1"/>
     <col min="11" max="11" width="30.5703125" style="43" bestFit="1" customWidth="1"/>
@@ -2551,8 +2551,12 @@
       <c r="L24" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="M24" s="78"/>
-      <c r="N24" s="78"/>
+      <c r="M24" s="78">
+        <v>112</v>
+      </c>
+      <c r="N24" s="78" t="s">
+        <v>190</v>
+      </c>
       <c r="O24" s="76"/>
     </row>
     <row r="25" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3205,6 +3209,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="מסמך" ma:contentTypeID="0x010100E111FB68E4AB3A458E6F1E68F8888CED" ma:contentTypeVersion="13" ma:contentTypeDescription="צור מסמך חדש." ma:contentTypeScope="" ma:versionID="bfe1cfa8ea064de69b4e2203b8e1e509">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4613b05c-4671-4207-a6b8-e30994dce502" xmlns:ns3="ae89acfa-0242-4570-84ca-e3aafb74daca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b8d078cf0bd54969afc6a4d318ee940" ns2:_="" ns3:_="">
     <xsd:import namespace="4613b05c-4671-4207-a6b8-e30994dce502"/>
@@ -3427,15 +3440,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3448,6 +3452,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A9BCE7-9EE4-4695-9AF6-872741DC1E3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3466,14 +3478,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
agregado de etiqueta 170 OJO DE BIFE 18 MADURADO - JABAT
</commit_message>
<xml_diff>
--- a/Copia de Copia de Codigos CHABAT NICO.xlsx
+++ b/Copia de Copia de Codigos CHABAT NICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E51E9433-6192-4E12-869A-2EB1EBB7A2D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2CB700-9C40-4183-90EC-E14EE777D074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="196">
   <si>
     <t>לשון בקר קפוא</t>
   </si>
@@ -1552,8 +1552,8 @@
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O24" sqref="O24"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1698,8 +1698,12 @@
       <c r="L4" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="M4" s="78"/>
-      <c r="N4" s="78"/>
+      <c r="M4" s="78">
+        <v>171</v>
+      </c>
+      <c r="N4" s="78" t="s">
+        <v>195</v>
+      </c>
       <c r="O4" s="76">
         <v>171</v>
       </c>
@@ -1744,8 +1748,12 @@
       <c r="L5" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="M5" s="78"/>
-      <c r="N5" s="78"/>
+      <c r="M5" s="78">
+        <v>170</v>
+      </c>
+      <c r="N5" s="78" t="s">
+        <v>195</v>
+      </c>
       <c r="O5" s="76">
         <v>170</v>
       </c>
@@ -3209,15 +3217,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="מסמך" ma:contentTypeID="0x010100E111FB68E4AB3A458E6F1E68F8888CED" ma:contentTypeVersion="13" ma:contentTypeDescription="צור מסמך חדש." ma:contentTypeScope="" ma:versionID="bfe1cfa8ea064de69b4e2203b8e1e509">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4613b05c-4671-4207-a6b8-e30994dce502" xmlns:ns3="ae89acfa-0242-4570-84ca-e3aafb74daca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b8d078cf0bd54969afc6a4d318ee940" ns2:_="" ns3:_="">
     <xsd:import namespace="4613b05c-4671-4207-a6b8-e30994dce502"/>
@@ -3440,6 +3439,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3452,14 +3460,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A9BCE7-9EE4-4695-9AF6-872741DC1E3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3478,6 +3478,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
agregado de etiqueta 130 AGUJA E TROZOS 22 - JABAT
</commit_message>
<xml_diff>
--- a/Copia de Copia de Codigos CHABAT NICO.xlsx
+++ b/Copia de Copia de Codigos CHABAT NICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2CB700-9C40-4183-90EC-E14EE777D074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92544B0E-38F1-4F66-B00F-49C775EB6AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="196">
   <si>
     <t>לשון בקר קפוא</t>
   </si>
@@ -1553,7 +1553,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M4" sqref="M4"/>
+      <selection pane="bottomLeft" activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1834,8 +1834,12 @@
       <c r="L7" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="M7" s="78"/>
-      <c r="N7" s="78"/>
+      <c r="M7" s="78">
+        <v>100</v>
+      </c>
+      <c r="N7" s="78" t="s">
+        <v>190</v>
+      </c>
       <c r="O7" s="76" t="s">
         <v>190</v>
       </c>
@@ -1875,12 +1879,8 @@
       <c r="L8" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="M8" s="78">
-        <v>100</v>
-      </c>
-      <c r="N8" s="78" t="s">
-        <v>190</v>
-      </c>
+      <c r="M8" s="78"/>
+      <c r="N8" s="78"/>
       <c r="O8" s="76" t="s">
         <v>190</v>
       </c>
@@ -1965,8 +1965,12 @@
       <c r="L10" s="73" t="s">
         <v>169</v>
       </c>
-      <c r="M10" s="79"/>
-      <c r="N10" s="79"/>
+      <c r="M10" s="79">
+        <v>130</v>
+      </c>
+      <c r="N10" s="79" t="s">
+        <v>195</v>
+      </c>
       <c r="O10" s="76">
         <v>130</v>
       </c>
@@ -3217,6 +3221,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="מסמך" ma:contentTypeID="0x010100E111FB68E4AB3A458E6F1E68F8888CED" ma:contentTypeVersion="13" ma:contentTypeDescription="צור מסמך חדש." ma:contentTypeScope="" ma:versionID="bfe1cfa8ea064de69b4e2203b8e1e509">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4613b05c-4671-4207-a6b8-e30994dce502" xmlns:ns3="ae89acfa-0242-4570-84ca-e3aafb74daca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b8d078cf0bd54969afc6a4d318ee940" ns2:_="" ns3:_="">
     <xsd:import namespace="4613b05c-4671-4207-a6b8-e30994dce502"/>
@@ -3439,15 +3452,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3460,6 +3464,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A9BCE7-9EE4-4695-9AF6-872741DC1E3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3478,14 +3490,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
agregado de etiqueta 181 asado 9 costillas ch -jabat. falta traduccion
</commit_message>
<xml_diff>
--- a/Copia de Copia de Codigos CHABAT NICO.xlsx
+++ b/Copia de Copia de Codigos CHABAT NICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92544B0E-38F1-4F66-B00F-49C775EB6AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46960F5B-3409-4149-9F1F-51914C4F3F41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="196">
   <si>
     <t>לשון בקר קפוא</t>
   </si>
@@ -1552,8 +1552,8 @@
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M11" sqref="M11"/>
+      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2772,8 +2772,12 @@
       <c r="L29" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="M29" s="78"/>
-      <c r="N29" s="78"/>
+      <c r="M29" s="78">
+        <v>181</v>
+      </c>
+      <c r="N29" s="78" t="s">
+        <v>190</v>
+      </c>
       <c r="O29" s="76"/>
     </row>
     <row r="30" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3221,15 +3225,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="מסמך" ma:contentTypeID="0x010100E111FB68E4AB3A458E6F1E68F8888CED" ma:contentTypeVersion="13" ma:contentTypeDescription="צור מסמך חדש." ma:contentTypeScope="" ma:versionID="bfe1cfa8ea064de69b4e2203b8e1e509">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4613b05c-4671-4207-a6b8-e30994dce502" xmlns:ns3="ae89acfa-0242-4570-84ca-e3aafb74daca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b8d078cf0bd54969afc6a4d318ee940" ns2:_="" ns3:_="">
     <xsd:import namespace="4613b05c-4671-4207-a6b8-e30994dce502"/>
@@ -3452,6 +3447,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3464,14 +3468,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A9BCE7-9EE4-4695-9AF6-872741DC1E3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3490,6 +3486,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
agregado de etiqueta 174 cogote 10 - JABAT
</commit_message>
<xml_diff>
--- a/Copia de Copia de Codigos CHABAT NICO.xlsx
+++ b/Copia de Copia de Codigos CHABAT NICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46960F5B-3409-4149-9F1F-51914C4F3F41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6033899-02C1-4FAF-89C1-64A179A9738F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="196">
   <si>
     <t>לשון בקר קפוא</t>
   </si>
@@ -1552,8 +1552,8 @@
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O29" sqref="O29"/>
+      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2649,8 +2649,12 @@
       <c r="L26" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="M26" s="78"/>
-      <c r="N26" s="78"/>
+      <c r="M26" s="78">
+        <v>174</v>
+      </c>
+      <c r="N26" s="78" t="s">
+        <v>195</v>
+      </c>
       <c r="O26" s="76"/>
     </row>
     <row r="27" spans="1:15" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3225,6 +3229,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="מסמך" ma:contentTypeID="0x010100E111FB68E4AB3A458E6F1E68F8888CED" ma:contentTypeVersion="13" ma:contentTypeDescription="צור מסמך חדש." ma:contentTypeScope="" ma:versionID="bfe1cfa8ea064de69b4e2203b8e1e509">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4613b05c-4671-4207-a6b8-e30994dce502" xmlns:ns3="ae89acfa-0242-4570-84ca-e3aafb74daca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b8d078cf0bd54969afc6a4d318ee940" ns2:_="" ns3:_="">
     <xsd:import namespace="4613b05c-4671-4207-a6b8-e30994dce502"/>
@@ -3447,15 +3460,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3468,6 +3472,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A9BCE7-9EE4-4695-9AF6-872741DC1E3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3486,14 +3498,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
agregado de etiqueta 187 ENTRECOSTILLA CH - JABAT. FALTA TRADUCCION
</commit_message>
<xml_diff>
--- a/Copia de Copia de Codigos CHABAT NICO.xlsx
+++ b/Copia de Copia de Codigos CHABAT NICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6033899-02C1-4FAF-89C1-64A179A9738F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E11CF7-0EAD-42C0-AAC6-1B297D451254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="199">
   <si>
     <t>לשון בקר קפוא</t>
   </si>
@@ -625,6 +625,15 @@
   </si>
   <si>
     <t>OK</t>
+  </si>
+  <si>
+    <t>van</t>
+  </si>
+  <si>
+    <t>falta traduccion</t>
+  </si>
+  <si>
+    <t>SIN VER</t>
   </si>
 </sst>
 </file>
@@ -977,7 +986,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1257,6 +1266,12 @@
     </xf>
     <xf numFmtId="44" fontId="4" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1552,8 +1567,8 @@
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N27" sqref="N27"/>
+      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2905,7 +2920,7 @@
       </c>
       <c r="O32" s="76"/>
     </row>
-    <row r="33" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="14"/>
       <c r="B33" s="15" t="s">
         <v>187</v>
@@ -2936,11 +2951,15 @@
       <c r="L33" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="M33" s="78"/>
-      <c r="N33" s="78"/>
+      <c r="M33" s="78">
+        <v>187</v>
+      </c>
+      <c r="N33" s="78" t="s">
+        <v>190</v>
+      </c>
       <c r="O33" s="76"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="14"/>
       <c r="B34" s="15" t="s">
         <v>187</v>
@@ -2977,7 +2996,7 @@
       <c r="N34" s="78"/>
       <c r="O34" s="76"/>
     </row>
-    <row r="35" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="33"/>
       <c r="B35" s="34" t="s">
         <v>187</v>
@@ -3014,7 +3033,7 @@
       <c r="N35" s="80"/>
       <c r="O35" s="76"/>
     </row>
-    <row r="36" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="33"/>
       <c r="B36" s="34" t="s">
         <v>187</v>
@@ -3051,7 +3070,7 @@
       <c r="N36" s="80"/>
       <c r="O36" s="76"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="33"/>
       <c r="B37" s="34" t="s">
         <v>187</v>
@@ -3089,8 +3108,15 @@
       <c r="M37" s="80"/>
       <c r="N37" s="80"/>
       <c r="O37" s="76"/>
-    </row>
-    <row r="38" spans="1:16" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P37" s="94" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q37" s="5">
+        <f>COUNTIF(N4:N38,"OK")</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="33"/>
       <c r="B38" s="34" t="s">
         <v>187</v>
@@ -3128,8 +3154,15 @@
       <c r="M38" s="81"/>
       <c r="N38" s="81"/>
       <c r="O38" s="76"/>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P38" s="95" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q38" s="5">
+        <f>COUNTIF(N4:N38,"FALTA")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="38"/>
       <c r="B39" s="39"/>
       <c r="C39" s="40"/>
@@ -3142,9 +3175,15 @@
       <c r="M39" s="5"/>
       <c r="N39" s="5"/>
       <c r="O39" s="70"/>
-      <c r="P39" s="5"/>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P39" s="94" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q39" s="5">
+        <f>COUNTIF(N4:N38,"")</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="56" t="s">
         <v>50</v>
       </c>
@@ -3156,12 +3195,10 @@
       <c r="J40" s="5"/>
       <c r="K40" s="5"/>
       <c r="L40" s="5"/>
-      <c r="M40" s="5"/>
-      <c r="N40" s="5"/>
       <c r="O40" s="70"/>
       <c r="P40" s="5"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="56" t="s">
         <v>48</v>
       </c>
@@ -3174,11 +3211,11 @@
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
       <c r="M41" s="5"/>
-      <c r="N41" s="5"/>
+      <c r="N41"/>
       <c r="O41" s="70"/>
       <c r="P41" s="5"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="56" t="s">
         <v>49</v>
       </c>
@@ -3195,7 +3232,7 @@
       <c r="O42" s="70"/>
       <c r="P42" s="5"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="65" t="s">
         <v>51</v>
       </c>
@@ -3229,15 +3266,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="מסמך" ma:contentTypeID="0x010100E111FB68E4AB3A458E6F1E68F8888CED" ma:contentTypeVersion="13" ma:contentTypeDescription="צור מסמך חדש." ma:contentTypeScope="" ma:versionID="bfe1cfa8ea064de69b4e2203b8e1e509">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4613b05c-4671-4207-a6b8-e30994dce502" xmlns:ns3="ae89acfa-0242-4570-84ca-e3aafb74daca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b8d078cf0bd54969afc6a4d318ee940" ns2:_="" ns3:_="">
     <xsd:import namespace="4613b05c-4671-4207-a6b8-e30994dce502"/>
@@ -3460,6 +3488,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3472,14 +3509,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A9BCE7-9EE4-4695-9AF6-872741DC1E3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3498,6 +3527,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
se agrego etiqueta 172 pecho trz 33 jabat
</commit_message>
<xml_diff>
--- a/Copia de Copia de Codigos CHABAT NICO.xlsx
+++ b/Copia de Copia de Codigos CHABAT NICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E11CF7-0EAD-42C0-AAC6-1B297D451254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B7AA81-38F3-4C2E-B92E-0733FBF65D07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="201">
   <si>
     <t>לשון בקר קפוא</t>
   </si>
@@ -634,6 +634,12 @@
   </si>
   <si>
     <t>SIN VER</t>
+  </si>
+  <si>
+    <t>DE CERO</t>
+  </si>
+  <si>
+    <t>CERO</t>
   </si>
 </sst>
 </file>
@@ -1231,6 +1237,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1266,12 +1278,6 @@
     </xf>
     <xf numFmtId="44" fontId="4" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1566,9 +1572,9 @@
   </sheetPr>
   <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J28" sqref="J28"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1588,7 +1594,8 @@
     <col min="13" max="14" width="12.42578125" style="4" customWidth="1"/>
     <col min="15" max="15" width="18.28515625" style="69" customWidth="1"/>
     <col min="16" max="16" width="19.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="11.42578125" style="4"/>
+    <col min="17" max="17" width="11.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1604,31 +1611,31 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="90" t="s">
         <v>122</v>
       </c>
       <c r="B2" s="7"/>
-      <c r="C2" s="82" t="s">
+      <c r="C2" s="84" t="s">
         <v>104</v>
       </c>
-      <c r="D2" s="86" t="s">
+      <c r="D2" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="86" t="s">
+      <c r="E2" s="88" t="s">
         <v>52</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-      <c r="H2" s="82" t="s">
+      <c r="H2" s="84" t="s">
         <v>113</v>
       </c>
-      <c r="I2" s="90" t="s">
+      <c r="I2" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="92" t="s">
+      <c r="J2" s="94" t="s">
         <v>123</v>
       </c>
-      <c r="K2" s="84" t="s">
+      <c r="K2" s="86" t="s">
         <v>20</v>
       </c>
       <c r="L2" s="2" t="s">
@@ -1641,25 +1648,25 @@
       </c>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="89"/>
+      <c r="A3" s="91"/>
       <c r="B3" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="83" t="s">
+      <c r="C3" s="85" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
       <c r="F3" s="9" t="s">
         <v>105</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="H3" s="83"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="87"/>
       <c r="L3" s="71" t="s">
         <v>168</v>
       </c>
@@ -1807,7 +1814,9 @@
         <v>173</v>
       </c>
       <c r="M6" s="78"/>
-      <c r="N6" s="78"/>
+      <c r="N6" s="78" t="s">
+        <v>200</v>
+      </c>
       <c r="O6" s="76" t="s">
         <v>190</v>
       </c>
@@ -1895,7 +1904,9 @@
         <v>169</v>
       </c>
       <c r="M8" s="78"/>
-      <c r="N8" s="78"/>
+      <c r="N8" s="78" t="s">
+        <v>200</v>
+      </c>
       <c r="O8" s="76" t="s">
         <v>190</v>
       </c>
@@ -1938,7 +1949,9 @@
         <v>169</v>
       </c>
       <c r="M9" s="78"/>
-      <c r="N9" s="78"/>
+      <c r="N9" s="78" t="s">
+        <v>200</v>
+      </c>
       <c r="O9" s="76" t="s">
         <v>190</v>
       </c>
@@ -2031,7 +2044,9 @@
         <v>169</v>
       </c>
       <c r="M11" s="78"/>
-      <c r="N11" s="78"/>
+      <c r="N11" s="78" t="s">
+        <v>200</v>
+      </c>
       <c r="O11" s="76"/>
     </row>
     <row r="12" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2071,8 +2086,12 @@
       <c r="L12" s="73" t="s">
         <v>169</v>
       </c>
-      <c r="M12" s="79"/>
-      <c r="N12" s="79"/>
+      <c r="M12" s="79">
+        <v>172</v>
+      </c>
+      <c r="N12" s="79" t="s">
+        <v>195</v>
+      </c>
       <c r="O12" s="76">
         <v>172</v>
       </c>
@@ -3069,6 +3088,13 @@
       <c r="M36" s="80"/>
       <c r="N36" s="80"/>
       <c r="O36" s="76"/>
+      <c r="P36" s="83" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q36" s="68">
+        <f>COUNTIF(N4:N38,"CERO")</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="33"/>
@@ -3108,12 +3134,12 @@
       <c r="M37" s="80"/>
       <c r="N37" s="80"/>
       <c r="O37" s="76"/>
-      <c r="P37" s="94" t="s">
+      <c r="P37" s="82" t="s">
         <v>196</v>
       </c>
       <c r="Q37" s="5">
         <f>COUNTIF(N4:N38,"OK")</f>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:17" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3154,7 +3180,7 @@
       <c r="M38" s="81"/>
       <c r="N38" s="81"/>
       <c r="O38" s="76"/>
-      <c r="P38" s="95" t="s">
+      <c r="P38" s="83" t="s">
         <v>197</v>
       </c>
       <c r="Q38" s="5">
@@ -3175,12 +3201,12 @@
       <c r="M39" s="5"/>
       <c r="N39" s="5"/>
       <c r="O39" s="70"/>
-      <c r="P39" s="94" t="s">
+      <c r="P39" s="82" t="s">
         <v>198</v>
       </c>
       <c r="Q39" s="5">
         <f>COUNTIF(N4:N38,"")</f>
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
agregado de etiqueta 182 asado sh 9C - jabat. falta traduccion
</commit_message>
<xml_diff>
--- a/Copia de Copia de Codigos CHABAT NICO.xlsx
+++ b/Copia de Copia de Codigos CHABAT NICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B7AA81-38F3-4C2E-B92E-0733FBF65D07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5945E6CF-674B-43BF-8097-65C58B1C9DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="201">
   <si>
     <t>לשון בקר קפוא</t>
   </si>
@@ -1573,8 +1573,8 @@
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M13" sqref="M13"/>
+      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2137,7 +2137,9 @@
         <v>169</v>
       </c>
       <c r="M13" s="78"/>
-      <c r="N13" s="78"/>
+      <c r="N13" s="78" t="s">
+        <v>200</v>
+      </c>
       <c r="O13" s="76"/>
     </row>
     <row r="14" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2223,7 +2225,9 @@
         <v>169</v>
       </c>
       <c r="M15" s="79"/>
-      <c r="N15" s="79"/>
+      <c r="N15" s="79" t="s">
+        <v>200</v>
+      </c>
       <c r="O15" s="76"/>
     </row>
     <row r="16" spans="1:17" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2262,7 +2266,9 @@
         <v>169</v>
       </c>
       <c r="M16" s="78"/>
-      <c r="N16" s="78"/>
+      <c r="N16" s="78" t="s">
+        <v>200</v>
+      </c>
       <c r="O16" s="76"/>
     </row>
     <row r="17" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2557,7 +2563,9 @@
         <v>169</v>
       </c>
       <c r="M23" s="78"/>
-      <c r="N23" s="78"/>
+      <c r="N23" s="78" t="s">
+        <v>200</v>
+      </c>
       <c r="O23" s="76"/>
     </row>
     <row r="24" spans="1:15" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2643,7 +2651,9 @@
         <v>173</v>
       </c>
       <c r="M25" s="78"/>
-      <c r="N25" s="78"/>
+      <c r="N25" s="78" t="s">
+        <v>200</v>
+      </c>
       <c r="O25" s="76"/>
     </row>
     <row r="26" spans="1:15" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2771,8 +2781,12 @@
       <c r="L28" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="M28" s="78"/>
-      <c r="N28" s="78"/>
+      <c r="M28" s="78">
+        <v>182</v>
+      </c>
+      <c r="N28" s="78" t="s">
+        <v>190</v>
+      </c>
       <c r="O28" s="76"/>
     </row>
     <row r="29" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2852,7 +2866,9 @@
         <v>169</v>
       </c>
       <c r="M30" s="78"/>
-      <c r="N30" s="78"/>
+      <c r="N30" s="78" t="s">
+        <v>200</v>
+      </c>
       <c r="O30" s="76"/>
     </row>
     <row r="31" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3093,7 +3109,7 @@
       </c>
       <c r="Q36" s="68">
         <f>COUNTIF(N4:N38,"CERO")</f>
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
@@ -3185,7 +3201,7 @@
       </c>
       <c r="Q38" s="5">
         <f>COUNTIF(N4:N38,"FALTA")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
@@ -3206,7 +3222,7 @@
       </c>
       <c r="Q39" s="5">
         <f>COUNTIF(N4:N38,"")</f>
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
@@ -3292,6 +3308,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="מסמך" ma:contentTypeID="0x010100E111FB68E4AB3A458E6F1E68F8888CED" ma:contentTypeVersion="13" ma:contentTypeDescription="צור מסמך חדש." ma:contentTypeScope="" ma:versionID="bfe1cfa8ea064de69b4e2203b8e1e509">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4613b05c-4671-4207-a6b8-e30994dce502" xmlns:ns3="ae89acfa-0242-4570-84ca-e3aafb74daca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b8d078cf0bd54969afc6a4d318ee940" ns2:_="" ns3:_="">
     <xsd:import namespace="4613b05c-4671-4207-a6b8-e30994dce502"/>
@@ -3514,27 +3550,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
+    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
+    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A9BCE7-9EE4-4695-9AF6-872741DC1E3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3551,24 +3587,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
-    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
-    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
agregado de etiqueta 179 HUESO MANO - jabat. falta traduccion
</commit_message>
<xml_diff>
--- a/Copia de Copia de Codigos CHABAT NICO.xlsx
+++ b/Copia de Copia de Codigos CHABAT NICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5945E6CF-674B-43BF-8097-65C58B1C9DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424F4B6A-56FF-493C-80B9-710BEEDCDFCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="201">
   <si>
     <t>לשון בקר קפוא</t>
   </si>
@@ -1573,8 +1573,8 @@
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L31" sqref="L31"/>
+      <pane ySplit="3" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2352,7 +2352,9 @@
         <v>169</v>
       </c>
       <c r="M18" s="79"/>
-      <c r="N18" s="79"/>
+      <c r="N18" s="79" t="s">
+        <v>200</v>
+      </c>
       <c r="O18" s="76"/>
     </row>
     <row r="19" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3027,8 +3029,12 @@
       <c r="L34" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="M34" s="78"/>
-      <c r="N34" s="78"/>
+      <c r="M34" s="78">
+        <v>179</v>
+      </c>
+      <c r="N34" s="78" t="s">
+        <v>190</v>
+      </c>
       <c r="O34" s="76"/>
     </row>
     <row r="35" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3109,7 +3115,7 @@
       </c>
       <c r="Q36" s="68">
         <f>COUNTIF(N4:N38,"CERO")</f>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
@@ -3201,7 +3207,7 @@
       </c>
       <c r="Q38" s="5">
         <f>COUNTIF(N4:N38,"FALTA")</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
@@ -3222,7 +3228,7 @@
       </c>
       <c r="Q39" s="5">
         <f>COUNTIF(N4:N38,"")</f>
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
@@ -3308,26 +3314,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="מסמך" ma:contentTypeID="0x010100E111FB68E4AB3A458E6F1E68F8888CED" ma:contentTypeVersion="13" ma:contentTypeDescription="צור מסמך חדש." ma:contentTypeScope="" ma:versionID="bfe1cfa8ea064de69b4e2203b8e1e509">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4613b05c-4671-4207-a6b8-e30994dce502" xmlns:ns3="ae89acfa-0242-4570-84ca-e3aafb74daca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b8d078cf0bd54969afc6a4d318ee940" ns2:_="" ns3:_="">
     <xsd:import namespace="4613b05c-4671-4207-a6b8-e30994dce502"/>
@@ -3550,27 +3536,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
-    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
-    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A9BCE7-9EE4-4695-9AF6-872741DC1E3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3587,4 +3573,24 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
+    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
+    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
agregado de traduccion a etiqueta 100 HE-AgujaTrozosS - jabat
</commit_message>
<xml_diff>
--- a/Copia de Copia de Codigos CHABAT NICO.xlsx
+++ b/Copia de Copia de Codigos CHABAT NICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424F4B6A-56FF-493C-80B9-710BEEDCDFCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D611FBA0-213D-4303-A5E3-322E73D8065C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -650,7 +650,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -746,6 +746,22 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="48"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="44"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -992,7 +1008,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1030,27 +1046,15 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
@@ -1069,12 +1073,6 @@
     <xf numFmtId="1" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1084,12 +1082,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="2"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1099,12 +1091,6 @@
     <xf numFmtId="1" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1120,9 +1106,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1243,16 +1226,52 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="2" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="2" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="3" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="2" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="4" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="4" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" readingOrder="2"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="4" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1572,27 +1591,27 @@
   </sheetPr>
   <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O34" sqref="O34"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="61.5" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" style="5" customWidth="1"/>
     <col min="3" max="3" width="16" style="5" customWidth="1"/>
     <col min="4" max="4" width="26.85546875" style="5" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="39.5703125" style="44" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="39.5703125" style="33" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="12.85546875" style="5" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="11" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26.85546875" style="5" customWidth="1"/>
     <col min="9" max="9" width="16.7109375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="11" style="61" customWidth="1"/>
-    <col min="11" max="11" width="30.5703125" style="43" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" style="50" customWidth="1"/>
+    <col min="11" max="11" width="119" style="74" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="12.42578125" style="4" customWidth="1"/>
-    <col min="15" max="15" width="18.28515625" style="69" customWidth="1"/>
+    <col min="15" max="15" width="18.28515625" style="58" customWidth="1"/>
     <col min="16" max="16" width="19.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="18" max="16384" width="11.42578125" style="4"/>
@@ -1604,86 +1623,86 @@
       </c>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
-      <c r="J1" s="60"/>
+      <c r="J1" s="49"/>
       <c r="K1" s="6"/>
       <c r="Q1" s="4" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="90" t="s">
+      <c r="A2" s="91" t="s">
         <v>122</v>
       </c>
       <c r="B2" s="7"/>
-      <c r="C2" s="84" t="s">
+      <c r="C2" s="85" t="s">
         <v>104</v>
       </c>
-      <c r="D2" s="88" t="s">
+      <c r="D2" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="88" t="s">
+      <c r="E2" s="89" t="s">
         <v>52</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-      <c r="H2" s="84" t="s">
+      <c r="H2" s="85" t="s">
         <v>113</v>
       </c>
-      <c r="I2" s="92" t="s">
+      <c r="I2" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="94" t="s">
+      <c r="J2" s="95" t="s">
         <v>123</v>
       </c>
-      <c r="K2" s="86" t="s">
+      <c r="K2" s="87" t="s">
         <v>20</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="M2" s="75"/>
-      <c r="N2" s="75"/>
-      <c r="Q2" s="67">
+      <c r="M2" s="64"/>
+      <c r="N2" s="64"/>
+      <c r="Q2" s="56">
         <v>45555</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="91"/>
+      <c r="A3" s="92"/>
       <c r="B3" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="85" t="s">
+      <c r="C3" s="86" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
       <c r="F3" s="9" t="s">
         <v>105</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="H3" s="85"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="95"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="71" t="s">
+      <c r="H3" s="86"/>
+      <c r="I3" s="94"/>
+      <c r="J3" s="96"/>
+      <c r="K3" s="88"/>
+      <c r="L3" s="60" t="s">
         <v>168</v>
       </c>
-      <c r="M3" s="77" t="s">
+      <c r="M3" s="66" t="s">
         <v>193</v>
       </c>
-      <c r="N3" s="77" t="s">
+      <c r="N3" s="66" t="s">
         <v>194</v>
       </c>
-      <c r="O3" s="76" t="s">
+      <c r="O3" s="65" t="s">
         <v>189</v>
       </c>
       <c r="Q3" s="4" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="1" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" s="1" customFormat="1" ht="57.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>171</v>
       </c>
@@ -1693,10 +1712,10 @@
       <c r="C4" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="45" t="s">
+      <c r="D4" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="46" t="s">
+      <c r="E4" s="35" t="s">
         <v>139</v>
       </c>
       <c r="F4" s="11" t="s">
@@ -1711,1519 +1730,1519 @@
       <c r="I4" s="12">
         <v>7290019570943</v>
       </c>
-      <c r="J4" s="62">
+      <c r="J4" s="51">
         <v>101861</v>
       </c>
-      <c r="K4" s="13" t="s">
+      <c r="K4" s="75" t="s">
         <v>91</v>
       </c>
-      <c r="L4" s="72" t="s">
+      <c r="L4" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M4" s="78">
+      <c r="M4" s="67">
         <v>171</v>
       </c>
-      <c r="N4" s="78" t="s">
+      <c r="N4" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="O4" s="76">
+      <c r="O4" s="65">
         <v>171</v>
       </c>
-      <c r="Q4" s="68" t="s">
+      <c r="Q4" s="57" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14">
+    <row r="5" spans="1:17" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
         <v>18</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="47" t="s">
+      <c r="D5" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="37" t="s">
         <v>139</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="H5" s="14" t="s">
         <v>172</v>
       </c>
       <c r="I5" s="12">
         <v>7290019570943</v>
       </c>
-      <c r="J5" s="62">
+      <c r="J5" s="51">
         <v>101862</v>
       </c>
-      <c r="K5" s="16" t="s">
+      <c r="K5" s="76" t="s">
         <v>91</v>
       </c>
-      <c r="L5" s="72" t="s">
+      <c r="L5" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M5" s="78">
+      <c r="M5" s="67">
         <v>170</v>
       </c>
-      <c r="N5" s="78" t="s">
+      <c r="N5" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="O5" s="76">
+      <c r="O5" s="65">
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="15" t="s">
+    <row r="6" spans="1:17" ht="57" x14ac:dyDescent="0.25">
+      <c r="A6" s="13"/>
+      <c r="B6" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="D6" s="47"/>
-      <c r="E6" s="48" t="s">
+      <c r="D6" s="36"/>
+      <c r="E6" s="37" t="s">
         <v>140</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="14" t="s">
         <v>59</v>
       </c>
       <c r="I6" s="12">
         <v>7290019570899</v>
       </c>
-      <c r="J6" s="62">
+      <c r="J6" s="51">
         <v>101865</v>
       </c>
-      <c r="K6" s="17" t="s">
+      <c r="K6" s="77" t="s">
         <v>54</v>
       </c>
-      <c r="L6" s="72" t="s">
+      <c r="L6" s="61" t="s">
         <v>173</v>
       </c>
-      <c r="M6" s="78"/>
-      <c r="N6" s="78" t="s">
+      <c r="M6" s="67"/>
+      <c r="N6" s="67" t="s">
         <v>200</v>
       </c>
-      <c r="O6" s="76" t="s">
+      <c r="O6" s="65" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14">
+    <row r="7" spans="1:17" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
         <v>2</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D7" s="47" t="s">
+      <c r="D7" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="48" t="s">
+      <c r="E7" s="37" t="s">
         <v>141</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="15">
         <v>7290019570882</v>
       </c>
-      <c r="J7" s="62">
+      <c r="J7" s="51">
         <v>102531</v>
       </c>
-      <c r="K7" s="19" t="s">
+      <c r="K7" s="78" t="s">
         <v>124</v>
       </c>
-      <c r="L7" s="72" t="s">
+      <c r="L7" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M7" s="78">
+      <c r="M7" s="67">
         <v>100</v>
       </c>
-      <c r="N7" s="78" t="s">
+      <c r="N7" s="67" t="s">
+        <v>195</v>
+      </c>
+      <c r="O7" s="65" t="s">
         <v>190</v>
       </c>
-      <c r="O7" s="76" t="s">
+    </row>
+    <row r="8" spans="1:17" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="H8" s="14"/>
+      <c r="I8" s="15">
+        <v>7290019570882</v>
+      </c>
+      <c r="J8" s="51">
+        <v>102532</v>
+      </c>
+      <c r="K8" s="78" t="s">
+        <v>125</v>
+      </c>
+      <c r="L8" s="61" t="s">
+        <v>169</v>
+      </c>
+      <c r="M8" s="67"/>
+      <c r="N8" s="67" t="s">
+        <v>200</v>
+      </c>
+      <c r="O8" s="65" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
+    <row r="9" spans="1:17" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="I9" s="15">
+        <v>7290019570882</v>
+      </c>
+      <c r="J9" s="51">
+        <v>102533</v>
+      </c>
+      <c r="K9" s="78" t="s">
+        <v>126</v>
+      </c>
+      <c r="L9" s="61" t="s">
+        <v>169</v>
+      </c>
+      <c r="M9" s="67"/>
+      <c r="N9" s="67" t="s">
+        <v>200</v>
+      </c>
+      <c r="O9" s="65" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+      <c r="A10" s="18">
         <v>22</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B10" s="19" t="s">
         <v>187</v>
       </c>
-      <c r="C8" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" s="47" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="48" t="s">
-        <v>142</v>
-      </c>
-      <c r="F8" s="15" t="s">
+      <c r="C10" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="39" t="s">
+        <v>144</v>
+      </c>
+      <c r="F10" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G10" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="H8" s="15"/>
-      <c r="I8" s="18">
+      <c r="H10" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="I10" s="21">
         <v>7290019570882</v>
       </c>
-      <c r="J8" s="62">
-        <v>102532</v>
-      </c>
-      <c r="K8" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="L8" s="72" t="s">
+      <c r="J10" s="52">
+        <v>102534</v>
+      </c>
+      <c r="K10" s="79" t="s">
+        <v>97</v>
+      </c>
+      <c r="L10" s="62" t="s">
         <v>169</v>
       </c>
-      <c r="M8" s="78"/>
-      <c r="N8" s="78" t="s">
-        <v>200</v>
-      </c>
-      <c r="O8" s="76" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>187</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="D9" s="47" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="48" t="s">
-        <v>143</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="G9" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="I9" s="18">
-        <v>7290019570882</v>
-      </c>
-      <c r="J9" s="62">
-        <v>102533</v>
-      </c>
-      <c r="K9" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="L9" s="72" t="s">
-        <v>169</v>
-      </c>
-      <c r="M9" s="78"/>
-      <c r="N9" s="78" t="s">
-        <v>200</v>
-      </c>
-      <c r="O9" s="76" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22">
-        <v>22</v>
-      </c>
-      <c r="B10" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="D10" s="49" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="50" t="s">
-        <v>144</v>
-      </c>
-      <c r="F10" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="G10" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="H10" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="I10" s="25">
-        <v>7290019570882</v>
-      </c>
-      <c r="J10" s="63">
-        <v>102534</v>
-      </c>
-      <c r="K10" s="26" t="s">
-        <v>97</v>
-      </c>
-      <c r="L10" s="73" t="s">
-        <v>169</v>
-      </c>
-      <c r="M10" s="79">
+      <c r="M10" s="68">
         <v>130</v>
       </c>
-      <c r="N10" s="79" t="s">
+      <c r="N10" s="68" t="s">
         <v>195</v>
       </c>
-      <c r="O10" s="76">
+      <c r="O10" s="65">
         <v>130</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
+    <row r="11" spans="1:17" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="17" t="s">
         <v>187</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D11" s="47" t="s">
+      <c r="D11" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="48" t="s">
+      <c r="E11" s="37" t="s">
         <v>145</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="H11" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="I11" s="18">
+      <c r="I11" s="15">
         <v>7290019570875</v>
       </c>
-      <c r="J11" s="62">
+      <c r="J11" s="51">
         <v>103521</v>
       </c>
-      <c r="K11" s="19" t="s">
+      <c r="K11" s="78" t="s">
         <v>127</v>
       </c>
-      <c r="L11" s="72" t="s">
+      <c r="L11" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M11" s="78"/>
-      <c r="N11" s="78" t="s">
+      <c r="M11" s="67"/>
+      <c r="N11" s="67" t="s">
         <v>200</v>
       </c>
-      <c r="O11" s="76"/>
-    </row>
-    <row r="12" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22">
+      <c r="O11" s="65"/>
+    </row>
+    <row r="12" spans="1:17" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+      <c r="A12" s="18">
         <v>33</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="19" t="s">
         <v>187</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="49" t="s">
+      <c r="D12" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="50" t="s">
+      <c r="E12" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="F12" s="24" t="s">
+      <c r="F12" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G12" s="24" t="s">
+      <c r="G12" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="H12" s="24" t="s">
+      <c r="H12" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="I12" s="25">
+      <c r="I12" s="21">
         <v>7290019570875</v>
       </c>
-      <c r="J12" s="63">
+      <c r="J12" s="52">
         <v>103522</v>
       </c>
-      <c r="K12" s="26" t="s">
+      <c r="K12" s="79" t="s">
         <v>128</v>
       </c>
-      <c r="L12" s="73" t="s">
+      <c r="L12" s="62" t="s">
         <v>169</v>
       </c>
-      <c r="M12" s="79">
+      <c r="M12" s="68">
         <v>172</v>
       </c>
-      <c r="N12" s="79" t="s">
+      <c r="N12" s="68" t="s">
         <v>195</v>
       </c>
-      <c r="O12" s="76">
+      <c r="O12" s="65">
         <v>172</v>
       </c>
       <c r="P12" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
+    <row r="13" spans="1:17" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="17" t="s">
         <v>187</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="D13" s="47" t="s">
+      <c r="D13" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="48" t="s">
+      <c r="E13" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="F13" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="G13" s="15" t="s">
+      <c r="G13" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="H13" s="15" t="s">
+      <c r="H13" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="I13" s="18">
+      <c r="I13" s="15">
         <v>7290019570875</v>
       </c>
-      <c r="J13" s="62">
+      <c r="J13" s="51">
         <v>103523</v>
       </c>
-      <c r="K13" s="19" t="s">
+      <c r="K13" s="78" t="s">
         <v>129</v>
       </c>
-      <c r="L13" s="72" t="s">
+      <c r="L13" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M13" s="78"/>
-      <c r="N13" s="78" t="s">
+      <c r="M13" s="67"/>
+      <c r="N13" s="67" t="s">
         <v>200</v>
       </c>
-      <c r="O13" s="76"/>
-    </row>
-    <row r="14" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="20">
+      <c r="O13" s="65"/>
+    </row>
+    <row r="14" spans="1:17" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+      <c r="A14" s="16">
         <v>3</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="17" t="s">
         <v>187</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D14" s="47" t="s">
+      <c r="D14" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="48" t="s">
+      <c r="E14" s="37" t="s">
         <v>147</v>
       </c>
-      <c r="F14" s="15" t="s">
+      <c r="F14" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="G14" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="H14" s="15" t="s">
+      <c r="H14" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="I14" s="18">
+      <c r="I14" s="15">
         <v>7290019570875</v>
       </c>
-      <c r="J14" s="62">
+      <c r="J14" s="51">
         <v>103524</v>
       </c>
-      <c r="K14" s="19" t="s">
+      <c r="K14" s="78" t="s">
         <v>130</v>
       </c>
-      <c r="L14" s="72" t="s">
+      <c r="L14" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M14" s="78">
+      <c r="M14" s="67">
         <v>104</v>
       </c>
-      <c r="N14" s="78" t="s">
+      <c r="N14" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="O14" s="76"/>
-    </row>
-    <row r="15" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="22">
+      <c r="O14" s="65"/>
+    </row>
+    <row r="15" spans="1:17" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+      <c r="A15" s="18">
         <v>44</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="19" t="s">
         <v>187</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="D15" s="49" t="s">
+      <c r="D15" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="50" t="s">
+      <c r="E15" s="39" t="s">
         <v>148</v>
       </c>
-      <c r="F15" s="24" t="s">
+      <c r="F15" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G15" s="24" t="s">
+      <c r="G15" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="H15" s="24" t="s">
+      <c r="H15" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="I15" s="25">
+      <c r="I15" s="21">
         <v>7290019570868</v>
       </c>
-      <c r="J15" s="63">
+      <c r="J15" s="52">
         <v>104521</v>
       </c>
-      <c r="K15" s="26" t="s">
+      <c r="K15" s="79" t="s">
         <v>131</v>
       </c>
-      <c r="L15" s="73" t="s">
+      <c r="L15" s="62" t="s">
         <v>169</v>
       </c>
-      <c r="M15" s="79"/>
-      <c r="N15" s="79" t="s">
+      <c r="M15" s="68"/>
+      <c r="N15" s="68" t="s">
         <v>200</v>
       </c>
-      <c r="O15" s="76"/>
-    </row>
-    <row r="16" spans="1:17" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
+      <c r="O15" s="65"/>
+    </row>
+    <row r="16" spans="1:17" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="17" t="s">
         <v>187</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="D16" s="47" t="s">
+      <c r="D16" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="48" t="s">
+      <c r="E16" s="37" t="s">
         <v>149</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="F16" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="G16" s="15" t="s">
+      <c r="G16" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="H16" s="15"/>
-      <c r="I16" s="18">
+      <c r="H16" s="14"/>
+      <c r="I16" s="15">
         <v>7290019570868</v>
       </c>
-      <c r="J16" s="62">
+      <c r="J16" s="51">
         <v>104522</v>
       </c>
-      <c r="K16" s="19" t="s">
+      <c r="K16" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="L16" s="72" t="s">
+      <c r="L16" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M16" s="78"/>
-      <c r="N16" s="78" t="s">
+      <c r="M16" s="67"/>
+      <c r="N16" s="67" t="s">
         <v>200</v>
       </c>
-      <c r="O16" s="76"/>
-    </row>
-    <row r="17" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="20">
+      <c r="O16" s="65"/>
+    </row>
+    <row r="17" spans="1:15" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+      <c r="A17" s="16">
         <v>4</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="17" t="s">
         <v>187</v>
       </c>
-      <c r="C17" s="66" t="s">
+      <c r="C17" s="55" t="s">
         <v>175</v>
       </c>
-      <c r="D17" s="47" t="s">
+      <c r="D17" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="48" t="s">
+      <c r="E17" s="37" t="s">
         <v>150</v>
       </c>
-      <c r="F17" s="15" t="s">
+      <c r="F17" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="G17" s="15" t="s">
+      <c r="G17" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="H17" s="15"/>
-      <c r="I17" s="18">
+      <c r="H17" s="14"/>
+      <c r="I17" s="15">
         <v>7290019570868</v>
       </c>
-      <c r="J17" s="62">
+      <c r="J17" s="51">
         <v>104523</v>
       </c>
-      <c r="K17" s="19" t="s">
+      <c r="K17" s="78" t="s">
         <v>133</v>
       </c>
-      <c r="L17" s="72" t="s">
+      <c r="L17" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M17" s="78">
+      <c r="M17" s="67">
         <v>111</v>
       </c>
-      <c r="N17" s="78" t="s">
+      <c r="N17" s="67" t="s">
         <v>190</v>
       </c>
-      <c r="O17" s="76"/>
-    </row>
-    <row r="18" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="22">
+      <c r="O17" s="65"/>
+    </row>
+    <row r="18" spans="1:15" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+      <c r="A18" s="18">
         <v>55</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="19" t="s">
         <v>187</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="D18" s="49" t="s">
+      <c r="D18" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="E18" s="50" t="s">
+      <c r="E18" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="F18" s="24" t="s">
+      <c r="F18" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G18" s="24" t="s">
+      <c r="G18" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="H18" s="24" t="s">
+      <c r="H18" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="I18" s="25">
+      <c r="I18" s="21">
         <v>7290019570851</v>
       </c>
-      <c r="J18" s="63">
+      <c r="J18" s="52">
         <v>105521</v>
       </c>
-      <c r="K18" s="26" t="s">
+      <c r="K18" s="79" t="s">
         <v>134</v>
       </c>
-      <c r="L18" s="73" t="s">
+      <c r="L18" s="62" t="s">
         <v>169</v>
       </c>
-      <c r="M18" s="79"/>
-      <c r="N18" s="79" t="s">
+      <c r="M18" s="68"/>
+      <c r="N18" s="68" t="s">
         <v>200</v>
       </c>
-      <c r="O18" s="76"/>
-    </row>
-    <row r="19" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14">
+      <c r="O18" s="65"/>
+    </row>
+    <row r="19" spans="1:15" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+      <c r="A19" s="13">
         <v>5</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="D19" s="47" t="s">
+      <c r="D19" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="48" t="s">
+      <c r="E19" s="37" t="s">
         <v>152</v>
       </c>
-      <c r="F19" s="15" t="s">
+      <c r="F19" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="G19" s="15" t="s">
+      <c r="G19" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="H19" s="15"/>
-      <c r="I19" s="18">
+      <c r="H19" s="14"/>
+      <c r="I19" s="15">
         <v>7290019570851</v>
       </c>
-      <c r="J19" s="62">
+      <c r="J19" s="51">
         <v>105522</v>
       </c>
-      <c r="K19" s="27" t="s">
+      <c r="K19" s="80" t="s">
         <v>92</v>
       </c>
-      <c r="L19" s="72" t="s">
+      <c r="L19" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M19" s="78">
+      <c r="M19" s="67">
         <v>101</v>
       </c>
-      <c r="N19" s="78" t="s">
+      <c r="N19" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="O19" s="76"/>
-    </row>
-    <row r="20" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14">
+      <c r="O19" s="65"/>
+    </row>
+    <row r="20" spans="1:15" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+      <c r="A20" s="13">
         <v>6</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="D20" s="47" t="s">
+      <c r="D20" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="48" t="s">
+      <c r="E20" s="37" t="s">
         <v>152</v>
       </c>
-      <c r="F20" s="15" t="s">
+      <c r="F20" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="G20" s="15" t="s">
+      <c r="G20" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="H20" s="15"/>
-      <c r="I20" s="18">
+      <c r="H20" s="14"/>
+      <c r="I20" s="15">
         <v>7290019570844</v>
       </c>
-      <c r="J20" s="62">
+      <c r="J20" s="51">
         <v>106521</v>
       </c>
-      <c r="K20" s="27" t="s">
+      <c r="K20" s="80" t="s">
         <v>93</v>
       </c>
-      <c r="L20" s="72" t="s">
+      <c r="L20" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M20" s="78">
+      <c r="M20" s="67">
         <v>102</v>
       </c>
-      <c r="N20" s="78" t="s">
+      <c r="N20" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="O20" s="76"/>
-    </row>
-    <row r="21" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
+      <c r="O20" s="65"/>
+    </row>
+    <row r="21" spans="1:15" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="D21" s="47" t="s">
+      <c r="D21" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="E21" s="48" t="s">
+      <c r="E21" s="37" t="s">
         <v>153</v>
       </c>
-      <c r="F21" s="15" t="s">
+      <c r="F21" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="G21" s="15" t="s">
+      <c r="G21" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="H21" s="15"/>
-      <c r="I21" s="18">
+      <c r="H21" s="14"/>
+      <c r="I21" s="15">
         <v>7290019570837</v>
       </c>
-      <c r="J21" s="62">
+      <c r="J21" s="51">
         <v>107521</v>
       </c>
-      <c r="K21" s="27" t="s">
+      <c r="K21" s="80" t="s">
         <v>94</v>
       </c>
-      <c r="L21" s="72" t="s">
+      <c r="L21" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M21" s="78">
+      <c r="M21" s="67">
         <v>120</v>
       </c>
-      <c r="N21" s="78" t="s">
+      <c r="N21" s="67" t="s">
         <v>190</v>
       </c>
-      <c r="O21" s="76"/>
-    </row>
-    <row r="22" spans="1:15" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="14">
+      <c r="O21" s="65"/>
+    </row>
+    <row r="22" spans="1:15" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+      <c r="A22" s="13">
         <v>8</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="D22" s="47" t="s">
+      <c r="D22" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="48" t="s">
+      <c r="E22" s="37" t="s">
         <v>154</v>
       </c>
-      <c r="F22" s="15" t="s">
+      <c r="F22" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="G22" s="15" t="s">
+      <c r="G22" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="H22" s="15" t="s">
+      <c r="H22" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="I22" s="18">
+      <c r="I22" s="15">
         <v>7290019570820</v>
       </c>
-      <c r="J22" s="62">
+      <c r="J22" s="51">
         <v>108521</v>
       </c>
-      <c r="K22" s="27" t="s">
+      <c r="K22" s="80" t="s">
         <v>95</v>
       </c>
-      <c r="L22" s="72" t="s">
+      <c r="L22" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M22" s="78">
+      <c r="M22" s="67">
         <v>103</v>
       </c>
-      <c r="N22" s="78" t="s">
+      <c r="N22" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="O22" s="76"/>
-    </row>
-    <row r="23" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="28"/>
-      <c r="B23" s="29" t="s">
+      <c r="O22" s="65"/>
+    </row>
+    <row r="23" spans="1:15" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+      <c r="A23" s="22"/>
+      <c r="B23" s="23" t="s">
         <v>187</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="D23" s="51"/>
-      <c r="E23" s="52" t="s">
+      <c r="D23" s="40"/>
+      <c r="E23" s="41" t="s">
         <v>155</v>
       </c>
-      <c r="F23" s="15" t="s">
+      <c r="F23" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="G23" s="15" t="s">
+      <c r="G23" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="H23" s="15" t="s">
+      <c r="H23" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="I23" s="30">
+      <c r="I23" s="24">
         <v>7290019570813</v>
       </c>
-      <c r="J23" s="62">
+      <c r="J23" s="51">
         <v>108522</v>
       </c>
-      <c r="K23" s="31" t="s">
+      <c r="K23" s="81" t="s">
         <v>96</v>
       </c>
-      <c r="L23" s="72" t="s">
+      <c r="L23" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M23" s="78"/>
-      <c r="N23" s="78" t="s">
+      <c r="M23" s="67"/>
+      <c r="N23" s="67" t="s">
         <v>200</v>
       </c>
-      <c r="O23" s="76"/>
-    </row>
-    <row r="24" spans="1:15" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="28" t="s">
+      <c r="O23" s="65"/>
+    </row>
+    <row r="24" spans="1:15" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+      <c r="A24" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="23" t="s">
         <v>187</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="C24" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="D24" s="53" t="s">
+      <c r="D24" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="52" t="s">
+      <c r="E24" s="41" t="s">
         <v>156</v>
       </c>
-      <c r="F24" s="15" t="s">
+      <c r="F24" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="G24" s="15" t="s">
+      <c r="G24" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="H24" s="15" t="s">
+      <c r="H24" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="I24" s="30">
+      <c r="I24" s="24">
         <v>7290019570806</v>
       </c>
-      <c r="J24" s="62">
+      <c r="J24" s="51">
         <v>110531</v>
       </c>
-      <c r="K24" s="32" t="s">
+      <c r="K24" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="L24" s="72" t="s">
+      <c r="L24" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M24" s="78">
+      <c r="M24" s="67">
         <v>112</v>
       </c>
-      <c r="N24" s="78" t="s">
+      <c r="N24" s="67" t="s">
         <v>190</v>
       </c>
-      <c r="O24" s="76"/>
-    </row>
-    <row r="25" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="20" t="s">
+      <c r="O24" s="65"/>
+    </row>
+    <row r="25" spans="1:15" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="17" t="s">
         <v>187</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="D25" s="47" t="s">
+      <c r="D25" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="E25" s="48" t="s">
+      <c r="E25" s="37" t="s">
         <v>157</v>
       </c>
-      <c r="F25" s="15" t="s">
+      <c r="F25" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="G25" s="15" t="s">
+      <c r="G25" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="H25" s="15" t="s">
+      <c r="H25" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="I25" s="18">
+      <c r="I25" s="15">
         <v>7290019570790</v>
       </c>
-      <c r="J25" s="62">
+      <c r="J25" s="51">
         <v>110532</v>
       </c>
-      <c r="K25" s="19" t="s">
+      <c r="K25" s="78" t="s">
         <v>135</v>
       </c>
-      <c r="L25" s="72" t="s">
+      <c r="L25" s="61" t="s">
         <v>173</v>
       </c>
-      <c r="M25" s="78"/>
-      <c r="N25" s="78" t="s">
+      <c r="M25" s="67"/>
+      <c r="N25" s="67" t="s">
         <v>200</v>
       </c>
-      <c r="O25" s="76"/>
-    </row>
-    <row r="26" spans="1:15" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="20">
+      <c r="O25" s="65"/>
+    </row>
+    <row r="26" spans="1:15" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+      <c r="A26" s="16">
         <v>10</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="17" t="s">
         <v>187</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="D26" s="47" t="s">
+      <c r="D26" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="E26" s="48" t="s">
+      <c r="E26" s="37" t="s">
         <v>158</v>
       </c>
-      <c r="F26" s="15" t="s">
+      <c r="F26" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="G26" s="15" t="s">
+      <c r="G26" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="H26" s="15" t="s">
+      <c r="H26" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="I26" s="18">
+      <c r="I26" s="15">
         <v>7290019570790</v>
       </c>
-      <c r="J26" s="62">
+      <c r="J26" s="51">
         <v>110533</v>
       </c>
-      <c r="K26" s="19" t="s">
+      <c r="K26" s="78" t="s">
         <v>136</v>
       </c>
-      <c r="L26" s="72" t="s">
+      <c r="L26" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M26" s="78">
+      <c r="M26" s="67">
         <v>174</v>
       </c>
-      <c r="N26" s="78" t="s">
+      <c r="N26" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="O26" s="76"/>
-    </row>
-    <row r="27" spans="1:15" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="s">
+      <c r="O26" s="65"/>
+    </row>
+    <row r="27" spans="1:15" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="D27" s="47" t="s">
+      <c r="D27" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="E27" s="48" t="s">
+      <c r="E27" s="37" t="s">
         <v>159</v>
       </c>
-      <c r="F27" s="15" t="s">
+      <c r="F27" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="G27" s="15" t="s">
+      <c r="G27" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="H27" s="15"/>
-      <c r="I27" s="18">
+      <c r="H27" s="14"/>
+      <c r="I27" s="15">
         <v>7290019570783</v>
       </c>
-      <c r="J27" s="62">
+      <c r="J27" s="51">
         <v>170521</v>
       </c>
-      <c r="K27" s="27" t="s">
+      <c r="K27" s="80" t="s">
         <v>98</v>
       </c>
-      <c r="L27" s="72" t="s">
+      <c r="L27" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M27" s="78">
+      <c r="M27" s="67">
         <v>121</v>
       </c>
-      <c r="N27" s="78" t="s">
+      <c r="N27" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="O27" s="76"/>
-    </row>
-    <row r="28" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="20">
+      <c r="O27" s="65"/>
+    </row>
+    <row r="28" spans="1:15" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+      <c r="A28" s="16">
         <v>99</v>
       </c>
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="17" t="s">
         <v>187</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="C28" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="D28" s="47" t="s">
+      <c r="D28" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="E28" s="48" t="s">
+      <c r="E28" s="37" t="s">
         <v>160</v>
       </c>
-      <c r="F28" s="15" t="s">
+      <c r="F28" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="G28" s="15" t="s">
+      <c r="G28" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="H28" s="15" t="s">
+      <c r="H28" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="I28" s="18">
+      <c r="I28" s="15">
         <v>7290019570776</v>
       </c>
-      <c r="J28" s="62">
+      <c r="J28" s="51">
         <v>109521</v>
       </c>
-      <c r="K28" s="19" t="s">
+      <c r="K28" s="78" t="s">
         <v>137</v>
       </c>
-      <c r="L28" s="72" t="s">
+      <c r="L28" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M28" s="78">
+      <c r="M28" s="67">
         <v>182</v>
       </c>
-      <c r="N28" s="78" t="s">
+      <c r="N28" s="67" t="s">
         <v>190</v>
       </c>
-      <c r="O28" s="76"/>
-    </row>
-    <row r="29" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="14">
+      <c r="O28" s="65"/>
+    </row>
+    <row r="29" spans="1:15" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+      <c r="A29" s="13">
         <v>9</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="C29" s="15" t="s">
+      <c r="C29" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="D29" s="47" t="s">
+      <c r="D29" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="E29" s="48" t="s">
+      <c r="E29" s="37" t="s">
         <v>161</v>
       </c>
-      <c r="F29" s="15" t="s">
+      <c r="F29" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="G29" s="15" t="s">
+      <c r="G29" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="H29" s="15"/>
-      <c r="I29" s="18">
+      <c r="H29" s="14"/>
+      <c r="I29" s="15">
         <v>7290019570776</v>
       </c>
-      <c r="J29" s="62">
+      <c r="J29" s="51">
         <v>109522</v>
       </c>
-      <c r="K29" s="27" t="s">
+      <c r="K29" s="80" t="s">
         <v>99</v>
       </c>
-      <c r="L29" s="72" t="s">
+      <c r="L29" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M29" s="78">
+      <c r="M29" s="67">
         <v>181</v>
       </c>
-      <c r="N29" s="78" t="s">
+      <c r="N29" s="67" t="s">
         <v>190</v>
       </c>
-      <c r="O29" s="76"/>
-    </row>
-    <row r="30" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
-      <c r="B30" s="15" t="s">
+      <c r="O29" s="65"/>
+    </row>
+    <row r="30" spans="1:15" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+      <c r="A30" s="13"/>
+      <c r="B30" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="C30" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="D30" s="47"/>
-      <c r="E30" s="48" t="s">
+      <c r="D30" s="36"/>
+      <c r="E30" s="37" t="s">
         <v>155</v>
       </c>
-      <c r="F30" s="15" t="s">
+      <c r="F30" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="G30" s="15" t="s">
+      <c r="G30" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="H30" s="15" t="s">
+      <c r="H30" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="I30" s="18">
+      <c r="I30" s="15">
         <v>7290019570769</v>
       </c>
-      <c r="J30" s="62">
+      <c r="J30" s="51">
         <v>109523</v>
       </c>
-      <c r="K30" s="31" t="s">
+      <c r="K30" s="81" t="s">
         <v>100</v>
       </c>
-      <c r="L30" s="72" t="s">
+      <c r="L30" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M30" s="78"/>
-      <c r="N30" s="78" t="s">
+      <c r="M30" s="67"/>
+      <c r="N30" s="67" t="s">
         <v>200</v>
       </c>
-      <c r="O30" s="76"/>
-    </row>
-    <row r="31" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="14"/>
-      <c r="B31" s="15" t="s">
+      <c r="O30" s="65"/>
+    </row>
+    <row r="31" spans="1:15" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+      <c r="A31" s="13"/>
+      <c r="B31" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="C31" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="D31" s="47" t="s">
+      <c r="D31" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="E31" s="48" t="s">
+      <c r="E31" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="F31" s="15" t="s">
+      <c r="F31" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="G31" s="15" t="s">
+      <c r="G31" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="H31" s="15"/>
-      <c r="I31" s="18">
+      <c r="H31" s="14"/>
+      <c r="I31" s="15">
         <v>7290019570752</v>
       </c>
-      <c r="J31" s="62">
+      <c r="J31" s="51">
         <v>157521</v>
       </c>
-      <c r="K31" s="27" t="s">
+      <c r="K31" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="L31" s="72" t="s">
+      <c r="L31" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M31" s="78">
+      <c r="M31" s="67">
         <v>110</v>
       </c>
-      <c r="N31" s="78" t="s">
+      <c r="N31" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="O31" s="76"/>
-    </row>
-    <row r="32" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
-      <c r="B32" s="15" t="s">
+      <c r="O31" s="65"/>
+    </row>
+    <row r="32" spans="1:15" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+      <c r="A32" s="13"/>
+      <c r="B32" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="C32" s="15" t="s">
+      <c r="C32" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="D32" s="47" t="s">
+      <c r="D32" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="E32" s="48" t="s">
+      <c r="E32" s="37" t="s">
         <v>163</v>
       </c>
-      <c r="F32" s="15" t="s">
+      <c r="F32" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="G32" s="15" t="s">
+      <c r="G32" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="H32" s="15" t="s">
+      <c r="H32" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="I32" s="18">
+      <c r="I32" s="15">
         <v>7290019570745</v>
       </c>
-      <c r="J32" s="62">
+      <c r="J32" s="51">
         <v>109524</v>
       </c>
-      <c r="K32" s="27" t="s">
+      <c r="K32" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="L32" s="72" t="s">
+      <c r="L32" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M32" s="78">
+      <c r="M32" s="67">
         <v>105</v>
       </c>
-      <c r="N32" s="78" t="s">
+      <c r="N32" s="67" t="s">
         <v>190</v>
       </c>
-      <c r="O32" s="76"/>
-    </row>
-    <row r="33" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
-      <c r="B33" s="15" t="s">
+      <c r="O32" s="65"/>
+    </row>
+    <row r="33" spans="1:17" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+      <c r="A33" s="13"/>
+      <c r="B33" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="C33" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="D33" s="47"/>
-      <c r="E33" s="48" t="s">
+      <c r="D33" s="36"/>
+      <c r="E33" s="37" t="s">
         <v>155</v>
       </c>
-      <c r="F33" s="15" t="s">
+      <c r="F33" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="G33" s="15" t="s">
+      <c r="G33" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="H33" s="15"/>
-      <c r="I33" s="18">
+      <c r="H33" s="14"/>
+      <c r="I33" s="15">
         <v>7290019570738</v>
       </c>
-      <c r="J33" s="62">
+      <c r="J33" s="51">
         <v>109525</v>
       </c>
-      <c r="K33" s="31" t="s">
+      <c r="K33" s="81" t="s">
         <v>53</v>
       </c>
-      <c r="L33" s="72" t="s">
+      <c r="L33" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M33" s="78">
+      <c r="M33" s="67">
         <v>187</v>
       </c>
-      <c r="N33" s="78" t="s">
+      <c r="N33" s="67" t="s">
         <v>190</v>
       </c>
-      <c r="O33" s="76"/>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
-      <c r="B34" s="15" t="s">
+      <c r="O33" s="65"/>
+    </row>
+    <row r="34" spans="1:17" ht="57" x14ac:dyDescent="0.25">
+      <c r="A34" s="13"/>
+      <c r="B34" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="C34" s="15" t="s">
+      <c r="C34" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="D34" s="47"/>
-      <c r="E34" s="48" t="s">
+      <c r="D34" s="36"/>
+      <c r="E34" s="37" t="s">
         <v>164</v>
       </c>
-      <c r="F34" s="15" t="s">
+      <c r="F34" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="G34" s="15" t="s">
+      <c r="G34" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="H34" s="15" t="s">
+      <c r="H34" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="I34" s="18">
+      <c r="I34" s="15">
         <v>7290019570684</v>
       </c>
-      <c r="J34" s="62">
+      <c r="J34" s="51">
         <v>155521</v>
       </c>
-      <c r="K34" s="19" t="s">
+      <c r="K34" s="78" t="s">
         <v>56</v>
       </c>
-      <c r="L34" s="72" t="s">
+      <c r="L34" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M34" s="78">
+      <c r="M34" s="67">
         <v>179</v>
       </c>
-      <c r="N34" s="78" t="s">
+      <c r="N34" s="67" t="s">
         <v>190</v>
       </c>
-      <c r="O34" s="76"/>
-    </row>
-    <row r="35" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="33"/>
-      <c r="B35" s="34" t="s">
+      <c r="O34" s="65"/>
+    </row>
+    <row r="35" spans="1:17" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+      <c r="A35" s="25"/>
+      <c r="B35" s="26" t="s">
         <v>187</v>
       </c>
-      <c r="C35" s="34" t="s">
+      <c r="C35" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="D35" s="54" t="s">
+      <c r="D35" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="E35" s="55" t="s">
+      <c r="E35" s="44" t="s">
         <v>165</v>
       </c>
-      <c r="F35" s="34" t="s">
+      <c r="F35" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="G35" s="34" t="s">
+      <c r="G35" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="H35" s="34"/>
-      <c r="I35" s="35">
+      <c r="H35" s="26"/>
+      <c r="I35" s="27">
         <v>7290019570721</v>
       </c>
-      <c r="J35" s="64">
+      <c r="J35" s="53">
         <v>153521</v>
       </c>
-      <c r="K35" s="36" t="s">
+      <c r="K35" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="L35" s="74" t="s">
+      <c r="L35" s="63" t="s">
         <v>169</v>
       </c>
-      <c r="M35" s="80"/>
-      <c r="N35" s="80"/>
-      <c r="O35" s="76"/>
-    </row>
-    <row r="36" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="33"/>
-      <c r="B36" s="34" t="s">
+      <c r="M35" s="69"/>
+      <c r="N35" s="69"/>
+      <c r="O35" s="65"/>
+    </row>
+    <row r="36" spans="1:17" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+      <c r="A36" s="25"/>
+      <c r="B36" s="26" t="s">
         <v>187</v>
       </c>
-      <c r="C36" s="34" t="s">
+      <c r="C36" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="D36" s="54" t="s">
+      <c r="D36" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="E36" s="55" t="s">
+      <c r="E36" s="44" t="s">
         <v>166</v>
       </c>
-      <c r="F36" s="34" t="s">
+      <c r="F36" s="26" t="s">
         <v>183</v>
       </c>
-      <c r="G36" s="34" t="s">
+      <c r="G36" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="H36" s="34"/>
-      <c r="I36" s="35">
+      <c r="H36" s="26"/>
+      <c r="I36" s="27">
         <v>7290019570714</v>
       </c>
-      <c r="J36" s="64">
+      <c r="J36" s="53">
         <v>150521</v>
       </c>
-      <c r="K36" s="36" t="s">
+      <c r="K36" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="L36" s="74" t="s">
+      <c r="L36" s="63" t="s">
         <v>169</v>
       </c>
-      <c r="M36" s="80"/>
-      <c r="N36" s="80"/>
-      <c r="O36" s="76"/>
-      <c r="P36" s="83" t="s">
+      <c r="M36" s="69"/>
+      <c r="N36" s="69"/>
+      <c r="O36" s="65"/>
+      <c r="P36" s="72" t="s">
         <v>199</v>
       </c>
-      <c r="Q36" s="68">
+      <c r="Q36" s="57">
         <f>COUNTIF(N4:N38,"CERO")</f>
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" s="33"/>
-      <c r="B37" s="34" t="s">
+    <row r="37" spans="1:17" ht="57" x14ac:dyDescent="0.25">
+      <c r="A37" s="25"/>
+      <c r="B37" s="26" t="s">
         <v>187</v>
       </c>
-      <c r="C37" s="34" t="s">
+      <c r="C37" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="D37" s="54" t="s">
+      <c r="D37" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="E37" s="55" t="s">
+      <c r="E37" s="44" t="s">
         <v>164</v>
       </c>
-      <c r="F37" s="34" t="s">
+      <c r="F37" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="G37" s="34" t="s">
+      <c r="G37" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="H37" s="15" t="s">
+      <c r="H37" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="I37" s="35">
+      <c r="I37" s="27">
         <v>7290019570707</v>
       </c>
-      <c r="J37" s="64">
+      <c r="J37" s="53">
         <v>151521</v>
       </c>
-      <c r="K37" s="37" t="s">
+      <c r="K37" s="84" t="s">
         <v>138</v>
       </c>
-      <c r="L37" s="74" t="s">
+      <c r="L37" s="63" t="s">
         <v>169</v>
       </c>
-      <c r="M37" s="80"/>
-      <c r="N37" s="80"/>
-      <c r="O37" s="76"/>
-      <c r="P37" s="82" t="s">
+      <c r="M37" s="69"/>
+      <c r="N37" s="69"/>
+      <c r="O37" s="65"/>
+      <c r="P37" s="71" t="s">
         <v>196</v>
       </c>
       <c r="Q37" s="5">
         <f>COUNTIF(N4:N38,"OK")</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="33"/>
-      <c r="B38" s="34" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" s="1" customFormat="1" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="25"/>
+      <c r="B38" s="26" t="s">
         <v>187</v>
       </c>
-      <c r="C38" s="34" t="s">
+      <c r="C38" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="D38" s="54" t="s">
+      <c r="D38" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="E38" s="55" t="s">
+      <c r="E38" s="44" t="s">
         <v>164</v>
       </c>
-      <c r="F38" s="34" t="s">
+      <c r="F38" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="G38" s="34" t="s">
+      <c r="G38" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="H38" s="34" t="s">
+      <c r="H38" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="I38" s="35">
+      <c r="I38" s="27">
         <v>7290019570691</v>
       </c>
-      <c r="J38" s="64">
+      <c r="J38" s="53">
         <v>156521</v>
       </c>
-      <c r="K38" s="36" t="s">
+      <c r="K38" s="83" t="s">
         <v>55</v>
       </c>
-      <c r="L38" s="74" t="s">
+      <c r="L38" s="63" t="s">
         <v>169</v>
       </c>
-      <c r="M38" s="81"/>
-      <c r="N38" s="81"/>
-      <c r="O38" s="76"/>
-      <c r="P38" s="83" t="s">
+      <c r="M38" s="70"/>
+      <c r="N38" s="70"/>
+      <c r="O38" s="65"/>
+      <c r="P38" s="72" t="s">
         <v>197</v>
       </c>
       <c r="Q38" s="5">
         <f>COUNTIF(N4:N38,"FALTA")</f>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" s="38"/>
-      <c r="B39" s="39"/>
-      <c r="C39" s="40"/>
-      <c r="D39" s="56"/>
-      <c r="E39" s="57"/>
+      <c r="A39" s="28"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="45"/>
+      <c r="E39" s="46"/>
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
-      <c r="K39" s="5"/>
+      <c r="K39" s="73"/>
       <c r="L39" s="5"/>
       <c r="M39" s="5"/>
       <c r="N39" s="5"/>
-      <c r="O39" s="70"/>
-      <c r="P39" s="82" t="s">
+      <c r="O39" s="59"/>
+      <c r="P39" s="71" t="s">
         <v>198</v>
       </c>
       <c r="Q39" s="5">
@@ -3232,69 +3251,69 @@
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" s="56" t="s">
+      <c r="A40" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="B40" s="39"/>
-      <c r="C40" s="40"/>
-      <c r="D40" s="56"/>
-      <c r="E40" s="57"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="45"/>
+      <c r="E40" s="46"/>
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
-      <c r="K40" s="5"/>
+      <c r="K40" s="73"/>
       <c r="L40" s="5"/>
-      <c r="O40" s="70"/>
+      <c r="O40" s="59"/>
       <c r="P40" s="5"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A41" s="56" t="s">
+      <c r="A41" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="B41" s="39"/>
-      <c r="C41" s="40"/>
-      <c r="D41" s="56"/>
-      <c r="E41" s="57"/>
+      <c r="B41" s="29"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="45"/>
+      <c r="E41" s="46"/>
       <c r="I41" s="5"/>
       <c r="J41" s="5"/>
-      <c r="K41" s="5"/>
+      <c r="K41" s="73"/>
       <c r="L41" s="5"/>
       <c r="M41" s="5"/>
       <c r="N41"/>
-      <c r="O41" s="70"/>
+      <c r="O41" s="59"/>
       <c r="P41" s="5"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A42" s="56" t="s">
+      <c r="A42" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="B42" s="39"/>
-      <c r="C42" s="40"/>
-      <c r="D42" s="56"/>
-      <c r="E42" s="57"/>
+      <c r="B42" s="29"/>
+      <c r="C42" s="30"/>
+      <c r="D42" s="45"/>
+      <c r="E42" s="46"/>
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
-      <c r="K42" s="5"/>
+      <c r="K42" s="73"/>
       <c r="L42" s="5"/>
       <c r="M42" s="5"/>
       <c r="N42" s="5"/>
-      <c r="O42" s="70"/>
+      <c r="O42" s="59"/>
       <c r="P42" s="5"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A43" s="65" t="s">
+      <c r="A43" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="B43" s="41"/>
-      <c r="C43" s="42"/>
-      <c r="D43" s="58"/>
-      <c r="E43" s="59"/>
+      <c r="B43" s="31"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="47"/>
+      <c r="E43" s="48"/>
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
-      <c r="K43" s="5"/>
+      <c r="K43" s="73"/>
       <c r="L43" s="5"/>
       <c r="M43" s="5"/>
       <c r="N43" s="5"/>
-      <c r="O43" s="70"/>
+      <c r="O43" s="59"/>
       <c r="P43" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
agregado de traduccion a etiqueta 111 he-paleta4 - jabat
</commit_message>
<xml_diff>
--- a/Copia de Copia de Codigos CHABAT NICO.xlsx
+++ b/Copia de Copia de Codigos CHABAT NICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D611FBA0-213D-4303-A5E3-322E73D8065C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007290E0-8957-49F1-947D-1F3B3D3D4E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1592,8 +1592,8 @@
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
+      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="61.5" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2329,7 +2329,7 @@
         <v>111</v>
       </c>
       <c r="N17" s="67" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="O17" s="65"/>
     </row>
@@ -3180,7 +3180,7 @@
       </c>
       <c r="Q37" s="5">
         <f>COUNTIF(N4:N38,"OK")</f>
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:17" s="1" customFormat="1" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3226,7 +3226,7 @@
       </c>
       <c r="Q38" s="5">
         <f>COUNTIF(N4:N38,"FALTA")</f>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
@@ -3333,6 +3333,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="מסמך" ma:contentTypeID="0x010100E111FB68E4AB3A458E6F1E68F8888CED" ma:contentTypeVersion="13" ma:contentTypeDescription="צור מסמך חדש." ma:contentTypeScope="" ma:versionID="bfe1cfa8ea064de69b4e2203b8e1e509">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4613b05c-4671-4207-a6b8-e30994dce502" xmlns:ns3="ae89acfa-0242-4570-84ca-e3aafb74daca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b8d078cf0bd54969afc6a4d318ee940" ns2:_="" ns3:_="">
     <xsd:import namespace="4613b05c-4671-4207-a6b8-e30994dce502"/>
@@ -3555,27 +3575,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
+    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
+    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A9BCE7-9EE4-4695-9AF6-872741DC1E3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3592,24 +3612,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
-    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
-    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
agregado de traduccion a etiqueta 120 HE-TapaAguja7b - jabat
</commit_message>
<xml_diff>
--- a/Copia de Copia de Codigos CHABAT NICO.xlsx
+++ b/Copia de Copia de Codigos CHABAT NICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007290E0-8957-49F1-947D-1F3B3D3D4E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA72A999-B47B-475F-A41F-AB2719E62A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1592,17 +1592,17 @@
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O17" sqref="O17"/>
+      <pane ySplit="3" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="61.5" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="16" style="5" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.85546875" style="5" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="39.5703125" style="33" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="39" style="33" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="12.85546875" style="5" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="11" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26.85546875" style="5" customWidth="1"/>
@@ -2501,7 +2501,7 @@
         <v>120</v>
       </c>
       <c r="N21" s="67" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="O21" s="65"/>
     </row>
@@ -3180,7 +3180,7 @@
       </c>
       <c r="Q37" s="5">
         <f>COUNTIF(N4:N38,"OK")</f>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:17" s="1" customFormat="1" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3226,7 +3226,7 @@
       </c>
       <c r="Q38" s="5">
         <f>COUNTIF(N4:N38,"FALTA")</f>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
@@ -3333,26 +3333,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="מסמך" ma:contentTypeID="0x010100E111FB68E4AB3A458E6F1E68F8888CED" ma:contentTypeVersion="13" ma:contentTypeDescription="צור מסמך חדש." ma:contentTypeScope="" ma:versionID="bfe1cfa8ea064de69b4e2203b8e1e509">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4613b05c-4671-4207-a6b8-e30994dce502" xmlns:ns3="ae89acfa-0242-4570-84ca-e3aafb74daca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b8d078cf0bd54969afc6a4d318ee940" ns2:_="" ns3:_="">
     <xsd:import namespace="4613b05c-4671-4207-a6b8-e30994dce502"/>
@@ -3575,27 +3555,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
-    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
-    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A9BCE7-9EE4-4695-9AF6-872741DC1E3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3612,4 +3592,24 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
+    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
+    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
agregado de traduccion a etiqueta 112 cogote trozos 10B - jabat
</commit_message>
<xml_diff>
--- a/Copia de Copia de Codigos CHABAT NICO.xlsx
+++ b/Copia de Copia de Codigos CHABAT NICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA72A999-B47B-475F-A41F-AB2719E62A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A16085-1CCA-4FD8-A4F0-6FF99A90C73D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1592,8 +1592,8 @@
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N22" sqref="N22"/>
+      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="61.5" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2630,7 +2630,7 @@
         <v>112</v>
       </c>
       <c r="N24" s="67" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="O24" s="65"/>
     </row>
@@ -3180,7 +3180,7 @@
       </c>
       <c r="Q37" s="5">
         <f>COUNTIF(N4:N38,"OK")</f>
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:17" s="1" customFormat="1" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3226,7 +3226,7 @@
       </c>
       <c r="Q38" s="5">
         <f>COUNTIF(N4:N38,"FALTA")</f>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
agregado de traduccion a etiqueta 179 HE HUESO MANO - jabat
</commit_message>
<xml_diff>
--- a/Copia de Copia de Codigos CHABAT NICO.xlsx
+++ b/Copia de Copia de Codigos CHABAT NICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A16085-1CCA-4FD8-A4F0-6FF99A90C73D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B3C984B-53FA-4E57-9206-D37D4896AE8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1592,8 +1592,8 @@
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O24" sqref="O24"/>
+      <pane ySplit="3" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="61.5" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -3052,7 +3052,7 @@
         <v>179</v>
       </c>
       <c r="N34" s="67" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="O34" s="65"/>
     </row>
@@ -3180,7 +3180,7 @@
       </c>
       <c r="Q37" s="5">
         <f>COUNTIF(N4:N38,"OK")</f>
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:17" s="1" customFormat="1" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3226,7 +3226,7 @@
       </c>
       <c r="Q38" s="5">
         <f>COUNTIF(N4:N38,"FALTA")</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
@@ -3333,6 +3333,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="מסמך" ma:contentTypeID="0x010100E111FB68E4AB3A458E6F1E68F8888CED" ma:contentTypeVersion="13" ma:contentTypeDescription="צור מסמך חדש." ma:contentTypeScope="" ma:versionID="bfe1cfa8ea064de69b4e2203b8e1e509">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4613b05c-4671-4207-a6b8-e30994dce502" xmlns:ns3="ae89acfa-0242-4570-84ca-e3aafb74daca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b8d078cf0bd54969afc6a4d318ee940" ns2:_="" ns3:_="">
     <xsd:import namespace="4613b05c-4671-4207-a6b8-e30994dce502"/>
@@ -3555,27 +3575,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
+    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
+    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A9BCE7-9EE4-4695-9AF6-872741DC1E3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3592,24 +3612,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
-    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
-    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
agregado de traduccion a etiqueta 187 he entrecostilla ch - jabat
</commit_message>
<xml_diff>
--- a/Copia de Copia de Codigos CHABAT NICO.xlsx
+++ b/Copia de Copia de Codigos CHABAT NICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B3C984B-53FA-4E57-9206-D37D4896AE8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C4F224-85AB-4C03-9A5A-4922EE304574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -650,7 +650,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -762,6 +762,14 @@
     <font>
       <b/>
       <sz val="44"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="36"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1008,7 +1016,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1297,6 +1305,9 @@
     </xf>
     <xf numFmtId="44" fontId="4" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="16" fillId="2" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1592,8 +1603,8 @@
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N35" sqref="N35"/>
+      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="61.5" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2976,7 +2987,7 @@
       </c>
       <c r="O32" s="65"/>
     </row>
-    <row r="33" spans="1:17" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" s="1" customFormat="1" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
       <c r="B33" s="14" t="s">
         <v>187</v>
@@ -3001,7 +3012,7 @@
       <c r="J33" s="51">
         <v>109525</v>
       </c>
-      <c r="K33" s="81" t="s">
+      <c r="K33" s="97" t="s">
         <v>53</v>
       </c>
       <c r="L33" s="61" t="s">
@@ -3011,7 +3022,7 @@
         <v>187</v>
       </c>
       <c r="N33" s="67" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="O33" s="65"/>
     </row>
@@ -3180,7 +3191,7 @@
       </c>
       <c r="Q37" s="5">
         <f>COUNTIF(N4:N38,"OK")</f>
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:17" s="1" customFormat="1" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3226,7 +3237,7 @@
       </c>
       <c r="Q38" s="5">
         <f>COUNTIF(N4:N38,"FALTA")</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
@@ -3333,26 +3344,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="מסמך" ma:contentTypeID="0x010100E111FB68E4AB3A458E6F1E68F8888CED" ma:contentTypeVersion="13" ma:contentTypeDescription="צור מסמך חדש." ma:contentTypeScope="" ma:versionID="bfe1cfa8ea064de69b4e2203b8e1e509">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4613b05c-4671-4207-a6b8-e30994dce502" xmlns:ns3="ae89acfa-0242-4570-84ca-e3aafb74daca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b8d078cf0bd54969afc6a4d318ee940" ns2:_="" ns3:_="">
     <xsd:import namespace="4613b05c-4671-4207-a6b8-e30994dce502"/>
@@ -3575,27 +3566,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
-    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
-    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A9BCE7-9EE4-4695-9AF6-872741DC1E3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3612,4 +3603,24 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
+    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
+    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
agregado de traduccion a etiqueta 105 he entrecostilla- jabat
</commit_message>
<xml_diff>
--- a/Copia de Copia de Codigos CHABAT NICO.xlsx
+++ b/Copia de Copia de Codigos CHABAT NICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C4F224-85AB-4C03-9A5A-4922EE304574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021039CC-D9DE-46B7-B784-18859FFA8633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -650,7 +650,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -770,6 +770,14 @@
     <font>
       <b/>
       <sz val="36"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="42"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1016,7 +1024,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1270,6 +1278,9 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
+    <xf numFmtId="1" fontId="16" fillId="2" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1306,7 +1317,7 @@
     <xf numFmtId="44" fontId="4" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="16" fillId="2" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="17" fillId="2" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" readingOrder="2"/>
     </xf>
   </cellXfs>
@@ -1603,8 +1614,8 @@
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L31" sqref="L31"/>
+      <pane ySplit="3" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="61.5" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1641,31 +1652,31 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="91" t="s">
+      <c r="A2" s="92" t="s">
         <v>122</v>
       </c>
       <c r="B2" s="7"/>
-      <c r="C2" s="85" t="s">
+      <c r="C2" s="86" t="s">
         <v>104</v>
       </c>
-      <c r="D2" s="89" t="s">
+      <c r="D2" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="89" t="s">
+      <c r="E2" s="90" t="s">
         <v>52</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-      <c r="H2" s="85" t="s">
+      <c r="H2" s="86" t="s">
         <v>113</v>
       </c>
-      <c r="I2" s="93" t="s">
+      <c r="I2" s="94" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="95" t="s">
+      <c r="J2" s="96" t="s">
         <v>123</v>
       </c>
-      <c r="K2" s="87" t="s">
+      <c r="K2" s="88" t="s">
         <v>20</v>
       </c>
       <c r="L2" s="2" t="s">
@@ -1678,25 +1689,25 @@
       </c>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="92"/>
+      <c r="A3" s="93"/>
       <c r="B3" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="86" t="s">
+      <c r="C3" s="87" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
       <c r="F3" s="9" t="s">
         <v>105</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="H3" s="86"/>
-      <c r="I3" s="94"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="88"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="95"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="89"/>
       <c r="L3" s="60" t="s">
         <v>168</v>
       </c>
@@ -2944,7 +2955,7 @@
       </c>
       <c r="O31" s="65"/>
     </row>
-    <row r="32" spans="1:15" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" s="1" customFormat="1" ht="54" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
       <c r="B32" s="14" t="s">
         <v>187</v>
@@ -2973,7 +2984,7 @@
       <c r="J32" s="51">
         <v>109524</v>
       </c>
-      <c r="K32" s="80" t="s">
+      <c r="K32" s="98" t="s">
         <v>2</v>
       </c>
       <c r="L32" s="61" t="s">
@@ -2983,7 +2994,7 @@
         <v>105</v>
       </c>
       <c r="N32" s="67" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="O32" s="65"/>
     </row>
@@ -3012,7 +3023,7 @@
       <c r="J33" s="51">
         <v>109525</v>
       </c>
-      <c r="K33" s="97" t="s">
+      <c r="K33" s="85" t="s">
         <v>53</v>
       </c>
       <c r="L33" s="61" t="s">
@@ -3191,7 +3202,7 @@
       </c>
       <c r="Q37" s="5">
         <f>COUNTIF(N4:N38,"OK")</f>
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:17" s="1" customFormat="1" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3237,7 +3248,7 @@
       </c>
       <c r="Q38" s="5">
         <f>COUNTIF(N4:N38,"FALTA")</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
@@ -3344,6 +3355,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="מסמך" ma:contentTypeID="0x010100E111FB68E4AB3A458E6F1E68F8888CED" ma:contentTypeVersion="13" ma:contentTypeDescription="צור מסמך חדש." ma:contentTypeScope="" ma:versionID="bfe1cfa8ea064de69b4e2203b8e1e509">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4613b05c-4671-4207-a6b8-e30994dce502" xmlns:ns3="ae89acfa-0242-4570-84ca-e3aafb74daca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b8d078cf0bd54969afc6a4d318ee940" ns2:_="" ns3:_="">
     <xsd:import namespace="4613b05c-4671-4207-a6b8-e30994dce502"/>
@@ -3566,27 +3597,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
+    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
+    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A9BCE7-9EE4-4695-9AF6-872741DC1E3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3603,24 +3634,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
-    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
-    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
agregado de traduccion a etiqueta 182 HE asado sh 9c 99- jabat
</commit_message>
<xml_diff>
--- a/Copia de Copia de Codigos CHABAT NICO.xlsx
+++ b/Copia de Copia de Codigos CHABAT NICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021039CC-D9DE-46B7-B784-18859FFA8633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF4778E-226F-4F0E-8E4F-0519D75E9998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1024,7 +1024,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1281,6 +1281,9 @@
     <xf numFmtId="1" fontId="16" fillId="2" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" readingOrder="2"/>
     </xf>
+    <xf numFmtId="1" fontId="17" fillId="2" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1317,8 +1320,8 @@
     <xf numFmtId="44" fontId="4" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="17" fillId="2" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1614,8 +1617,8 @@
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O32" sqref="O32"/>
+      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="61.5" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1652,31 +1655,31 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="92" t="s">
+      <c r="A2" s="93" t="s">
         <v>122</v>
       </c>
       <c r="B2" s="7"/>
-      <c r="C2" s="86" t="s">
+      <c r="C2" s="87" t="s">
         <v>104</v>
       </c>
-      <c r="D2" s="90" t="s">
+      <c r="D2" s="91" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="90" t="s">
+      <c r="E2" s="91" t="s">
         <v>52</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-      <c r="H2" s="86" t="s">
+      <c r="H2" s="87" t="s">
         <v>113</v>
       </c>
-      <c r="I2" s="94" t="s">
+      <c r="I2" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="96" t="s">
+      <c r="J2" s="97" t="s">
         <v>123</v>
       </c>
-      <c r="K2" s="88" t="s">
+      <c r="K2" s="89" t="s">
         <v>20</v>
       </c>
       <c r="L2" s="2" t="s">
@@ -1689,25 +1692,25 @@
       </c>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="93"/>
+      <c r="A3" s="94"/>
       <c r="B3" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="87" t="s">
+      <c r="C3" s="88" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
+      <c r="D3" s="92"/>
+      <c r="E3" s="92"/>
       <c r="F3" s="9" t="s">
         <v>105</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="H3" s="87"/>
-      <c r="I3" s="95"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="89"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="90"/>
       <c r="L3" s="60" t="s">
         <v>168</v>
       </c>
@@ -2787,7 +2790,7 @@
       </c>
       <c r="O27" s="65"/>
     </row>
-    <row r="28" spans="1:15" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" s="1" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
         <v>99</v>
       </c>
@@ -2818,7 +2821,7 @@
       <c r="J28" s="51">
         <v>109521</v>
       </c>
-      <c r="K28" s="78" t="s">
+      <c r="K28" s="99" t="s">
         <v>137</v>
       </c>
       <c r="L28" s="61" t="s">
@@ -2828,11 +2831,11 @@
         <v>182</v>
       </c>
       <c r="N28" s="67" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="O28" s="65"/>
     </row>
-    <row r="29" spans="1:15" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" s="1" customFormat="1" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13">
         <v>9</v>
       </c>
@@ -2984,7 +2987,7 @@
       <c r="J32" s="51">
         <v>109524</v>
       </c>
-      <c r="K32" s="98" t="s">
+      <c r="K32" s="86" t="s">
         <v>2</v>
       </c>
       <c r="L32" s="61" t="s">
@@ -3202,7 +3205,7 @@
       </c>
       <c r="Q37" s="5">
         <f>COUNTIF(N4:N38,"OK")</f>
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:17" s="1" customFormat="1" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3248,7 +3251,7 @@
       </c>
       <c r="Q38" s="5">
         <f>COUNTIF(N4:N38,"FALTA")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
@@ -3355,26 +3358,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="מסמך" ma:contentTypeID="0x010100E111FB68E4AB3A458E6F1E68F8888CED" ma:contentTypeVersion="13" ma:contentTypeDescription="צור מסמך חדש." ma:contentTypeScope="" ma:versionID="bfe1cfa8ea064de69b4e2203b8e1e509">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4613b05c-4671-4207-a6b8-e30994dce502" xmlns:ns3="ae89acfa-0242-4570-84ca-e3aafb74daca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b8d078cf0bd54969afc6a4d318ee940" ns2:_="" ns3:_="">
     <xsd:import namespace="4613b05c-4671-4207-a6b8-e30994dce502"/>
@@ -3597,27 +3580,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
-    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
-    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A9BCE7-9EE4-4695-9AF6-872741DC1E3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3634,4 +3617,24 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
+    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
+    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
agregado de traduccion a etiqueta 181 HE asado sh 9c 9- jabat
</commit_message>
<xml_diff>
--- a/Copia de Copia de Codigos CHABAT NICO.xlsx
+++ b/Copia de Copia de Codigos CHABAT NICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF4778E-226F-4F0E-8E4F-0519D75E9998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C983BC79-E3EC-4423-B852-8BB0BB946E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1284,6 +1284,9 @@
     <xf numFmtId="1" fontId="17" fillId="2" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" readingOrder="2"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1319,9 +1322,6 @@
     </xf>
     <xf numFmtId="44" fontId="4" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1618,7 +1618,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K27" sqref="K27"/>
+      <selection pane="bottomLeft" activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="61.5" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1655,31 +1655,31 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="94" t="s">
         <v>122</v>
       </c>
       <c r="B2" s="7"/>
-      <c r="C2" s="87" t="s">
+      <c r="C2" s="88" t="s">
         <v>104</v>
       </c>
-      <c r="D2" s="91" t="s">
+      <c r="D2" s="92" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="91" t="s">
+      <c r="E2" s="92" t="s">
         <v>52</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-      <c r="H2" s="87" t="s">
+      <c r="H2" s="88" t="s">
         <v>113</v>
       </c>
-      <c r="I2" s="95" t="s">
+      <c r="I2" s="96" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="97" t="s">
+      <c r="J2" s="98" t="s">
         <v>123</v>
       </c>
-      <c r="K2" s="89" t="s">
+      <c r="K2" s="90" t="s">
         <v>20</v>
       </c>
       <c r="L2" s="2" t="s">
@@ -1692,25 +1692,25 @@
       </c>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="94"/>
+      <c r="A3" s="95"/>
       <c r="B3" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="88" t="s">
+      <c r="C3" s="89" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="92"/>
-      <c r="E3" s="92"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
       <c r="F3" s="9" t="s">
         <v>105</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="H3" s="88"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="90"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="91"/>
       <c r="L3" s="60" t="s">
         <v>168</v>
       </c>
@@ -2821,7 +2821,7 @@
       <c r="J28" s="51">
         <v>109521</v>
       </c>
-      <c r="K28" s="99" t="s">
+      <c r="K28" s="87" t="s">
         <v>137</v>
       </c>
       <c r="L28" s="61" t="s">
@@ -2874,7 +2874,7 @@
         <v>181</v>
       </c>
       <c r="N29" s="67" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="O29" s="65"/>
     </row>
@@ -3205,7 +3205,7 @@
       </c>
       <c r="Q37" s="5">
         <f>COUNTIF(N4:N38,"OK")</f>
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:17" s="1" customFormat="1" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3251,7 +3251,7 @@
       </c>
       <c r="Q38" s="5">
         <f>COUNTIF(N4:N38,"FALTA")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
@@ -3358,6 +3358,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="מסמך" ma:contentTypeID="0x010100E111FB68E4AB3A458E6F1E68F8888CED" ma:contentTypeVersion="13" ma:contentTypeDescription="צור מסמך חדש." ma:contentTypeScope="" ma:versionID="bfe1cfa8ea064de69b4e2203b8e1e509">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4613b05c-4671-4207-a6b8-e30994dce502" xmlns:ns3="ae89acfa-0242-4570-84ca-e3aafb74daca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b8d078cf0bd54969afc6a4d318ee940" ns2:_="" ns3:_="">
     <xsd:import namespace="4613b05c-4671-4207-a6b8-e30994dce502"/>
@@ -3580,27 +3600,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
+    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
+    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A9BCE7-9EE4-4695-9AF6-872741DC1E3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3617,24 +3637,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
-    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
-    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
agregado de etiquetas menudencias lengua, molleja, quijada, tendon- jabat
</commit_message>
<xml_diff>
--- a/Copia de Copia de Codigos CHABAT NICO.xlsx
+++ b/Copia de Copia de Codigos CHABAT NICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C983BC79-E3EC-4423-B852-8BB0BB946E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD35C4CB-8328-4F1C-965F-14874E2AAF5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="201">
   <si>
     <t>לשון בקר קפוא</t>
   </si>
@@ -1617,8 +1617,8 @@
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N30" sqref="N30"/>
+      <pane ySplit="3" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="61.5" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -3114,8 +3114,12 @@
       <c r="L35" s="63" t="s">
         <v>169</v>
       </c>
-      <c r="M35" s="69"/>
-      <c r="N35" s="69"/>
+      <c r="M35" s="69">
+        <v>161</v>
+      </c>
+      <c r="N35" s="69" t="s">
+        <v>195</v>
+      </c>
       <c r="O35" s="65"/>
     </row>
     <row r="36" spans="1:17" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
@@ -3151,8 +3155,12 @@
       <c r="L36" s="63" t="s">
         <v>169</v>
       </c>
-      <c r="M36" s="69"/>
-      <c r="N36" s="69"/>
+      <c r="M36" s="69">
+        <v>163</v>
+      </c>
+      <c r="N36" s="69" t="s">
+        <v>195</v>
+      </c>
       <c r="O36" s="65"/>
       <c r="P36" s="72" t="s">
         <v>199</v>
@@ -3197,15 +3205,19 @@
       <c r="L37" s="63" t="s">
         <v>169</v>
       </c>
-      <c r="M37" s="69"/>
-      <c r="N37" s="69"/>
+      <c r="M37" s="69">
+        <v>177</v>
+      </c>
+      <c r="N37" s="69" t="s">
+        <v>195</v>
+      </c>
       <c r="O37" s="65"/>
       <c r="P37" s="71" t="s">
         <v>196</v>
       </c>
       <c r="Q37" s="5">
         <f>COUNTIF(N4:N38,"OK")</f>
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="38" spans="1:17" s="1" customFormat="1" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3243,8 +3255,12 @@
       <c r="L38" s="63" t="s">
         <v>169</v>
       </c>
-      <c r="M38" s="70"/>
-      <c r="N38" s="70"/>
+      <c r="M38" s="70">
+        <v>162</v>
+      </c>
+      <c r="N38" s="70" t="s">
+        <v>195</v>
+      </c>
       <c r="O38" s="65"/>
       <c r="P38" s="72" t="s">
         <v>197</v>
@@ -3272,7 +3288,7 @@
       </c>
       <c r="Q39" s="5">
         <f>COUNTIF(N4:N38,"")</f>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
@@ -3358,26 +3374,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="מסמך" ma:contentTypeID="0x010100E111FB68E4AB3A458E6F1E68F8888CED" ma:contentTypeVersion="13" ma:contentTypeDescription="צור מסמך חדש." ma:contentTypeScope="" ma:versionID="bfe1cfa8ea064de69b4e2203b8e1e509">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4613b05c-4671-4207-a6b8-e30994dce502" xmlns:ns3="ae89acfa-0242-4570-84ca-e3aafb74daca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b8d078cf0bd54969afc6a4d318ee940" ns2:_="" ns3:_="">
     <xsd:import namespace="4613b05c-4671-4207-a6b8-e30994dce502"/>
@@ -3600,27 +3596,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
-    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
-    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A9BCE7-9EE4-4695-9AF6-872741DC1E3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3637,4 +3633,24 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
+    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
+    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
cambio de nombres de etiquetas, agregado de etiquetas 300 y 301 jabat
</commit_message>
<xml_diff>
--- a/Copia de Copia de Codigos CHABAT NICO.xlsx
+++ b/Copia de Copia de Codigos CHABAT NICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD35C4CB-8328-4F1C-965F-14874E2AAF5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3CE68BA-85ED-433F-9F37-7F9816CDD4DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -650,7 +650,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -783,8 +783,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Fira Code"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Fira Code"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Ebrima"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -794,12 +809,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1024,7 +1033,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1077,16 +1086,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1098,13 +1107,13 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1137,10 +1146,10 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1152,10 +1161,10 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1179,12 +1188,12 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1209,12 +1218,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1227,20 +1236,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1254,28 +1257,22 @@
     <xf numFmtId="0" fontId="15" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="1" fontId="15" fillId="2" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" readingOrder="2"/>
     </xf>
+    <xf numFmtId="1" fontId="15" fillId="2" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="2"/>
+    </xf>
     <xf numFmtId="1" fontId="15" fillId="3" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" readingOrder="2"/>
     </xf>
-    <xf numFmtId="1" fontId="15" fillId="2" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="4" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="1" fontId="16" fillId="2" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1322,6 +1319,21 @@
     </xf>
     <xf numFmtId="44" fontId="4" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1616,9 +1628,9 @@
   </sheetPr>
   <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N39" sqref="N39"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="61.5" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1633,7 +1645,7 @@
     <col min="8" max="8" width="26.85546875" style="5" customWidth="1"/>
     <col min="9" max="9" width="16.7109375" style="4" customWidth="1"/>
     <col min="10" max="10" width="11" style="50" customWidth="1"/>
-    <col min="11" max="11" width="119" style="74" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="119" style="72" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="12.42578125" style="4" customWidth="1"/>
     <col min="15" max="15" width="18.28515625" style="58" customWidth="1"/>
@@ -1655,31 +1667,31 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="90" t="s">
         <v>122</v>
       </c>
       <c r="B2" s="7"/>
-      <c r="C2" s="88" t="s">
+      <c r="C2" s="84" t="s">
         <v>104</v>
       </c>
-      <c r="D2" s="92" t="s">
+      <c r="D2" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="92" t="s">
+      <c r="E2" s="88" t="s">
         <v>52</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-      <c r="H2" s="88" t="s">
+      <c r="H2" s="84" t="s">
         <v>113</v>
       </c>
-      <c r="I2" s="96" t="s">
+      <c r="I2" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="98" t="s">
+      <c r="J2" s="94" t="s">
         <v>123</v>
       </c>
-      <c r="K2" s="90" t="s">
+      <c r="K2" s="86" t="s">
         <v>20</v>
       </c>
       <c r="L2" s="2" t="s">
@@ -1692,25 +1704,25 @@
       </c>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="95"/>
+      <c r="A3" s="91"/>
       <c r="B3" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="89" t="s">
+      <c r="C3" s="85" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
       <c r="F3" s="9" t="s">
         <v>105</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="H3" s="89"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="99"/>
-      <c r="K3" s="91"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="87"/>
       <c r="L3" s="60" t="s">
         <v>168</v>
       </c>
@@ -1758,7 +1770,7 @@
       <c r="J4" s="51">
         <v>101861</v>
       </c>
-      <c r="K4" s="75" t="s">
+      <c r="K4" s="73" t="s">
         <v>91</v>
       </c>
       <c r="L4" s="61" t="s">
@@ -1808,7 +1820,7 @@
       <c r="J5" s="51">
         <v>101862</v>
       </c>
-      <c r="K5" s="76" t="s">
+      <c r="K5" s="74" t="s">
         <v>91</v>
       </c>
       <c r="L5" s="61" t="s">
@@ -1824,7 +1836,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="57" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="14" t="s">
         <v>187</v>
@@ -1851,15 +1863,17 @@
       <c r="J6" s="51">
         <v>101865</v>
       </c>
-      <c r="K6" s="77" t="s">
+      <c r="K6" s="74" t="s">
         <v>54</v>
       </c>
       <c r="L6" s="61" t="s">
         <v>173</v>
       </c>
-      <c r="M6" s="67"/>
+      <c r="M6" s="67">
+        <v>300</v>
+      </c>
       <c r="N6" s="67" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="O6" s="65" t="s">
         <v>190</v>
@@ -1896,7 +1910,7 @@
       <c r="J7" s="51">
         <v>102531</v>
       </c>
-      <c r="K7" s="78" t="s">
+      <c r="K7" s="75" t="s">
         <v>124</v>
       </c>
       <c r="L7" s="61" t="s">
@@ -1912,7 +1926,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" s="1" customFormat="1" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>22</v>
       </c>
@@ -1941,15 +1955,17 @@
       <c r="J8" s="51">
         <v>102532</v>
       </c>
-      <c r="K8" s="78" t="s">
+      <c r="K8" s="75" t="s">
         <v>125</v>
       </c>
       <c r="L8" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M8" s="67"/>
+      <c r="M8" s="67">
+        <v>301</v>
+      </c>
       <c r="N8" s="67" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="O8" s="65" t="s">
         <v>190</v>
@@ -1986,7 +2002,7 @@
       <c r="J9" s="51">
         <v>102533</v>
       </c>
-      <c r="K9" s="78" t="s">
+      <c r="K9" s="75" t="s">
         <v>126</v>
       </c>
       <c r="L9" s="61" t="s">
@@ -2031,7 +2047,7 @@
       <c r="J10" s="52">
         <v>102534</v>
       </c>
-      <c r="K10" s="79" t="s">
+      <c r="K10" s="76" t="s">
         <v>97</v>
       </c>
       <c r="L10" s="62" t="s">
@@ -2081,7 +2097,7 @@
       <c r="J11" s="51">
         <v>103521</v>
       </c>
-      <c r="K11" s="78" t="s">
+      <c r="K11" s="75" t="s">
         <v>127</v>
       </c>
       <c r="L11" s="61" t="s">
@@ -2124,7 +2140,7 @@
       <c r="J12" s="52">
         <v>103522</v>
       </c>
-      <c r="K12" s="79" t="s">
+      <c r="K12" s="76" t="s">
         <v>128</v>
       </c>
       <c r="L12" s="62" t="s">
@@ -2174,7 +2190,7 @@
       <c r="J13" s="51">
         <v>103523</v>
       </c>
-      <c r="K13" s="78" t="s">
+      <c r="K13" s="75" t="s">
         <v>129</v>
       </c>
       <c r="L13" s="61" t="s">
@@ -2217,7 +2233,7 @@
       <c r="J14" s="51">
         <v>103524</v>
       </c>
-      <c r="K14" s="78" t="s">
+      <c r="K14" s="75" t="s">
         <v>130</v>
       </c>
       <c r="L14" s="61" t="s">
@@ -2262,7 +2278,7 @@
       <c r="J15" s="52">
         <v>104521</v>
       </c>
-      <c r="K15" s="79" t="s">
+      <c r="K15" s="76" t="s">
         <v>131</v>
       </c>
       <c r="L15" s="62" t="s">
@@ -2303,7 +2319,7 @@
       <c r="J16" s="51">
         <v>104522</v>
       </c>
-      <c r="K16" s="78" t="s">
+      <c r="K16" s="75" t="s">
         <v>132</v>
       </c>
       <c r="L16" s="61" t="s">
@@ -2344,7 +2360,7 @@
       <c r="J17" s="51">
         <v>104523</v>
       </c>
-      <c r="K17" s="78" t="s">
+      <c r="K17" s="75" t="s">
         <v>133</v>
       </c>
       <c r="L17" s="61" t="s">
@@ -2389,7 +2405,7 @@
       <c r="J18" s="52">
         <v>105521</v>
       </c>
-      <c r="K18" s="79" t="s">
+      <c r="K18" s="76" t="s">
         <v>134</v>
       </c>
       <c r="L18" s="62" t="s">
@@ -2430,7 +2446,7 @@
       <c r="J19" s="51">
         <v>105522</v>
       </c>
-      <c r="K19" s="80" t="s">
+      <c r="K19" s="77" t="s">
         <v>92</v>
       </c>
       <c r="L19" s="61" t="s">
@@ -2473,7 +2489,7 @@
       <c r="J20" s="51">
         <v>106521</v>
       </c>
-      <c r="K20" s="80" t="s">
+      <c r="K20" s="77" t="s">
         <v>93</v>
       </c>
       <c r="L20" s="61" t="s">
@@ -2516,7 +2532,7 @@
       <c r="J21" s="51">
         <v>107521</v>
       </c>
-      <c r="K21" s="80" t="s">
+      <c r="K21" s="77" t="s">
         <v>94</v>
       </c>
       <c r="L21" s="61" t="s">
@@ -2561,7 +2577,7 @@
       <c r="J22" s="51">
         <v>108521</v>
       </c>
-      <c r="K22" s="80" t="s">
+      <c r="K22" s="77" t="s">
         <v>95</v>
       </c>
       <c r="L22" s="61" t="s">
@@ -2602,7 +2618,7 @@
       <c r="J23" s="51">
         <v>108522</v>
       </c>
-      <c r="K23" s="81" t="s">
+      <c r="K23" s="77" t="s">
         <v>96</v>
       </c>
       <c r="L23" s="61" t="s">
@@ -2645,7 +2661,7 @@
       <c r="J24" s="51">
         <v>110531</v>
       </c>
-      <c r="K24" s="82" t="s">
+      <c r="K24" s="78" t="s">
         <v>4</v>
       </c>
       <c r="L24" s="61" t="s">
@@ -2690,7 +2706,7 @@
       <c r="J25" s="51">
         <v>110532</v>
       </c>
-      <c r="K25" s="78" t="s">
+      <c r="K25" s="75" t="s">
         <v>135</v>
       </c>
       <c r="L25" s="61" t="s">
@@ -2733,7 +2749,7 @@
       <c r="J26" s="51">
         <v>110533</v>
       </c>
-      <c r="K26" s="78" t="s">
+      <c r="K26" s="75" t="s">
         <v>136</v>
       </c>
       <c r="L26" s="61" t="s">
@@ -2776,7 +2792,7 @@
       <c r="J27" s="51">
         <v>170521</v>
       </c>
-      <c r="K27" s="80" t="s">
+      <c r="K27" s="77" t="s">
         <v>98</v>
       </c>
       <c r="L27" s="61" t="s">
@@ -2821,7 +2837,7 @@
       <c r="J28" s="51">
         <v>109521</v>
       </c>
-      <c r="K28" s="87" t="s">
+      <c r="K28" s="83" t="s">
         <v>137</v>
       </c>
       <c r="L28" s="61" t="s">
@@ -2864,7 +2880,7 @@
       <c r="J29" s="51">
         <v>109522</v>
       </c>
-      <c r="K29" s="80" t="s">
+      <c r="K29" s="77" t="s">
         <v>99</v>
       </c>
       <c r="L29" s="61" t="s">
@@ -2905,7 +2921,7 @@
       <c r="J30" s="51">
         <v>109523</v>
       </c>
-      <c r="K30" s="81" t="s">
+      <c r="K30" s="77" t="s">
         <v>100</v>
       </c>
       <c r="L30" s="61" t="s">
@@ -2944,7 +2960,7 @@
       <c r="J31" s="51">
         <v>157521</v>
       </c>
-      <c r="K31" s="80" t="s">
+      <c r="K31" s="77" t="s">
         <v>1</v>
       </c>
       <c r="L31" s="61" t="s">
@@ -2987,7 +3003,7 @@
       <c r="J32" s="51">
         <v>109524</v>
       </c>
-      <c r="K32" s="86" t="s">
+      <c r="K32" s="82" t="s">
         <v>2</v>
       </c>
       <c r="L32" s="61" t="s">
@@ -3026,7 +3042,7 @@
       <c r="J33" s="51">
         <v>109525</v>
       </c>
-      <c r="K33" s="85" t="s">
+      <c r="K33" s="81" t="s">
         <v>53</v>
       </c>
       <c r="L33" s="61" t="s">
@@ -3067,7 +3083,7 @@
       <c r="J34" s="51">
         <v>155521</v>
       </c>
-      <c r="K34" s="78" t="s">
+      <c r="K34" s="75" t="s">
         <v>56</v>
       </c>
       <c r="L34" s="61" t="s">
@@ -3108,7 +3124,7 @@
       <c r="J35" s="53">
         <v>153521</v>
       </c>
-      <c r="K35" s="83" t="s">
+      <c r="K35" s="79" t="s">
         <v>0</v>
       </c>
       <c r="L35" s="63" t="s">
@@ -3149,7 +3165,7 @@
       <c r="J36" s="53">
         <v>150521</v>
       </c>
-      <c r="K36" s="83" t="s">
+      <c r="K36" s="79" t="s">
         <v>3</v>
       </c>
       <c r="L36" s="63" t="s">
@@ -3162,12 +3178,12 @@
         <v>195</v>
       </c>
       <c r="O36" s="65"/>
-      <c r="P36" s="72" t="s">
+      <c r="P36" s="100" t="s">
         <v>199</v>
       </c>
-      <c r="Q36" s="57">
+      <c r="Q36" s="97">
         <f>COUNTIF(N4:N38,"CERO")</f>
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:17" ht="57" x14ac:dyDescent="0.25">
@@ -3199,7 +3215,7 @@
       <c r="J37" s="53">
         <v>151521</v>
       </c>
-      <c r="K37" s="84" t="s">
+      <c r="K37" s="80" t="s">
         <v>138</v>
       </c>
       <c r="L37" s="63" t="s">
@@ -3212,12 +3228,12 @@
         <v>195</v>
       </c>
       <c r="O37" s="65"/>
-      <c r="P37" s="71" t="s">
+      <c r="P37" s="98" t="s">
         <v>196</v>
       </c>
-      <c r="Q37" s="5">
+      <c r="Q37" s="99">
         <f>COUNTIF(N4:N38,"OK")</f>
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="38" spans="1:17" s="1" customFormat="1" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3249,7 +3265,7 @@
       <c r="J38" s="53">
         <v>156521</v>
       </c>
-      <c r="K38" s="83" t="s">
+      <c r="K38" s="79" t="s">
         <v>55</v>
       </c>
       <c r="L38" s="63" t="s">
@@ -3262,10 +3278,10 @@
         <v>195</v>
       </c>
       <c r="O38" s="65"/>
-      <c r="P38" s="72" t="s">
+      <c r="P38" s="96" t="s">
         <v>197</v>
       </c>
-      <c r="Q38" s="5">
+      <c r="Q38" s="99">
         <f>COUNTIF(N4:N38,"FALTA")</f>
         <v>0</v>
       </c>
@@ -3278,15 +3294,15 @@
       <c r="E39" s="46"/>
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
-      <c r="K39" s="73"/>
+      <c r="K39" s="71"/>
       <c r="L39" s="5"/>
       <c r="M39" s="5"/>
       <c r="N39" s="5"/>
       <c r="O39" s="59"/>
-      <c r="P39" s="71" t="s">
+      <c r="P39" s="98" t="s">
         <v>198</v>
       </c>
-      <c r="Q39" s="5">
+      <c r="Q39" s="99">
         <f>COUNTIF(N4:N38,"")</f>
         <v>0</v>
       </c>
@@ -3301,7 +3317,7 @@
       <c r="E40" s="46"/>
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
-      <c r="K40" s="73"/>
+      <c r="K40" s="71"/>
       <c r="L40" s="5"/>
       <c r="O40" s="59"/>
       <c r="P40" s="5"/>
@@ -3316,7 +3332,7 @@
       <c r="E41" s="46"/>
       <c r="I41" s="5"/>
       <c r="J41" s="5"/>
-      <c r="K41" s="73"/>
+      <c r="K41" s="71"/>
       <c r="L41" s="5"/>
       <c r="M41" s="5"/>
       <c r="N41"/>
@@ -3333,7 +3349,7 @@
       <c r="E42" s="46"/>
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
-      <c r="K42" s="73"/>
+      <c r="K42" s="71"/>
       <c r="L42" s="5"/>
       <c r="M42" s="5"/>
       <c r="N42" s="5"/>
@@ -3350,7 +3366,7 @@
       <c r="E43" s="48"/>
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
-      <c r="K43" s="73"/>
+      <c r="K43" s="71"/>
       <c r="L43" s="5"/>
       <c r="M43" s="5"/>
       <c r="N43" s="5"/>
@@ -3374,6 +3390,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="מסמך" ma:contentTypeID="0x010100E111FB68E4AB3A458E6F1E68F8888CED" ma:contentTypeVersion="13" ma:contentTypeDescription="צור מסמך חדש." ma:contentTypeScope="" ma:versionID="bfe1cfa8ea064de69b4e2203b8e1e509">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4613b05c-4671-4207-a6b8-e30994dce502" xmlns:ns3="ae89acfa-0242-4570-84ca-e3aafb74daca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b8d078cf0bd54969afc6a4d318ee940" ns2:_="" ns3:_="">
     <xsd:import namespace="4613b05c-4671-4207-a6b8-e30994dce502"/>
@@ -3596,27 +3632,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
+    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
+    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A9BCE7-9EE4-4695-9AF6-872741DC1E3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3633,24 +3669,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
-    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
-    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
agregado de etiquetas 302- HE aguja trozos H 2C- jabat
</commit_message>
<xml_diff>
--- a/Copia de Copia de Codigos CHABAT NICO.xlsx
+++ b/Copia de Copia de Codigos CHABAT NICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3CE68BA-85ED-433F-9F37-7F9816CDD4DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E9468B-B31E-483E-989C-7E6F9A83DF81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1284,6 +1284,21 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1319,21 +1334,6 @@
     </xf>
     <xf numFmtId="44" fontId="4" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1630,7 +1630,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N9" sqref="N9"/>
+      <selection pane="bottomLeft" activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="61.5" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1667,31 +1667,31 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="90" t="s">
+      <c r="A2" s="95" t="s">
         <v>122</v>
       </c>
       <c r="B2" s="7"/>
-      <c r="C2" s="84" t="s">
+      <c r="C2" s="89" t="s">
         <v>104</v>
       </c>
-      <c r="D2" s="88" t="s">
+      <c r="D2" s="93" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="88" t="s">
+      <c r="E2" s="93" t="s">
         <v>52</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-      <c r="H2" s="84" t="s">
+      <c r="H2" s="89" t="s">
         <v>113</v>
       </c>
-      <c r="I2" s="92" t="s">
+      <c r="I2" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="94" t="s">
+      <c r="J2" s="99" t="s">
         <v>123</v>
       </c>
-      <c r="K2" s="86" t="s">
+      <c r="K2" s="91" t="s">
         <v>20</v>
       </c>
       <c r="L2" s="2" t="s">
@@ -1704,25 +1704,25 @@
       </c>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="91"/>
+      <c r="A3" s="96"/>
       <c r="B3" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="85" t="s">
+      <c r="C3" s="90" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="94"/>
       <c r="F3" s="9" t="s">
         <v>105</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="H3" s="85"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="95"/>
-      <c r="K3" s="87"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="92"/>
       <c r="L3" s="60" t="s">
         <v>168</v>
       </c>
@@ -1971,7 +1971,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" s="1" customFormat="1" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>23</v>
       </c>
@@ -2008,9 +2008,11 @@
       <c r="L9" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M9" s="67"/>
+      <c r="M9" s="67">
+        <v>302</v>
+      </c>
       <c r="N9" s="67" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="O9" s="65" t="s">
         <v>190</v>
@@ -3178,12 +3180,12 @@
         <v>195</v>
       </c>
       <c r="O36" s="65"/>
-      <c r="P36" s="100" t="s">
+      <c r="P36" s="88" t="s">
         <v>199</v>
       </c>
-      <c r="Q36" s="97">
+      <c r="Q36" s="85">
         <f>COUNTIF(N4:N38,"CERO")</f>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:17" ht="57" x14ac:dyDescent="0.25">
@@ -3228,12 +3230,12 @@
         <v>195</v>
       </c>
       <c r="O37" s="65"/>
-      <c r="P37" s="98" t="s">
+      <c r="P37" s="86" t="s">
         <v>196</v>
       </c>
-      <c r="Q37" s="99">
+      <c r="Q37" s="87">
         <f>COUNTIF(N4:N38,"OK")</f>
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:17" s="1" customFormat="1" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3278,10 +3280,10 @@
         <v>195</v>
       </c>
       <c r="O38" s="65"/>
-      <c r="P38" s="96" t="s">
+      <c r="P38" s="84" t="s">
         <v>197</v>
       </c>
-      <c r="Q38" s="99">
+      <c r="Q38" s="87">
         <f>COUNTIF(N4:N38,"FALTA")</f>
         <v>0</v>
       </c>
@@ -3299,10 +3301,10 @@
       <c r="M39" s="5"/>
       <c r="N39" s="5"/>
       <c r="O39" s="59"/>
-      <c r="P39" s="98" t="s">
+      <c r="P39" s="86" t="s">
         <v>198</v>
       </c>
-      <c r="Q39" s="99">
+      <c r="Q39" s="87">
         <f>COUNTIF(N4:N38,"")</f>
         <v>0</v>
       </c>
@@ -3390,26 +3392,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="מסמך" ma:contentTypeID="0x010100E111FB68E4AB3A458E6F1E68F8888CED" ma:contentTypeVersion="13" ma:contentTypeDescription="צור מסמך חדש." ma:contentTypeScope="" ma:versionID="bfe1cfa8ea064de69b4e2203b8e1e509">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4613b05c-4671-4207-a6b8-e30994dce502" xmlns:ns3="ae89acfa-0242-4570-84ca-e3aafb74daca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b8d078cf0bd54969afc6a4d318ee940" ns2:_="" ns3:_="">
     <xsd:import namespace="4613b05c-4671-4207-a6b8-e30994dce502"/>
@@ -3632,27 +3614,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
-    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
-    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A9BCE7-9EE4-4695-9AF6-872741DC1E3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3669,4 +3651,24 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
+    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
+    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
agregado de etiqueta 303-HE-PECHO 3A - jabat
</commit_message>
<xml_diff>
--- a/Copia de Copia de Codigos CHABAT NICO.xlsx
+++ b/Copia de Copia de Codigos CHABAT NICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E9468B-B31E-483E-989C-7E6F9A83DF81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F572A3-8E05-47DB-9663-CE30E19E5F99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1033,7 +1033,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1334,6 +1334,9 @@
     </xf>
     <xf numFmtId="44" fontId="4" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1630,7 +1633,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N10" sqref="N10"/>
+      <selection pane="bottomLeft" activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="61.5" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2068,7 +2071,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" s="1" customFormat="1" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>24</v>
       </c>
@@ -2105,9 +2108,11 @@
       <c r="L11" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M11" s="67"/>
+      <c r="M11" s="67">
+        <v>303</v>
+      </c>
       <c r="N11" s="67" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="O11" s="65"/>
     </row>
@@ -2151,7 +2156,7 @@
       <c r="M12" s="68">
         <v>172</v>
       </c>
-      <c r="N12" s="68" t="s">
+      <c r="N12" s="101" t="s">
         <v>195</v>
       </c>
       <c r="O12" s="65">
@@ -3185,7 +3190,7 @@
       </c>
       <c r="Q36" s="85">
         <f>COUNTIF(N4:N38,"CERO")</f>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:17" ht="57" x14ac:dyDescent="0.25">
@@ -3235,7 +3240,7 @@
       </c>
       <c r="Q37" s="87">
         <f>COUNTIF(N4:N38,"OK")</f>
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:17" s="1" customFormat="1" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3392,6 +3397,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="מסמך" ma:contentTypeID="0x010100E111FB68E4AB3A458E6F1E68F8888CED" ma:contentTypeVersion="13" ma:contentTypeDescription="צור מסמך חדש." ma:contentTypeScope="" ma:versionID="bfe1cfa8ea064de69b4e2203b8e1e509">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4613b05c-4671-4207-a6b8-e30994dce502" xmlns:ns3="ae89acfa-0242-4570-84ca-e3aafb74daca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b8d078cf0bd54969afc6a4d318ee940" ns2:_="" ns3:_="">
     <xsd:import namespace="4613b05c-4671-4207-a6b8-e30994dce502"/>
@@ -3614,27 +3639,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
+    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
+    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A9BCE7-9EE4-4695-9AF6-872741DC1E3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3651,24 +3676,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
-    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
-    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
agregado de etiquetas hasta 305 - jabat
</commit_message>
<xml_diff>
--- a/Copia de Copia de Codigos CHABAT NICO.xlsx
+++ b/Copia de Copia de Codigos CHABAT NICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F572A3-8E05-47DB-9663-CE30E19E5F99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151DF20A-70CB-4283-9D0F-F870EF63FD71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1033,7 +1033,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1299,6 +1299,12 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1334,9 +1340,6 @@
     </xf>
     <xf numFmtId="44" fontId="4" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1632,8 +1635,8 @@
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N12" sqref="N12"/>
+      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="61.5" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1670,31 +1673,31 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="95" t="s">
+      <c r="A2" s="97" t="s">
         <v>122</v>
       </c>
       <c r="B2" s="7"/>
-      <c r="C2" s="89" t="s">
+      <c r="C2" s="91" t="s">
         <v>104</v>
       </c>
-      <c r="D2" s="93" t="s">
+      <c r="D2" s="95" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="93" t="s">
+      <c r="E2" s="95" t="s">
         <v>52</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-      <c r="H2" s="89" t="s">
+      <c r="H2" s="91" t="s">
         <v>113</v>
       </c>
-      <c r="I2" s="97" t="s">
+      <c r="I2" s="99" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="99" t="s">
+      <c r="J2" s="101" t="s">
         <v>123</v>
       </c>
-      <c r="K2" s="91" t="s">
+      <c r="K2" s="93" t="s">
         <v>20</v>
       </c>
       <c r="L2" s="2" t="s">
@@ -1707,25 +1710,25 @@
       </c>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="96"/>
+      <c r="A3" s="98"/>
       <c r="B3" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="90" t="s">
+      <c r="C3" s="92" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="94"/>
-      <c r="E3" s="94"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
       <c r="F3" s="9" t="s">
         <v>105</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="H3" s="90"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="100"/>
-      <c r="K3" s="92"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="102"/>
+      <c r="K3" s="94"/>
       <c r="L3" s="60" t="s">
         <v>168</v>
       </c>
@@ -2116,7 +2119,7 @@
       </c>
       <c r="O11" s="65"/>
     </row>
-    <row r="12" spans="1:17" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" s="1" customFormat="1" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18">
         <v>33</v>
       </c>
@@ -2147,7 +2150,7 @@
       <c r="J12" s="52">
         <v>103522</v>
       </c>
-      <c r="K12" s="76" t="s">
+      <c r="K12" s="90" t="s">
         <v>128</v>
       </c>
       <c r="L12" s="62" t="s">
@@ -2156,7 +2159,7 @@
       <c r="M12" s="68">
         <v>172</v>
       </c>
-      <c r="N12" s="101" t="s">
+      <c r="N12" s="89" t="s">
         <v>195</v>
       </c>
       <c r="O12" s="65">
@@ -2166,7 +2169,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" s="1" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>25</v>
       </c>
@@ -2203,9 +2206,11 @@
       <c r="L13" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M13" s="67"/>
+      <c r="M13" s="67">
+        <v>304</v>
+      </c>
       <c r="N13" s="67" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="O13" s="65"/>
     </row>
@@ -2254,7 +2259,7 @@
       </c>
       <c r="O14" s="65"/>
     </row>
-    <row r="15" spans="1:17" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" s="1" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18">
         <v>44</v>
       </c>
@@ -2285,15 +2290,17 @@
       <c r="J15" s="52">
         <v>104521</v>
       </c>
-      <c r="K15" s="76" t="s">
+      <c r="K15" s="90" t="s">
         <v>131</v>
       </c>
       <c r="L15" s="62" t="s">
         <v>169</v>
       </c>
-      <c r="M15" s="68"/>
+      <c r="M15" s="68">
+        <v>305</v>
+      </c>
       <c r="N15" s="68" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="O15" s="65"/>
     </row>
@@ -3190,7 +3197,7 @@
       </c>
       <c r="Q36" s="85">
         <f>COUNTIF(N4:N38,"CERO")</f>
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:17" ht="57" x14ac:dyDescent="0.25">
@@ -3240,7 +3247,7 @@
       </c>
       <c r="Q37" s="87">
         <f>COUNTIF(N4:N38,"OK")</f>
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:17" s="1" customFormat="1" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
agregado de etiquetas 306-HE PALETA BLOQ 4C - jabat
</commit_message>
<xml_diff>
--- a/Copia de Copia de Codigos CHABAT NICO.xlsx
+++ b/Copia de Copia de Codigos CHABAT NICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151DF20A-70CB-4283-9D0F-F870EF63FD71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1967F60C-C99F-4993-868A-231B6813E492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1635,8 +1635,8 @@
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N16" sqref="N16"/>
+      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="61.5" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2304,7 +2304,7 @@
       </c>
       <c r="O15" s="65"/>
     </row>
-    <row r="16" spans="1:17" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" s="1" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>26</v>
       </c>
@@ -2339,9 +2339,11 @@
       <c r="L16" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M16" s="67"/>
+      <c r="M16" s="67">
+        <v>306</v>
+      </c>
       <c r="N16" s="67" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="O16" s="65"/>
     </row>
@@ -3197,7 +3199,7 @@
       </c>
       <c r="Q36" s="85">
         <f>COUNTIF(N4:N38,"CERO")</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:17" ht="57" x14ac:dyDescent="0.25">
@@ -3247,7 +3249,7 @@
       </c>
       <c r="Q37" s="87">
         <f>COUNTIF(N4:N38,"OK")</f>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:17" s="1" customFormat="1" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3404,26 +3406,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="מסמך" ma:contentTypeID="0x010100E111FB68E4AB3A458E6F1E68F8888CED" ma:contentTypeVersion="13" ma:contentTypeDescription="צור מסמך חדש." ma:contentTypeScope="" ma:versionID="bfe1cfa8ea064de69b4e2203b8e1e509">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4613b05c-4671-4207-a6b8-e30994dce502" xmlns:ns3="ae89acfa-0242-4570-84ca-e3aafb74daca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b8d078cf0bd54969afc6a4d318ee940" ns2:_="" ns3:_="">
     <xsd:import namespace="4613b05c-4671-4207-a6b8-e30994dce502"/>
@@ -3646,27 +3628,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
-    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
-    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A9BCE7-9EE4-4695-9AF6-872741DC1E3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3683,4 +3665,24 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
+    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
+    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
agregado de etiquetas 307-HE-MARUCHA TRZ 55 - jabat
</commit_message>
<xml_diff>
--- a/Copia de Copia de Codigos CHABAT NICO.xlsx
+++ b/Copia de Copia de Codigos CHABAT NICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1967F60C-C99F-4993-868A-231B6813E492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC41F89-F3F1-4106-9E2C-7BF1FD10CD64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1635,8 +1635,8 @@
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N17" sqref="N17"/>
+      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="61.5" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2390,7 +2390,7 @@
       </c>
       <c r="O17" s="65"/>
     </row>
-    <row r="18" spans="1:15" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" s="1" customFormat="1" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18">
         <v>55</v>
       </c>
@@ -2421,15 +2421,17 @@
       <c r="J18" s="52">
         <v>105521</v>
       </c>
-      <c r="K18" s="76" t="s">
+      <c r="K18" s="90" t="s">
         <v>134</v>
       </c>
       <c r="L18" s="62" t="s">
         <v>169</v>
       </c>
-      <c r="M18" s="68"/>
+      <c r="M18" s="68">
+        <v>307</v>
+      </c>
       <c r="N18" s="68" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="O18" s="65"/>
     </row>
@@ -3199,7 +3201,7 @@
       </c>
       <c r="Q36" s="85">
         <f>COUNTIF(N4:N38,"CERO")</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:17" ht="57" x14ac:dyDescent="0.25">
@@ -3249,7 +3251,7 @@
       </c>
       <c r="Q37" s="87">
         <f>COUNTIF(N4:N38,"OK")</f>
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:17" s="1" customFormat="1" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3406,6 +3408,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="מסמך" ma:contentTypeID="0x010100E111FB68E4AB3A458E6F1E68F8888CED" ma:contentTypeVersion="13" ma:contentTypeDescription="צור מסמך חדש." ma:contentTypeScope="" ma:versionID="bfe1cfa8ea064de69b4e2203b8e1e509">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4613b05c-4671-4207-a6b8-e30994dce502" xmlns:ns3="ae89acfa-0242-4570-84ca-e3aafb74daca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b8d078cf0bd54969afc6a4d318ee940" ns2:_="" ns3:_="">
     <xsd:import namespace="4613b05c-4671-4207-a6b8-e30994dce502"/>
@@ -3628,27 +3650,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
+    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
+    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A9BCE7-9EE4-4695-9AF6-872741DC1E3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3665,24 +3687,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
-    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
-    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
agregado de etiquetas 308 Y 309 - jabat
</commit_message>
<xml_diff>
--- a/Copia de Copia de Codigos CHABAT NICO.xlsx
+++ b/Copia de Copia de Codigos CHABAT NICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC41F89-F3F1-4106-9E2C-7BF1FD10CD64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB506E3-568B-4B39-B58F-A724F8BAB1CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1635,8 +1635,8 @@
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N19" sqref="N19"/>
+      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="61.5" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2609,7 +2609,7 @@
       </c>
       <c r="O22" s="65"/>
     </row>
-    <row r="23" spans="1:15" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" s="1" customFormat="1" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="22"/>
       <c r="B23" s="23" t="s">
         <v>187</v>
@@ -2642,9 +2642,11 @@
       <c r="L23" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M23" s="67"/>
+      <c r="M23" s="67">
+        <v>308</v>
+      </c>
       <c r="N23" s="67" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="O23" s="65"/>
     </row>
@@ -2693,7 +2695,7 @@
       </c>
       <c r="O24" s="65"/>
     </row>
-    <row r="25" spans="1:15" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" s="1" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
         <v>8</v>
       </c>
@@ -2730,9 +2732,11 @@
       <c r="L25" s="61" t="s">
         <v>173</v>
       </c>
-      <c r="M25" s="67"/>
+      <c r="M25" s="67">
+        <v>309</v>
+      </c>
       <c r="N25" s="67" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="O25" s="65"/>
     </row>
@@ -3201,7 +3205,7 @@
       </c>
       <c r="Q36" s="85">
         <f>COUNTIF(N4:N38,"CERO")</f>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:17" ht="57" x14ac:dyDescent="0.25">
@@ -3251,7 +3255,7 @@
       </c>
       <c r="Q37" s="87">
         <f>COUNTIF(N4:N38,"OK")</f>
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:17" s="1" customFormat="1" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3408,26 +3412,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="מסמך" ma:contentTypeID="0x010100E111FB68E4AB3A458E6F1E68F8888CED" ma:contentTypeVersion="13" ma:contentTypeDescription="צור מסמך חדש." ma:contentTypeScope="" ma:versionID="bfe1cfa8ea064de69b4e2203b8e1e509">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4613b05c-4671-4207-a6b8-e30994dce502" xmlns:ns3="ae89acfa-0242-4570-84ca-e3aafb74daca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b8d078cf0bd54969afc6a4d318ee940" ns2:_="" ns3:_="">
     <xsd:import namespace="4613b05c-4671-4207-a6b8-e30994dce502"/>
@@ -3650,27 +3634,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
-    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
-    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A9BCE7-9EE4-4695-9AF6-872741DC1E3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3687,4 +3671,24 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
+    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
+    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
agregado de etiqueta 310-HE-ASADO CH 9C - jabat
</commit_message>
<xml_diff>
--- a/Copia de Copia de Codigos CHABAT NICO.xlsx
+++ b/Copia de Copia de Codigos CHABAT NICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB506E3-568B-4B39-B58F-A724F8BAB1CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5435906-6B6F-4BA5-9702-8DAD97E96A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="200">
   <si>
     <t>לשון בקר קפוא</t>
   </si>
@@ -637,9 +637,6 @@
   </si>
   <si>
     <t>DE CERO</t>
-  </si>
-  <si>
-    <t>CERO</t>
   </si>
 </sst>
 </file>
@@ -1635,8 +1632,8 @@
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N26" sqref="N26"/>
+      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="61.5" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2916,7 +2913,7 @@
       </c>
       <c r="O29" s="65"/>
     </row>
-    <row r="30" spans="1:15" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" s="1" customFormat="1" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="14" t="s">
         <v>187</v>
@@ -2949,9 +2946,11 @@
       <c r="L30" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M30" s="67"/>
+      <c r="M30" s="67">
+        <v>310</v>
+      </c>
       <c r="N30" s="67" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="O30" s="65"/>
     </row>
@@ -3205,7 +3204,7 @@
       </c>
       <c r="Q36" s="85">
         <f>COUNTIF(N4:N38,"CERO")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:17" ht="57" x14ac:dyDescent="0.25">
@@ -3255,7 +3254,7 @@
       </c>
       <c r="Q37" s="87">
         <f>COUNTIF(N4:N38,"OK")</f>
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:17" s="1" customFormat="1" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3412,6 +3411,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="מסמך" ma:contentTypeID="0x010100E111FB68E4AB3A458E6F1E68F8888CED" ma:contentTypeVersion="13" ma:contentTypeDescription="צור מסמך חדש." ma:contentTypeScope="" ma:versionID="bfe1cfa8ea064de69b4e2203b8e1e509">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4613b05c-4671-4207-a6b8-e30994dce502" xmlns:ns3="ae89acfa-0242-4570-84ca-e3aafb74daca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b8d078cf0bd54969afc6a4d318ee940" ns2:_="" ns3:_="">
     <xsd:import namespace="4613b05c-4671-4207-a6b8-e30994dce502"/>
@@ -3634,27 +3653,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
+    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
+    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A9BCE7-9EE4-4695-9AF6-872741DC1E3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3671,24 +3690,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
-    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
-    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
agregado de etiqueta 311-he-braz bloq 8a - jabat
</commit_message>
<xml_diff>
--- a/Copia de Copia de Codigos CHABAT NICO.xlsx
+++ b/Copia de Copia de Codigos CHABAT NICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5435906-6B6F-4BA5-9702-8DAD97E96A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484403BB-3E9A-4487-8F75-DF286482A45E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1633,7 +1633,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N31" sqref="N31"/>
+      <selection pane="bottomLeft" activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="61.5" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -3411,26 +3411,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="מסמך" ma:contentTypeID="0x010100E111FB68E4AB3A458E6F1E68F8888CED" ma:contentTypeVersion="13" ma:contentTypeDescription="צור מסמך חדש." ma:contentTypeScope="" ma:versionID="bfe1cfa8ea064de69b4e2203b8e1e509">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4613b05c-4671-4207-a6b8-e30994dce502" xmlns:ns3="ae89acfa-0242-4570-84ca-e3aafb74daca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b8d078cf0bd54969afc6a4d318ee940" ns2:_="" ns3:_="">
     <xsd:import namespace="4613b05c-4671-4207-a6b8-e30994dce502"/>
@@ -3653,27 +3633,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
-    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
-    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A9BCE7-9EE4-4695-9AF6-872741DC1E3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3690,4 +3670,24 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
+    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
+    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fin de edicion de etiquetas jabat
</commit_message>
<xml_diff>
--- a/Copia de Copia de Codigos CHABAT NICO.xlsx
+++ b/Copia de Copia de Codigos CHABAT NICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484403BB-3E9A-4487-8F75-DF286482A45E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991F9805-D197-4A99-B61B-91D6B331170C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -647,7 +647,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -757,43 +757,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="44"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="36"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="42"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Fira Code"/>
+      <name val="Cascadia Code"/>
+      <family val="3"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Fira Code"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Ebrima"/>
+      <name val="Cascadia Code"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1030,7 +1003,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1248,60 +1221,9 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" readingOrder="2"/>
     </xf>
-    <xf numFmtId="1" fontId="15" fillId="2" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="2" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="2" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="3" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="1" fontId="16" fillId="2" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="1" fontId="17" fillId="2" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1337,6 +1259,45 @@
     </xf>
     <xf numFmtId="44" fontId="4" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1631,9 +1592,9 @@
   </sheetPr>
   <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M23" sqref="M23"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N37" sqref="N37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="61.5" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1648,11 +1609,11 @@
     <col min="8" max="8" width="26.85546875" style="5" customWidth="1"/>
     <col min="9" max="9" width="16.7109375" style="4" customWidth="1"/>
     <col min="10" max="10" width="11" style="50" customWidth="1"/>
-    <col min="11" max="11" width="119" style="72" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28" style="72" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="12.42578125" style="4" customWidth="1"/>
     <col min="15" max="15" width="18.28515625" style="58" customWidth="1"/>
-    <col min="16" max="16" width="19.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="18" max="16384" width="11.42578125" style="4"/>
   </cols>
@@ -1670,31 +1631,31 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="80" t="s">
         <v>122</v>
       </c>
       <c r="B2" s="7"/>
-      <c r="C2" s="91" t="s">
+      <c r="C2" s="74" t="s">
         <v>104</v>
       </c>
-      <c r="D2" s="95" t="s">
+      <c r="D2" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="95" t="s">
+      <c r="E2" s="78" t="s">
         <v>52</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-      <c r="H2" s="91" t="s">
+      <c r="H2" s="74" t="s">
         <v>113</v>
       </c>
-      <c r="I2" s="99" t="s">
+      <c r="I2" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="101" t="s">
+      <c r="J2" s="84" t="s">
         <v>123</v>
       </c>
-      <c r="K2" s="93" t="s">
+      <c r="K2" s="76" t="s">
         <v>20</v>
       </c>
       <c r="L2" s="2" t="s">
@@ -1707,25 +1668,25 @@
       </c>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="98"/>
+      <c r="A3" s="81"/>
       <c r="B3" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="92" t="s">
+      <c r="C3" s="75" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
       <c r="F3" s="9" t="s">
         <v>105</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="H3" s="92"/>
-      <c r="I3" s="100"/>
-      <c r="J3" s="102"/>
-      <c r="K3" s="94"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="83"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="77"/>
       <c r="L3" s="60" t="s">
         <v>168</v>
       </c>
@@ -1742,7 +1703,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="1" customFormat="1" ht="57.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" s="1" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>171</v>
       </c>
@@ -1773,7 +1734,7 @@
       <c r="J4" s="51">
         <v>101861</v>
       </c>
-      <c r="K4" s="73" t="s">
+      <c r="K4" s="86" t="s">
         <v>91</v>
       </c>
       <c r="L4" s="61" t="s">
@@ -1792,7 +1753,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>18</v>
       </c>
@@ -1823,7 +1784,7 @@
       <c r="J5" s="51">
         <v>101862</v>
       </c>
-      <c r="K5" s="74" t="s">
+      <c r="K5" s="87" t="s">
         <v>91</v>
       </c>
       <c r="L5" s="61" t="s">
@@ -1866,7 +1827,7 @@
       <c r="J6" s="51">
         <v>101865</v>
       </c>
-      <c r="K6" s="74" t="s">
+      <c r="K6" s="87" t="s">
         <v>54</v>
       </c>
       <c r="L6" s="61" t="s">
@@ -1882,7 +1843,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>2</v>
       </c>
@@ -1913,7 +1874,7 @@
       <c r="J7" s="51">
         <v>102531</v>
       </c>
-      <c r="K7" s="75" t="s">
+      <c r="K7" s="88" t="s">
         <v>124</v>
       </c>
       <c r="L7" s="61" t="s">
@@ -1958,7 +1919,7 @@
       <c r="J8" s="51">
         <v>102532</v>
       </c>
-      <c r="K8" s="75" t="s">
+      <c r="K8" s="88" t="s">
         <v>125</v>
       </c>
       <c r="L8" s="61" t="s">
@@ -2005,7 +1966,7 @@
       <c r="J9" s="51">
         <v>102533</v>
       </c>
-      <c r="K9" s="75" t="s">
+      <c r="K9" s="88" t="s">
         <v>126</v>
       </c>
       <c r="L9" s="61" t="s">
@@ -2021,7 +1982,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="18">
         <v>22</v>
       </c>
@@ -2052,7 +2013,7 @@
       <c r="J10" s="52">
         <v>102534</v>
       </c>
-      <c r="K10" s="76" t="s">
+      <c r="K10" s="89" t="s">
         <v>97</v>
       </c>
       <c r="L10" s="62" t="s">
@@ -2102,7 +2063,7 @@
       <c r="J11" s="51">
         <v>103521</v>
       </c>
-      <c r="K11" s="75" t="s">
+      <c r="K11" s="88" t="s">
         <v>127</v>
       </c>
       <c r="L11" s="61" t="s">
@@ -2156,7 +2117,7 @@
       <c r="M12" s="68">
         <v>172</v>
       </c>
-      <c r="N12" s="89" t="s">
+      <c r="N12" s="73" t="s">
         <v>195</v>
       </c>
       <c r="O12" s="65">
@@ -2197,7 +2158,7 @@
       <c r="J13" s="51">
         <v>103523</v>
       </c>
-      <c r="K13" s="75" t="s">
+      <c r="K13" s="88" t="s">
         <v>129</v>
       </c>
       <c r="L13" s="61" t="s">
@@ -2211,7 +2172,7 @@
       </c>
       <c r="O13" s="65"/>
     </row>
-    <row r="14" spans="1:17" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="16">
         <v>3</v>
       </c>
@@ -2242,7 +2203,7 @@
       <c r="J14" s="51">
         <v>103524</v>
       </c>
-      <c r="K14" s="75" t="s">
+      <c r="K14" s="88" t="s">
         <v>130</v>
       </c>
       <c r="L14" s="61" t="s">
@@ -2330,7 +2291,7 @@
       <c r="J16" s="51">
         <v>104522</v>
       </c>
-      <c r="K16" s="75" t="s">
+      <c r="K16" s="88" t="s">
         <v>132</v>
       </c>
       <c r="L16" s="61" t="s">
@@ -2344,7 +2305,7 @@
       </c>
       <c r="O16" s="65"/>
     </row>
-    <row r="17" spans="1:15" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="16">
         <v>4</v>
       </c>
@@ -2373,7 +2334,7 @@
       <c r="J17" s="51">
         <v>104523</v>
       </c>
-      <c r="K17" s="75" t="s">
+      <c r="K17" s="88" t="s">
         <v>133</v>
       </c>
       <c r="L17" s="61" t="s">
@@ -2432,7 +2393,7 @@
       </c>
       <c r="O18" s="65"/>
     </row>
-    <row r="19" spans="1:15" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="13">
         <v>5</v>
       </c>
@@ -2461,7 +2422,7 @@
       <c r="J19" s="51">
         <v>105522</v>
       </c>
-      <c r="K19" s="77" t="s">
+      <c r="K19" s="91" t="s">
         <v>92</v>
       </c>
       <c r="L19" s="61" t="s">
@@ -2475,7 +2436,7 @@
       </c>
       <c r="O19" s="65"/>
     </row>
-    <row r="20" spans="1:15" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
         <v>6</v>
       </c>
@@ -2504,7 +2465,7 @@
       <c r="J20" s="51">
         <v>106521</v>
       </c>
-      <c r="K20" s="77" t="s">
+      <c r="K20" s="91" t="s">
         <v>93</v>
       </c>
       <c r="L20" s="61" t="s">
@@ -2518,7 +2479,7 @@
       </c>
       <c r="O20" s="65"/>
     </row>
-    <row r="21" spans="1:15" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>5</v>
       </c>
@@ -2547,7 +2508,7 @@
       <c r="J21" s="51">
         <v>107521</v>
       </c>
-      <c r="K21" s="77" t="s">
+      <c r="K21" s="91" t="s">
         <v>94</v>
       </c>
       <c r="L21" s="61" t="s">
@@ -2561,7 +2522,7 @@
       </c>
       <c r="O21" s="65"/>
     </row>
-    <row r="22" spans="1:15" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
         <v>8</v>
       </c>
@@ -2592,7 +2553,7 @@
       <c r="J22" s="51">
         <v>108521</v>
       </c>
-      <c r="K22" s="77" t="s">
+      <c r="K22" s="91" t="s">
         <v>95</v>
       </c>
       <c r="L22" s="61" t="s">
@@ -2633,7 +2594,7 @@
       <c r="J23" s="51">
         <v>108522</v>
       </c>
-      <c r="K23" s="77" t="s">
+      <c r="K23" s="91" t="s">
         <v>96</v>
       </c>
       <c r="L23" s="61" t="s">
@@ -2647,7 +2608,7 @@
       </c>
       <c r="O23" s="65"/>
     </row>
-    <row r="24" spans="1:15" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
         <v>6</v>
       </c>
@@ -2678,7 +2639,7 @@
       <c r="J24" s="51">
         <v>110531</v>
       </c>
-      <c r="K24" s="78" t="s">
+      <c r="K24" s="92" t="s">
         <v>4</v>
       </c>
       <c r="L24" s="61" t="s">
@@ -2723,7 +2684,7 @@
       <c r="J25" s="51">
         <v>110532</v>
       </c>
-      <c r="K25" s="75" t="s">
+      <c r="K25" s="88" t="s">
         <v>135</v>
       </c>
       <c r="L25" s="61" t="s">
@@ -2737,7 +2698,7 @@
       </c>
       <c r="O25" s="65"/>
     </row>
-    <row r="26" spans="1:15" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="16">
         <v>10</v>
       </c>
@@ -2768,7 +2729,7 @@
       <c r="J26" s="51">
         <v>110533</v>
       </c>
-      <c r="K26" s="75" t="s">
+      <c r="K26" s="88" t="s">
         <v>136</v>
       </c>
       <c r="L26" s="61" t="s">
@@ -2782,7 +2743,7 @@
       </c>
       <c r="O26" s="65"/>
     </row>
-    <row r="27" spans="1:15" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>7</v>
       </c>
@@ -2811,7 +2772,7 @@
       <c r="J27" s="51">
         <v>170521</v>
       </c>
-      <c r="K27" s="77" t="s">
+      <c r="K27" s="91" t="s">
         <v>98</v>
       </c>
       <c r="L27" s="61" t="s">
@@ -2856,7 +2817,7 @@
       <c r="J28" s="51">
         <v>109521</v>
       </c>
-      <c r="K28" s="83" t="s">
+      <c r="K28" s="88" t="s">
         <v>137</v>
       </c>
       <c r="L28" s="61" t="s">
@@ -2899,7 +2860,7 @@
       <c r="J29" s="51">
         <v>109522</v>
       </c>
-      <c r="K29" s="77" t="s">
+      <c r="K29" s="91" t="s">
         <v>99</v>
       </c>
       <c r="L29" s="61" t="s">
@@ -2940,7 +2901,7 @@
       <c r="J30" s="51">
         <v>109523</v>
       </c>
-      <c r="K30" s="77" t="s">
+      <c r="K30" s="91" t="s">
         <v>100</v>
       </c>
       <c r="L30" s="61" t="s">
@@ -2954,7 +2915,7 @@
       </c>
       <c r="O30" s="65"/>
     </row>
-    <row r="31" spans="1:15" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
       <c r="B31" s="14" t="s">
         <v>187</v>
@@ -2981,7 +2942,7 @@
       <c r="J31" s="51">
         <v>157521</v>
       </c>
-      <c r="K31" s="77" t="s">
+      <c r="K31" s="91" t="s">
         <v>1</v>
       </c>
       <c r="L31" s="61" t="s">
@@ -2995,7 +2956,7 @@
       </c>
       <c r="O31" s="65"/>
     </row>
-    <row r="32" spans="1:15" s="1" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
       <c r="B32" s="14" t="s">
         <v>187</v>
@@ -3024,7 +2985,7 @@
       <c r="J32" s="51">
         <v>109524</v>
       </c>
-      <c r="K32" s="82" t="s">
+      <c r="K32" s="91" t="s">
         <v>2</v>
       </c>
       <c r="L32" s="61" t="s">
@@ -3038,7 +2999,7 @@
       </c>
       <c r="O32" s="65"/>
     </row>
-    <row r="33" spans="1:17" s="1" customFormat="1" ht="46.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
       <c r="B33" s="14" t="s">
         <v>187</v>
@@ -3063,7 +3024,7 @@
       <c r="J33" s="51">
         <v>109525</v>
       </c>
-      <c r="K33" s="81" t="s">
+      <c r="K33" s="91" t="s">
         <v>53</v>
       </c>
       <c r="L33" s="61" t="s">
@@ -3077,7 +3038,7 @@
       </c>
       <c r="O33" s="65"/>
     </row>
-    <row r="34" spans="1:17" ht="57" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34" s="14" t="s">
         <v>187</v>
@@ -3104,7 +3065,7 @@
       <c r="J34" s="51">
         <v>155521</v>
       </c>
-      <c r="K34" s="75" t="s">
+      <c r="K34" s="88" t="s">
         <v>56</v>
       </c>
       <c r="L34" s="61" t="s">
@@ -3118,7 +3079,7 @@
       </c>
       <c r="O34" s="65"/>
     </row>
-    <row r="35" spans="1:17" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="25"/>
       <c r="B35" s="26" t="s">
         <v>187</v>
@@ -3145,7 +3106,7 @@
       <c r="J35" s="53">
         <v>153521</v>
       </c>
-      <c r="K35" s="79" t="s">
+      <c r="K35" s="93" t="s">
         <v>0</v>
       </c>
       <c r="L35" s="63" t="s">
@@ -3159,7 +3120,7 @@
       </c>
       <c r="O35" s="65"/>
     </row>
-    <row r="36" spans="1:17" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A36" s="25"/>
       <c r="B36" s="26" t="s">
         <v>187</v>
@@ -3186,7 +3147,7 @@
       <c r="J36" s="53">
         <v>150521</v>
       </c>
-      <c r="K36" s="79" t="s">
+      <c r="K36" s="93" t="s">
         <v>3</v>
       </c>
       <c r="L36" s="63" t="s">
@@ -3199,15 +3160,15 @@
         <v>195</v>
       </c>
       <c r="O36" s="65"/>
-      <c r="P36" s="88" t="s">
+      <c r="P36" s="95" t="s">
         <v>199</v>
       </c>
-      <c r="Q36" s="85">
+      <c r="Q36" s="96">
         <f>COUNTIF(N4:N38,"CERO")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="57" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A37" s="25"/>
       <c r="B37" s="26" t="s">
         <v>187</v>
@@ -3236,7 +3197,7 @@
       <c r="J37" s="53">
         <v>151521</v>
       </c>
-      <c r="K37" s="80" t="s">
+      <c r="K37" s="94" t="s">
         <v>138</v>
       </c>
       <c r="L37" s="63" t="s">
@@ -3249,15 +3210,15 @@
         <v>195</v>
       </c>
       <c r="O37" s="65"/>
-      <c r="P37" s="86" t="s">
+      <c r="P37" s="97" t="s">
         <v>196</v>
       </c>
-      <c r="Q37" s="87">
+      <c r="Q37" s="98">
         <f>COUNTIF(N4:N38,"OK")</f>
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="1" customFormat="1" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="25"/>
       <c r="B38" s="26" t="s">
         <v>187</v>
@@ -3286,7 +3247,7 @@
       <c r="J38" s="53">
         <v>156521</v>
       </c>
-      <c r="K38" s="79" t="s">
+      <c r="K38" s="93" t="s">
         <v>55</v>
       </c>
       <c r="L38" s="63" t="s">
@@ -3299,10 +3260,10 @@
         <v>195</v>
       </c>
       <c r="O38" s="65"/>
-      <c r="P38" s="84" t="s">
+      <c r="P38" s="95" t="s">
         <v>197</v>
       </c>
-      <c r="Q38" s="87">
+      <c r="Q38" s="98">
         <f>COUNTIF(N4:N38,"FALTA")</f>
         <v>0</v>
       </c>
@@ -3320,10 +3281,10 @@
       <c r="M39" s="5"/>
       <c r="N39" s="5"/>
       <c r="O39" s="59"/>
-      <c r="P39" s="86" t="s">
+      <c r="P39" s="97" t="s">
         <v>198</v>
       </c>
-      <c r="Q39" s="87">
+      <c r="Q39" s="98">
         <f>COUNTIF(N4:N38,"")</f>
         <v>0</v>
       </c>
@@ -3411,6 +3372,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="מסמך" ma:contentTypeID="0x010100E111FB68E4AB3A458E6F1E68F8888CED" ma:contentTypeVersion="13" ma:contentTypeDescription="צור מסמך חדש." ma:contentTypeScope="" ma:versionID="bfe1cfa8ea064de69b4e2203b8e1e509">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4613b05c-4671-4207-a6b8-e30994dce502" xmlns:ns3="ae89acfa-0242-4570-84ca-e3aafb74daca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b8d078cf0bd54969afc6a4d318ee940" ns2:_="" ns3:_="">
     <xsd:import namespace="4613b05c-4671-4207-a6b8-e30994dce502"/>
@@ -3633,27 +3614,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
+    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
+    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A9BCE7-9EE4-4695-9AF6-872741DC1E3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3670,24 +3651,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
-    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
-    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
arreglando detalles de etiquetas internas
</commit_message>
<xml_diff>
--- a/Copia de Copia de Codigos CHABAT NICO.xlsx
+++ b/Copia de Copia de Codigos CHABAT NICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991F9805-D197-4A99-B61B-91D6B331170C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC184725-D631-4C20-AFB5-428E98B78061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$Q$43</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$1:$L$38</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -769,7 +770,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -791,6 +792,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1003,7 +1022,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1224,6 +1243,45 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1260,44 +1318,47 @@
     <xf numFmtId="44" fontId="4" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="2" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="2" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="2" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="3" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1593,11 +1654,11 @@
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N37" sqref="N37"/>
+      <pane ySplit="3" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="61.5" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="61.5" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" style="5" customWidth="1"/>
@@ -1631,31 +1692,31 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="80" t="s">
+      <c r="A2" s="93" t="s">
         <v>122</v>
       </c>
       <c r="B2" s="7"/>
-      <c r="C2" s="74" t="s">
+      <c r="C2" s="87" t="s">
         <v>104</v>
       </c>
-      <c r="D2" s="78" t="s">
+      <c r="D2" s="91" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="78" t="s">
+      <c r="E2" s="91" t="s">
         <v>52</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-      <c r="H2" s="74" t="s">
+      <c r="H2" s="87" t="s">
         <v>113</v>
       </c>
-      <c r="I2" s="82" t="s">
+      <c r="I2" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="84" t="s">
+      <c r="J2" s="97" t="s">
         <v>123</v>
       </c>
-      <c r="K2" s="76" t="s">
+      <c r="K2" s="89" t="s">
         <v>20</v>
       </c>
       <c r="L2" s="2" t="s">
@@ -1668,25 +1729,25 @@
       </c>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="81"/>
+      <c r="A3" s="94"/>
       <c r="B3" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="75" t="s">
+      <c r="C3" s="88" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
+      <c r="D3" s="92"/>
+      <c r="E3" s="92"/>
       <c r="F3" s="9" t="s">
         <v>105</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="H3" s="75"/>
-      <c r="I3" s="83"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="77"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="90"/>
       <c r="L3" s="60" t="s">
         <v>168</v>
       </c>
@@ -1734,7 +1795,7 @@
       <c r="J4" s="51">
         <v>101861</v>
       </c>
-      <c r="K4" s="86" t="s">
+      <c r="K4" s="74" t="s">
         <v>91</v>
       </c>
       <c r="L4" s="61" t="s">
@@ -1784,7 +1845,7 @@
       <c r="J5" s="51">
         <v>101862</v>
       </c>
-      <c r="K5" s="87" t="s">
+      <c r="K5" s="75" t="s">
         <v>91</v>
       </c>
       <c r="L5" s="61" t="s">
@@ -1827,7 +1888,7 @@
       <c r="J6" s="51">
         <v>101865</v>
       </c>
-      <c r="K6" s="87" t="s">
+      <c r="K6" s="75" t="s">
         <v>54</v>
       </c>
       <c r="L6" s="61" t="s">
@@ -1874,13 +1935,13 @@
       <c r="J7" s="51">
         <v>102531</v>
       </c>
-      <c r="K7" s="88" t="s">
+      <c r="K7" s="76" t="s">
         <v>124</v>
       </c>
       <c r="L7" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M7" s="67">
+      <c r="M7" s="101">
         <v>100</v>
       </c>
       <c r="N7" s="67" t="s">
@@ -1891,47 +1952,47 @@
       </c>
     </row>
     <row r="8" spans="1:17" s="1" customFormat="1" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="102" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="103" t="s">
         <v>187</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="104" t="s">
         <v>60</v>
       </c>
-      <c r="D8" s="36" t="s">
+      <c r="D8" s="105" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="37" t="s">
+      <c r="E8" s="106" t="s">
         <v>142</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="104" t="s">
         <v>111</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="104" t="s">
         <v>108</v>
       </c>
-      <c r="H8" s="14"/>
-      <c r="I8" s="15">
+      <c r="H8" s="104"/>
+      <c r="I8" s="107">
         <v>7290019570882</v>
       </c>
-      <c r="J8" s="51">
+      <c r="J8" s="108">
         <v>102532</v>
       </c>
-      <c r="K8" s="88" t="s">
+      <c r="K8" s="109" t="s">
         <v>125</v>
       </c>
-      <c r="L8" s="61" t="s">
+      <c r="L8" s="110" t="s">
         <v>169</v>
       </c>
-      <c r="M8" s="67">
+      <c r="M8" s="111">
         <v>301</v>
       </c>
-      <c r="N8" s="67" t="s">
+      <c r="N8" s="111" t="s">
         <v>195</v>
       </c>
-      <c r="O8" s="65" t="s">
+      <c r="O8" s="112" t="s">
         <v>190</v>
       </c>
     </row>
@@ -1966,14 +2027,14 @@
       <c r="J9" s="51">
         <v>102533</v>
       </c>
-      <c r="K9" s="88" t="s">
+      <c r="K9" s="76" t="s">
         <v>126</v>
       </c>
       <c r="L9" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M9" s="67">
-        <v>302</v>
+      <c r="M9" s="101">
+        <v>352</v>
       </c>
       <c r="N9" s="67" t="s">
         <v>195</v>
@@ -2013,13 +2074,13 @@
       <c r="J10" s="52">
         <v>102534</v>
       </c>
-      <c r="K10" s="89" t="s">
+      <c r="K10" s="77" t="s">
         <v>97</v>
       </c>
       <c r="L10" s="62" t="s">
         <v>169</v>
       </c>
-      <c r="M10" s="68">
+      <c r="M10" s="101">
         <v>130</v>
       </c>
       <c r="N10" s="68" t="s">
@@ -2063,14 +2124,14 @@
       <c r="J11" s="51">
         <v>103521</v>
       </c>
-      <c r="K11" s="88" t="s">
+      <c r="K11" s="76" t="s">
         <v>127</v>
       </c>
       <c r="L11" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M11" s="67">
-        <v>303</v>
+      <c r="M11" s="101">
+        <v>353</v>
       </c>
       <c r="N11" s="67" t="s">
         <v>195</v>
@@ -2108,13 +2169,13 @@
       <c r="J12" s="52">
         <v>103522</v>
       </c>
-      <c r="K12" s="90" t="s">
+      <c r="K12" s="78" t="s">
         <v>128</v>
       </c>
       <c r="L12" s="62" t="s">
         <v>169</v>
       </c>
-      <c r="M12" s="68">
+      <c r="M12" s="101">
         <v>172</v>
       </c>
       <c r="N12" s="73" t="s">
@@ -2158,14 +2219,14 @@
       <c r="J13" s="51">
         <v>103523</v>
       </c>
-      <c r="K13" s="88" t="s">
+      <c r="K13" s="76" t="s">
         <v>129</v>
       </c>
       <c r="L13" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M13" s="67">
-        <v>304</v>
+      <c r="M13" s="101">
+        <v>354</v>
       </c>
       <c r="N13" s="67" t="s">
         <v>195</v>
@@ -2203,13 +2264,13 @@
       <c r="J14" s="51">
         <v>103524</v>
       </c>
-      <c r="K14" s="88" t="s">
+      <c r="K14" s="76" t="s">
         <v>130</v>
       </c>
       <c r="L14" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M14" s="67">
+      <c r="M14" s="101">
         <v>104</v>
       </c>
       <c r="N14" s="67" t="s">
@@ -2248,14 +2309,14 @@
       <c r="J15" s="52">
         <v>104521</v>
       </c>
-      <c r="K15" s="90" t="s">
+      <c r="K15" s="78" t="s">
         <v>131</v>
       </c>
       <c r="L15" s="62" t="s">
         <v>169</v>
       </c>
-      <c r="M15" s="68">
-        <v>305</v>
+      <c r="M15" s="101">
+        <v>355</v>
       </c>
       <c r="N15" s="68" t="s">
         <v>195</v>
@@ -2291,14 +2352,14 @@
       <c r="J16" s="51">
         <v>104522</v>
       </c>
-      <c r="K16" s="88" t="s">
+      <c r="K16" s="76" t="s">
         <v>132</v>
       </c>
       <c r="L16" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M16" s="67">
-        <v>306</v>
+      <c r="M16" s="101">
+        <v>356</v>
       </c>
       <c r="N16" s="67" t="s">
         <v>195</v>
@@ -2334,13 +2395,13 @@
       <c r="J17" s="51">
         <v>104523</v>
       </c>
-      <c r="K17" s="88" t="s">
+      <c r="K17" s="76" t="s">
         <v>133</v>
       </c>
       <c r="L17" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M17" s="67">
+      <c r="M17" s="101">
         <v>111</v>
       </c>
       <c r="N17" s="67" t="s">
@@ -2379,14 +2440,14 @@
       <c r="J18" s="52">
         <v>105521</v>
       </c>
-      <c r="K18" s="90" t="s">
+      <c r="K18" s="78" t="s">
         <v>134</v>
       </c>
       <c r="L18" s="62" t="s">
         <v>169</v>
       </c>
-      <c r="M18" s="68">
-        <v>307</v>
+      <c r="M18" s="101">
+        <v>173</v>
       </c>
       <c r="N18" s="68" t="s">
         <v>195</v>
@@ -2422,13 +2483,13 @@
       <c r="J19" s="51">
         <v>105522</v>
       </c>
-      <c r="K19" s="91" t="s">
+      <c r="K19" s="79" t="s">
         <v>92</v>
       </c>
       <c r="L19" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M19" s="67">
+      <c r="M19" s="101">
         <v>101</v>
       </c>
       <c r="N19" s="67" t="s">
@@ -2465,13 +2526,13 @@
       <c r="J20" s="51">
         <v>106521</v>
       </c>
-      <c r="K20" s="91" t="s">
+      <c r="K20" s="79" t="s">
         <v>93</v>
       </c>
       <c r="L20" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M20" s="67">
+      <c r="M20" s="101">
         <v>102</v>
       </c>
       <c r="N20" s="67" t="s">
@@ -2508,13 +2569,13 @@
       <c r="J21" s="51">
         <v>107521</v>
       </c>
-      <c r="K21" s="91" t="s">
+      <c r="K21" s="79" t="s">
         <v>94</v>
       </c>
       <c r="L21" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M21" s="67">
+      <c r="M21" s="101">
         <v>120</v>
       </c>
       <c r="N21" s="67" t="s">
@@ -2553,13 +2614,13 @@
       <c r="J22" s="51">
         <v>108521</v>
       </c>
-      <c r="K22" s="91" t="s">
+      <c r="K22" s="79" t="s">
         <v>95</v>
       </c>
       <c r="L22" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M22" s="67">
+      <c r="M22" s="101">
         <v>103</v>
       </c>
       <c r="N22" s="67" t="s">
@@ -2594,14 +2655,14 @@
       <c r="J23" s="51">
         <v>108522</v>
       </c>
-      <c r="K23" s="91" t="s">
+      <c r="K23" s="79" t="s">
         <v>96</v>
       </c>
       <c r="L23" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M23" s="67">
-        <v>308</v>
+      <c r="M23" s="101">
+        <v>188</v>
       </c>
       <c r="N23" s="67" t="s">
         <v>195</v>
@@ -2639,13 +2700,13 @@
       <c r="J24" s="51">
         <v>110531</v>
       </c>
-      <c r="K24" s="92" t="s">
+      <c r="K24" s="80" t="s">
         <v>4</v>
       </c>
       <c r="L24" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M24" s="67">
+      <c r="M24" s="101">
         <v>112</v>
       </c>
       <c r="N24" s="67" t="s">
@@ -2684,7 +2745,7 @@
       <c r="J25" s="51">
         <v>110532</v>
       </c>
-      <c r="K25" s="88" t="s">
+      <c r="K25" s="76" t="s">
         <v>135</v>
       </c>
       <c r="L25" s="61" t="s">
@@ -2729,16 +2790,16 @@
       <c r="J26" s="51">
         <v>110533</v>
       </c>
-      <c r="K26" s="88" t="s">
+      <c r="K26" s="76" t="s">
         <v>136</v>
       </c>
       <c r="L26" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M26" s="67">
+      <c r="M26" s="101">
         <v>174</v>
       </c>
-      <c r="N26" s="67" t="s">
+      <c r="N26" s="99" t="s">
         <v>195</v>
       </c>
       <c r="O26" s="65"/>
@@ -2772,13 +2833,13 @@
       <c r="J27" s="51">
         <v>170521</v>
       </c>
-      <c r="K27" s="91" t="s">
+      <c r="K27" s="79" t="s">
         <v>98</v>
       </c>
       <c r="L27" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M27" s="67">
+      <c r="M27" s="101">
         <v>121</v>
       </c>
       <c r="N27" s="67" t="s">
@@ -2817,13 +2878,13 @@
       <c r="J28" s="51">
         <v>109521</v>
       </c>
-      <c r="K28" s="88" t="s">
+      <c r="K28" s="76" t="s">
         <v>137</v>
       </c>
       <c r="L28" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M28" s="67">
+      <c r="M28" s="100">
         <v>182</v>
       </c>
       <c r="N28" s="67" t="s">
@@ -2860,13 +2921,13 @@
       <c r="J29" s="51">
         <v>109522</v>
       </c>
-      <c r="K29" s="91" t="s">
+      <c r="K29" s="79" t="s">
         <v>99</v>
       </c>
       <c r="L29" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M29" s="67">
+      <c r="M29" s="69">
         <v>181</v>
       </c>
       <c r="N29" s="67" t="s">
@@ -2901,7 +2962,7 @@
       <c r="J30" s="51">
         <v>109523</v>
       </c>
-      <c r="K30" s="91" t="s">
+      <c r="K30" s="79" t="s">
         <v>100</v>
       </c>
       <c r="L30" s="61" t="s">
@@ -2942,13 +3003,13 @@
       <c r="J31" s="51">
         <v>157521</v>
       </c>
-      <c r="K31" s="91" t="s">
+      <c r="K31" s="79" t="s">
         <v>1</v>
       </c>
       <c r="L31" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M31" s="67">
+      <c r="M31" s="101">
         <v>110</v>
       </c>
       <c r="N31" s="67" t="s">
@@ -2985,13 +3046,13 @@
       <c r="J32" s="51">
         <v>109524</v>
       </c>
-      <c r="K32" s="91" t="s">
+      <c r="K32" s="79" t="s">
         <v>2</v>
       </c>
       <c r="L32" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M32" s="67">
+      <c r="M32" s="101">
         <v>105</v>
       </c>
       <c r="N32" s="67" t="s">
@@ -3024,13 +3085,13 @@
       <c r="J33" s="51">
         <v>109525</v>
       </c>
-      <c r="K33" s="91" t="s">
+      <c r="K33" s="79" t="s">
         <v>53</v>
       </c>
       <c r="L33" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M33" s="67">
+      <c r="M33" s="101">
         <v>187</v>
       </c>
       <c r="N33" s="67" t="s">
@@ -3065,13 +3126,13 @@
       <c r="J34" s="51">
         <v>155521</v>
       </c>
-      <c r="K34" s="88" t="s">
+      <c r="K34" s="76" t="s">
         <v>56</v>
       </c>
       <c r="L34" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M34" s="67">
+      <c r="M34" s="101">
         <v>179</v>
       </c>
       <c r="N34" s="67" t="s">
@@ -3079,7 +3140,7 @@
       </c>
       <c r="O34" s="65"/>
     </row>
-    <row r="35" spans="1:17" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" s="1" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A35" s="25"/>
       <c r="B35" s="26" t="s">
         <v>187</v>
@@ -3106,7 +3167,7 @@
       <c r="J35" s="53">
         <v>153521</v>
       </c>
-      <c r="K35" s="93" t="s">
+      <c r="K35" s="81" t="s">
         <v>0</v>
       </c>
       <c r="L35" s="63" t="s">
@@ -3120,7 +3181,7 @@
       </c>
       <c r="O35" s="65"/>
     </row>
-    <row r="36" spans="1:17" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" s="1" customFormat="1" ht="16.5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A36" s="25"/>
       <c r="B36" s="26" t="s">
         <v>187</v>
@@ -3147,7 +3208,7 @@
       <c r="J36" s="53">
         <v>150521</v>
       </c>
-      <c r="K36" s="93" t="s">
+      <c r="K36" s="81" t="s">
         <v>3</v>
       </c>
       <c r="L36" s="63" t="s">
@@ -3160,15 +3221,15 @@
         <v>195</v>
       </c>
       <c r="O36" s="65"/>
-      <c r="P36" s="95" t="s">
+      <c r="P36" s="83" t="s">
         <v>199</v>
       </c>
-      <c r="Q36" s="96">
+      <c r="Q36" s="84">
         <f>COUNTIF(N4:N38,"CERO")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" ht="16.5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A37" s="25"/>
       <c r="B37" s="26" t="s">
         <v>187</v>
@@ -3197,7 +3258,7 @@
       <c r="J37" s="53">
         <v>151521</v>
       </c>
-      <c r="K37" s="94" t="s">
+      <c r="K37" s="82" t="s">
         <v>138</v>
       </c>
       <c r="L37" s="63" t="s">
@@ -3210,15 +3271,15 @@
         <v>195</v>
       </c>
       <c r="O37" s="65"/>
-      <c r="P37" s="97" t="s">
+      <c r="P37" s="85" t="s">
         <v>196</v>
       </c>
-      <c r="Q37" s="98">
+      <c r="Q37" s="86">
         <f>COUNTIF(N4:N38,"OK")</f>
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" s="1" customFormat="1" ht="17.25" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="25"/>
       <c r="B38" s="26" t="s">
         <v>187</v>
@@ -3247,7 +3308,7 @@
       <c r="J38" s="53">
         <v>156521</v>
       </c>
-      <c r="K38" s="93" t="s">
+      <c r="K38" s="81" t="s">
         <v>55</v>
       </c>
       <c r="L38" s="63" t="s">
@@ -3260,15 +3321,15 @@
         <v>195</v>
       </c>
       <c r="O38" s="65"/>
-      <c r="P38" s="95" t="s">
+      <c r="P38" s="83" t="s">
         <v>197</v>
       </c>
-      <c r="Q38" s="98">
+      <c r="Q38" s="86">
         <f>COUNTIF(N4:N38,"FALTA")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A39" s="28"/>
       <c r="B39" s="29"/>
       <c r="C39" s="30"/>
@@ -3281,10 +3342,10 @@
       <c r="M39" s="5"/>
       <c r="N39" s="5"/>
       <c r="O39" s="59"/>
-      <c r="P39" s="97" t="s">
+      <c r="P39" s="85" t="s">
         <v>198</v>
       </c>
-      <c r="Q39" s="98">
+      <c r="Q39" s="86">
         <f>COUNTIF(N4:N38,"")</f>
         <v>0</v>
       </c>
@@ -3372,6 +3433,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
@@ -3380,15 +3450,6 @@
     <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3615,6 +3676,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -3622,14 +3691,6 @@
     <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
     <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
     <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
actualizacion de diseños de etiquetas
</commit_message>
<xml_diff>
--- a/Copia de Copia de Codigos CHABAT NICO.xlsx
+++ b/Copia de Copia de Codigos CHABAT NICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC184725-D631-4C20-AFB5-428E98B78061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{949B6029-2BC4-4F54-A753-9C63762B319F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -770,7 +770,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -792,12 +792,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1022,7 +1016,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1282,6 +1276,45 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1317,48 +1350,6 @@
     </xf>
     <xf numFmtId="44" fontId="4" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1654,8 +1645,8 @@
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M24" sqref="M24"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="61.5" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1663,9 +1654,9 @@
     <col min="1" max="1" width="7.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" style="5" customWidth="1"/>
     <col min="3" max="3" width="19.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" style="5" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="39" style="33" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="12.85546875" style="5" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.85546875" style="5" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="39" style="33" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="12.85546875" style="5" customWidth="1"/>
     <col min="7" max="7" width="11" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26.85546875" style="5" customWidth="1"/>
     <col min="9" max="9" width="16.7109375" style="4" customWidth="1"/>
@@ -1692,31 +1683,31 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="106" t="s">
         <v>122</v>
       </c>
       <c r="B2" s="7"/>
-      <c r="C2" s="87" t="s">
+      <c r="C2" s="100" t="s">
         <v>104</v>
       </c>
-      <c r="D2" s="91" t="s">
+      <c r="D2" s="104" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="91" t="s">
+      <c r="E2" s="104" t="s">
         <v>52</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-      <c r="H2" s="87" t="s">
+      <c r="H2" s="100" t="s">
         <v>113</v>
       </c>
-      <c r="I2" s="95" t="s">
+      <c r="I2" s="108" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="97" t="s">
+      <c r="J2" s="110" t="s">
         <v>123</v>
       </c>
-      <c r="K2" s="89" t="s">
+      <c r="K2" s="102" t="s">
         <v>20</v>
       </c>
       <c r="L2" s="2" t="s">
@@ -1729,25 +1720,25 @@
       </c>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="94"/>
+      <c r="A3" s="107"/>
       <c r="B3" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="88" t="s">
+      <c r="C3" s="101" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="92"/>
-      <c r="E3" s="92"/>
+      <c r="D3" s="105"/>
+      <c r="E3" s="105"/>
       <c r="F3" s="9" t="s">
         <v>105</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="H3" s="88"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="90"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="109"/>
+      <c r="J3" s="111"/>
+      <c r="K3" s="103"/>
       <c r="L3" s="60" t="s">
         <v>168</v>
       </c>
@@ -1801,7 +1792,7 @@
       <c r="L4" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M4" s="67">
+      <c r="M4" s="88">
         <v>171</v>
       </c>
       <c r="N4" s="67" t="s">
@@ -1851,7 +1842,7 @@
       <c r="L5" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M5" s="67">
+      <c r="M5" s="88">
         <v>170</v>
       </c>
       <c r="N5" s="67" t="s">
@@ -1894,8 +1885,8 @@
       <c r="L6" s="61" t="s">
         <v>173</v>
       </c>
-      <c r="M6" s="67">
-        <v>300</v>
+      <c r="M6" s="88">
+        <v>184</v>
       </c>
       <c r="N6" s="67" t="s">
         <v>195</v>
@@ -1941,7 +1932,7 @@
       <c r="L7" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M7" s="101">
+      <c r="M7" s="88">
         <v>100</v>
       </c>
       <c r="N7" s="67" t="s">
@@ -1952,47 +1943,47 @@
       </c>
     </row>
     <row r="8" spans="1:17" s="1" customFormat="1" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="102" t="s">
+      <c r="A8" s="89" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="103" t="s">
+      <c r="B8" s="90" t="s">
         <v>187</v>
       </c>
-      <c r="C8" s="104" t="s">
+      <c r="C8" s="91" t="s">
         <v>60</v>
       </c>
-      <c r="D8" s="105" t="s">
+      <c r="D8" s="92" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="106" t="s">
+      <c r="E8" s="93" t="s">
         <v>142</v>
       </c>
-      <c r="F8" s="104" t="s">
+      <c r="F8" s="91" t="s">
         <v>111</v>
       </c>
-      <c r="G8" s="104" t="s">
+      <c r="G8" s="91" t="s">
         <v>108</v>
       </c>
-      <c r="H8" s="104"/>
-      <c r="I8" s="107">
+      <c r="H8" s="91"/>
+      <c r="I8" s="94">
         <v>7290019570882</v>
       </c>
-      <c r="J8" s="108">
+      <c r="J8" s="95">
         <v>102532</v>
       </c>
-      <c r="K8" s="109" t="s">
+      <c r="K8" s="96" t="s">
         <v>125</v>
       </c>
-      <c r="L8" s="110" t="s">
+      <c r="L8" s="97" t="s">
         <v>169</v>
       </c>
-      <c r="M8" s="111">
+      <c r="M8" s="98">
         <v>301</v>
       </c>
-      <c r="N8" s="111" t="s">
+      <c r="N8" s="98" t="s">
         <v>195</v>
       </c>
-      <c r="O8" s="112" t="s">
+      <c r="O8" s="99" t="s">
         <v>190</v>
       </c>
     </row>
@@ -2033,7 +2024,7 @@
       <c r="L9" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M9" s="101">
+      <c r="M9" s="88">
         <v>352</v>
       </c>
       <c r="N9" s="67" t="s">
@@ -2080,7 +2071,7 @@
       <c r="L10" s="62" t="s">
         <v>169</v>
       </c>
-      <c r="M10" s="101">
+      <c r="M10" s="88">
         <v>130</v>
       </c>
       <c r="N10" s="68" t="s">
@@ -2130,7 +2121,7 @@
       <c r="L11" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M11" s="101">
+      <c r="M11" s="88">
         <v>353</v>
       </c>
       <c r="N11" s="67" t="s">
@@ -2175,7 +2166,7 @@
       <c r="L12" s="62" t="s">
         <v>169</v>
       </c>
-      <c r="M12" s="101">
+      <c r="M12" s="88">
         <v>172</v>
       </c>
       <c r="N12" s="73" t="s">
@@ -2225,7 +2216,7 @@
       <c r="L13" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M13" s="101">
+      <c r="M13" s="88">
         <v>354</v>
       </c>
       <c r="N13" s="67" t="s">
@@ -2270,7 +2261,7 @@
       <c r="L14" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M14" s="101">
+      <c r="M14" s="88">
         <v>104</v>
       </c>
       <c r="N14" s="67" t="s">
@@ -2315,7 +2306,7 @@
       <c r="L15" s="62" t="s">
         <v>169</v>
       </c>
-      <c r="M15" s="101">
+      <c r="M15" s="88">
         <v>355</v>
       </c>
       <c r="N15" s="68" t="s">
@@ -2358,7 +2349,7 @@
       <c r="L16" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M16" s="101">
+      <c r="M16" s="88">
         <v>356</v>
       </c>
       <c r="N16" s="67" t="s">
@@ -2401,7 +2392,7 @@
       <c r="L17" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M17" s="101">
+      <c r="M17" s="88">
         <v>111</v>
       </c>
       <c r="N17" s="67" t="s">
@@ -2446,7 +2437,7 @@
       <c r="L18" s="62" t="s">
         <v>169</v>
       </c>
-      <c r="M18" s="101">
+      <c r="M18" s="88">
         <v>173</v>
       </c>
       <c r="N18" s="68" t="s">
@@ -2489,7 +2480,7 @@
       <c r="L19" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M19" s="101">
+      <c r="M19" s="88">
         <v>101</v>
       </c>
       <c r="N19" s="67" t="s">
@@ -2532,7 +2523,7 @@
       <c r="L20" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M20" s="101">
+      <c r="M20" s="88">
         <v>102</v>
       </c>
       <c r="N20" s="67" t="s">
@@ -2575,7 +2566,7 @@
       <c r="L21" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M21" s="101">
+      <c r="M21" s="88">
         <v>120</v>
       </c>
       <c r="N21" s="67" t="s">
@@ -2620,7 +2611,7 @@
       <c r="L22" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M22" s="101">
+      <c r="M22" s="88">
         <v>103</v>
       </c>
       <c r="N22" s="67" t="s">
@@ -2661,7 +2652,7 @@
       <c r="L23" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M23" s="101">
+      <c r="M23" s="88">
         <v>188</v>
       </c>
       <c r="N23" s="67" t="s">
@@ -2706,7 +2697,7 @@
       <c r="L24" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M24" s="101">
+      <c r="M24" s="88">
         <v>112</v>
       </c>
       <c r="N24" s="67" t="s">
@@ -2751,8 +2742,8 @@
       <c r="L25" s="61" t="s">
         <v>173</v>
       </c>
-      <c r="M25" s="67">
-        <v>309</v>
+      <c r="M25" s="88">
+        <v>357</v>
       </c>
       <c r="N25" s="67" t="s">
         <v>195</v>
@@ -2796,10 +2787,10 @@
       <c r="L26" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M26" s="101">
+      <c r="M26" s="88">
         <v>174</v>
       </c>
-      <c r="N26" s="99" t="s">
+      <c r="N26" s="87" t="s">
         <v>195</v>
       </c>
       <c r="O26" s="65"/>
@@ -2839,7 +2830,7 @@
       <c r="L27" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M27" s="101">
+      <c r="M27" s="88">
         <v>121</v>
       </c>
       <c r="N27" s="67" t="s">
@@ -2884,8 +2875,8 @@
       <c r="L28" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M28" s="100">
-        <v>182</v>
+      <c r="M28" s="88">
+        <v>350</v>
       </c>
       <c r="N28" s="67" t="s">
         <v>195</v>
@@ -2927,7 +2918,7 @@
       <c r="L29" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M29" s="69">
+      <c r="M29" s="88">
         <v>181</v>
       </c>
       <c r="N29" s="67" t="s">
@@ -2968,8 +2959,8 @@
       <c r="L30" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M30" s="67">
-        <v>310</v>
+      <c r="M30" s="88">
+        <v>182</v>
       </c>
       <c r="N30" s="67" t="s">
         <v>195</v>
@@ -3009,7 +3000,7 @@
       <c r="L31" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M31" s="101">
+      <c r="M31" s="88">
         <v>110</v>
       </c>
       <c r="N31" s="67" t="s">
@@ -3052,7 +3043,7 @@
       <c r="L32" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M32" s="101">
+      <c r="M32" s="88">
         <v>105</v>
       </c>
       <c r="N32" s="67" t="s">
@@ -3091,7 +3082,7 @@
       <c r="L33" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M33" s="101">
+      <c r="M33" s="88">
         <v>187</v>
       </c>
       <c r="N33" s="67" t="s">
@@ -3132,7 +3123,7 @@
       <c r="L34" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="M34" s="101">
+      <c r="M34" s="88">
         <v>179</v>
       </c>
       <c r="N34" s="67" t="s">
@@ -3433,26 +3424,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="מסמך" ma:contentTypeID="0x010100E111FB68E4AB3A458E6F1E68F8888CED" ma:contentTypeVersion="13" ma:contentTypeDescription="צור מסמך חדש." ma:contentTypeScope="" ma:versionID="bfe1cfa8ea064de69b4e2203b8e1e509">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4613b05c-4671-4207-a6b8-e30994dce502" xmlns:ns3="ae89acfa-0242-4570-84ca-e3aafb74daca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b8d078cf0bd54969afc6a4d318ee940" ns2:_="" ns3:_="">
     <xsd:import namespace="4613b05c-4671-4207-a6b8-e30994dce502"/>
@@ -3675,10 +3646,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A9BCE7-9EE4-4695-9AF6-872741DC1E3D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
+    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3696,20 +3698,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A9BCE7-9EE4-4695-9AF6-872741DC1E3D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
-    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
guradando todos los cambios
</commit_message>
<xml_diff>
--- a/Copia de Copia de Codigos CHABAT NICO.xlsx
+++ b/Copia de Copia de Codigos CHABAT NICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{949B6029-2BC4-4F54-A753-9C63762B319F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B00CE6E-11D7-4D89-AF24-90A5119698B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$Q$43</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$Q$44</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$1:$L$38</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="205">
   <si>
     <t>לשון בקר קפוא</t>
   </si>
@@ -638,6 +638,21 @@
   </si>
   <si>
     <t>DE CERO</t>
+  </si>
+  <si>
+    <t>no hay entradas</t>
+  </si>
+  <si>
+    <t>AGUJA 2P PREMIUM</t>
+  </si>
+  <si>
+    <t>צלעות מיוחדות בקר קפוא</t>
+  </si>
+  <si>
+    <t>2P</t>
+  </si>
+  <si>
+    <t>ok</t>
   </si>
 </sst>
 </file>
@@ -648,7 +663,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -742,14 +757,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="48"/>
       <color theme="1"/>
@@ -769,8 +776,29 @@
       <name val="Cascadia Code"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="36"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -791,12 +819,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -807,8 +829,19 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -1009,14 +1042,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1045,51 +1103,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1117,33 +1130,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1168,27 +1154,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1198,12 +1172,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1216,105 +1184,151 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="2" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="2" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="2" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="3" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="13" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="10" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="13" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="13" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="16" fillId="6" borderId="13" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="10" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="16" fillId="6" borderId="13" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="16" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="14" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="10" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="10" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="16" fillId="6" borderId="10" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="10" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="16" fillId="6" borderId="10" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="1" fontId="16" fillId="6" borderId="9" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="10" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="9" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="9" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="1" fontId="16" fillId="6" borderId="9" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1351,8 +1365,40 @@
     <xf numFmtId="44" fontId="4" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="18" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
+    <cellStyle name="Bueno" xfId="4" builtinId="26"/>
     <cellStyle name="Millares" xfId="3" builtinId="3"/>
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1642,11 +1688,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q43"/>
+  <dimension ref="A1:Q44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M25" sqref="M25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="61.5" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1654,17 +1700,17 @@
     <col min="1" max="1" width="7.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" style="5" customWidth="1"/>
     <col min="3" max="3" width="19.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" style="5" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="39" style="33" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="12.85546875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" style="5" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="39" style="18" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="12.85546875" style="5" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="11" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26.85546875" style="5" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="11" style="50" customWidth="1"/>
-    <col min="11" max="11" width="28" style="72" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" style="26" customWidth="1"/>
+    <col min="11" max="11" width="75.42578125" style="40" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="12.42578125" style="4" customWidth="1"/>
-    <col min="15" max="15" width="18.28515625" style="58" customWidth="1"/>
+    <col min="15" max="15" width="18.28515625" style="30" customWidth="1"/>
     <col min="16" max="16" width="22.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="18" max="16384" width="11.42578125" style="4"/>
@@ -1676,1736 +1722,1772 @@
       </c>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
-      <c r="J1" s="49"/>
+      <c r="J1" s="25"/>
       <c r="K1" s="6"/>
       <c r="Q1" s="4" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="106" t="s">
+      <c r="A2" s="92" t="s">
         <v>122</v>
       </c>
       <c r="B2" s="7"/>
-      <c r="C2" s="100" t="s">
+      <c r="C2" s="86" t="s">
         <v>104</v>
       </c>
-      <c r="D2" s="104" t="s">
+      <c r="D2" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="104" t="s">
+      <c r="E2" s="90" t="s">
         <v>52</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-      <c r="H2" s="100" t="s">
+      <c r="H2" s="86" t="s">
         <v>113</v>
       </c>
-      <c r="I2" s="108" t="s">
+      <c r="I2" s="94" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="110" t="s">
+      <c r="J2" s="96" t="s">
         <v>123</v>
       </c>
-      <c r="K2" s="102" t="s">
+      <c r="K2" s="88" t="s">
         <v>20</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="Q2" s="56">
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="Q2" s="29">
         <v>45555</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="107"/>
+      <c r="A3" s="93"/>
       <c r="B3" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="101" t="s">
+      <c r="C3" s="87" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="105"/>
-      <c r="E3" s="105"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
       <c r="F3" s="9" t="s">
         <v>105</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="H3" s="101"/>
-      <c r="I3" s="109"/>
-      <c r="J3" s="111"/>
-      <c r="K3" s="103"/>
-      <c r="L3" s="60" t="s">
+      <c r="H3" s="87"/>
+      <c r="I3" s="95"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="32" t="s">
         <v>168</v>
       </c>
-      <c r="M3" s="66" t="s">
+      <c r="M3" s="36" t="s">
         <v>193</v>
       </c>
-      <c r="N3" s="66" t="s">
+      <c r="N3" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="O3" s="65" t="s">
+      <c r="O3" s="35" t="s">
         <v>189</v>
       </c>
       <c r="Q3" s="4" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="1" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:17" s="69" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="81" t="s">
         <v>171</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="82" t="s">
         <v>188</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="82" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="83" t="s">
         <v>139</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="82" t="s">
         <v>111</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="82" t="s">
         <v>107</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="82" t="s">
         <v>110</v>
       </c>
-      <c r="I4" s="12">
+      <c r="I4" s="77">
         <v>7290019570943</v>
       </c>
-      <c r="J4" s="51">
+      <c r="J4" s="65">
         <v>101861</v>
       </c>
-      <c r="K4" s="74" t="s">
+      <c r="K4" s="84" t="s">
         <v>91</v>
       </c>
-      <c r="L4" s="61" t="s">
+      <c r="L4" s="65" t="s">
         <v>169</v>
       </c>
-      <c r="M4" s="88">
+      <c r="M4" s="67">
         <v>171</v>
       </c>
       <c r="N4" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="O4" s="65">
+      <c r="O4" s="68">
         <v>171</v>
       </c>
-      <c r="Q4" s="57" t="s">
+      <c r="Q4" s="80" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
+    <row r="5" spans="1:17" s="69" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="75">
         <v>18</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="61" t="s">
         <v>187</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="72" t="s">
         <v>139</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="61" t="s">
         <v>172</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="77">
         <v>7290019570943</v>
       </c>
-      <c r="J5" s="51">
+      <c r="J5" s="65">
         <v>101862</v>
       </c>
-      <c r="K5" s="75" t="s">
+      <c r="K5" s="78" t="s">
         <v>91</v>
       </c>
-      <c r="L5" s="61" t="s">
+      <c r="L5" s="65" t="s">
         <v>169</v>
       </c>
-      <c r="M5" s="88">
+      <c r="M5" s="67">
         <v>170</v>
       </c>
       <c r="N5" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="O5" s="65">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="14" t="s">
+      <c r="O5" s="68" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" s="69" customFormat="1" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="75"/>
+      <c r="B6" s="61" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="D6" s="36"/>
-      <c r="E6" s="37" t="s">
+      <c r="D6" s="61"/>
+      <c r="E6" s="72" t="s">
         <v>140</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="61" t="s">
         <v>109</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="61" t="s">
         <v>59</v>
       </c>
-      <c r="I6" s="12">
+      <c r="I6" s="77">
         <v>7290019570899</v>
       </c>
-      <c r="J6" s="51">
+      <c r="J6" s="65">
         <v>101865</v>
       </c>
-      <c r="K6" s="75" t="s">
+      <c r="K6" s="78" t="s">
         <v>54</v>
       </c>
-      <c r="L6" s="61" t="s">
+      <c r="L6" s="65" t="s">
         <v>173</v>
       </c>
-      <c r="M6" s="88">
+      <c r="M6" s="67">
         <v>184</v>
       </c>
       <c r="N6" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="O6" s="65" t="s">
+      <c r="O6" s="68" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
+    <row r="7" spans="1:17" s="69" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="75">
         <v>2</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="61" t="s">
         <v>187</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="61" t="s">
         <v>66</v>
       </c>
-      <c r="D7" s="36" t="s">
+      <c r="D7" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="37" t="s">
+      <c r="E7" s="72" t="s">
         <v>141</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="61" t="s">
         <v>65</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="73">
         <v>7290019570882</v>
       </c>
-      <c r="J7" s="51">
+      <c r="J7" s="65">
         <v>102531</v>
       </c>
-      <c r="K7" s="76" t="s">
+      <c r="K7" s="74" t="s">
         <v>124</v>
       </c>
-      <c r="L7" s="61" t="s">
+      <c r="L7" s="65" t="s">
         <v>169</v>
       </c>
-      <c r="M7" s="88">
+      <c r="M7" s="67">
         <v>100</v>
       </c>
       <c r="N7" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="O7" s="65" t="s">
+      <c r="O7" s="68" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="8" spans="1:17" s="1" customFormat="1" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="89" t="s">
+      <c r="A8" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="90" t="s">
+      <c r="B8" s="48" t="s">
         <v>187</v>
       </c>
-      <c r="C8" s="91" t="s">
+      <c r="C8" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="D8" s="92" t="s">
+      <c r="D8" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="93" t="s">
+      <c r="E8" s="51" t="s">
         <v>142</v>
       </c>
-      <c r="F8" s="91" t="s">
+      <c r="F8" s="49" t="s">
         <v>111</v>
       </c>
-      <c r="G8" s="91" t="s">
+      <c r="G8" s="49" t="s">
         <v>108</v>
       </c>
-      <c r="H8" s="91"/>
-      <c r="I8" s="94">
+      <c r="H8" s="49"/>
+      <c r="I8" s="52">
         <v>7290019570882</v>
       </c>
-      <c r="J8" s="95">
+      <c r="J8" s="53">
         <v>102532</v>
       </c>
-      <c r="K8" s="96" t="s">
+      <c r="K8" s="54" t="s">
         <v>125</v>
       </c>
-      <c r="L8" s="97" t="s">
+      <c r="L8" s="55" t="s">
         <v>169</v>
       </c>
-      <c r="M8" s="98">
+      <c r="M8" s="56">
         <v>301</v>
       </c>
-      <c r="N8" s="98" t="s">
+      <c r="N8" s="56" t="s">
         <v>195</v>
       </c>
-      <c r="O8" s="99" t="s">
+      <c r="O8" s="57" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="1" customFormat="1" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
+    <row r="9" spans="1:17" s="69" customFormat="1" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="71" t="s">
         <v>187</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="61" t="s">
         <v>90</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="37" t="s">
+      <c r="E9" s="72" t="s">
         <v>143</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="H9" s="61" t="s">
         <v>63</v>
       </c>
-      <c r="I9" s="15">
+      <c r="I9" s="73">
         <v>7290019570882</v>
       </c>
-      <c r="J9" s="51">
+      <c r="J9" s="65">
         <v>102533</v>
       </c>
-      <c r="K9" s="76" t="s">
+      <c r="K9" s="74" t="s">
         <v>126</v>
       </c>
-      <c r="L9" s="61" t="s">
+      <c r="L9" s="65" t="s">
         <v>169</v>
       </c>
-      <c r="M9" s="88">
+      <c r="M9" s="67">
         <v>352</v>
       </c>
       <c r="N9" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="O9" s="65" t="s">
+      <c r="O9" s="68" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="18">
+    <row r="10" spans="1:17" s="69" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="70">
         <v>22</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="71" t="s">
         <v>187</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="D10" s="38" t="s">
+      <c r="D10" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="39" t="s">
+      <c r="E10" s="72" t="s">
         <v>144</v>
       </c>
-      <c r="F10" s="20" t="s">
+      <c r="F10" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="20" t="s">
+      <c r="G10" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="H10" s="20" t="s">
+      <c r="H10" s="61" t="s">
         <v>114</v>
       </c>
-      <c r="I10" s="21">
+      <c r="I10" s="73">
         <v>7290019570882</v>
       </c>
-      <c r="J10" s="52">
+      <c r="J10" s="65">
         <v>102534</v>
       </c>
-      <c r="K10" s="77" t="s">
+      <c r="K10" s="74" t="s">
         <v>97</v>
       </c>
-      <c r="L10" s="62" t="s">
+      <c r="L10" s="65" t="s">
         <v>169</v>
       </c>
-      <c r="M10" s="88">
+      <c r="M10" s="67">
         <v>130</v>
       </c>
-      <c r="N10" s="68" t="s">
+      <c r="N10" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="O10" s="65">
+      <c r="O10" s="68">
         <v>130</v>
       </c>
-      <c r="P10" s="1" t="s">
+      <c r="P10" s="69" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="1" customFormat="1" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
+    <row r="11" spans="1:17" s="69" customFormat="1" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="71" t="s">
         <v>187</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="D11" s="36" t="s">
+      <c r="D11" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="37" t="s">
+      <c r="E11" s="72" t="s">
         <v>145</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="H11" s="14" t="s">
+      <c r="H11" s="61" t="s">
         <v>115</v>
       </c>
-      <c r="I11" s="15">
+      <c r="I11" s="73">
         <v>7290019570875</v>
       </c>
-      <c r="J11" s="51">
+      <c r="J11" s="65">
         <v>103521</v>
       </c>
-      <c r="K11" s="76" t="s">
+      <c r="K11" s="74" t="s">
         <v>127</v>
       </c>
-      <c r="L11" s="61" t="s">
+      <c r="L11" s="65" t="s">
         <v>169</v>
       </c>
-      <c r="M11" s="88">
+      <c r="M11" s="67">
         <v>353</v>
       </c>
       <c r="N11" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="O11" s="65"/>
-    </row>
-    <row r="12" spans="1:17" s="1" customFormat="1" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18">
+      <c r="O11" s="68"/>
+    </row>
+    <row r="12" spans="1:17" s="69" customFormat="1" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="70">
         <v>33</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="71" t="s">
         <v>187</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="38" t="s">
+      <c r="D12" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="39" t="s">
+      <c r="E12" s="72" t="s">
         <v>144</v>
       </c>
-      <c r="F12" s="20" t="s">
+      <c r="F12" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="G12" s="20" t="s">
+      <c r="G12" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="H12" s="20" t="s">
+      <c r="H12" s="61" t="s">
         <v>174</v>
       </c>
-      <c r="I12" s="21">
+      <c r="I12" s="73">
         <v>7290019570875</v>
       </c>
-      <c r="J12" s="52">
+      <c r="J12" s="65">
         <v>103522</v>
       </c>
-      <c r="K12" s="78" t="s">
+      <c r="K12" s="74" t="s">
         <v>128</v>
       </c>
-      <c r="L12" s="62" t="s">
+      <c r="L12" s="65" t="s">
         <v>169</v>
       </c>
-      <c r="M12" s="88">
+      <c r="M12" s="67">
         <v>172</v>
       </c>
-      <c r="N12" s="73" t="s">
+      <c r="N12" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="O12" s="65">
+      <c r="O12" s="68">
         <v>172</v>
       </c>
-      <c r="P12" s="1" t="s">
+      <c r="P12" s="69" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="1" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
+    <row r="13" spans="1:17" s="69" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="71" t="s">
         <v>187</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="D13" s="36" t="s">
+      <c r="D13" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="37" t="s">
+      <c r="E13" s="72" t="s">
         <v>146</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H13" s="61" t="s">
         <v>67</v>
       </c>
-      <c r="I13" s="15">
+      <c r="I13" s="73">
         <v>7290019570875</v>
       </c>
-      <c r="J13" s="51">
+      <c r="J13" s="65">
         <v>103523</v>
       </c>
-      <c r="K13" s="76" t="s">
+      <c r="K13" s="74" t="s">
         <v>129</v>
       </c>
-      <c r="L13" s="61" t="s">
+      <c r="L13" s="65" t="s">
         <v>169</v>
       </c>
-      <c r="M13" s="88">
+      <c r="M13" s="67">
         <v>354</v>
       </c>
       <c r="N13" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="O13" s="65"/>
-    </row>
-    <row r="14" spans="1:17" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="16">
+      <c r="O13" s="68"/>
+    </row>
+    <row r="14" spans="1:17" s="69" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="70">
         <v>3</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="71" t="s">
         <v>187</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="D14" s="36" t="s">
+      <c r="D14" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="37" t="s">
+      <c r="E14" s="72" t="s">
         <v>147</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="H14" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="I14" s="15">
+      <c r="I14" s="73">
         <v>7290019570875</v>
       </c>
-      <c r="J14" s="51">
+      <c r="J14" s="65">
         <v>103524</v>
       </c>
-      <c r="K14" s="76" t="s">
+      <c r="K14" s="74" t="s">
         <v>130</v>
       </c>
-      <c r="L14" s="61" t="s">
+      <c r="L14" s="65" t="s">
         <v>169</v>
       </c>
-      <c r="M14" s="88">
+      <c r="M14" s="67">
         <v>104</v>
       </c>
       <c r="N14" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="O14" s="65"/>
-    </row>
-    <row r="15" spans="1:17" s="1" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18">
+      <c r="O14" s="68" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" s="69" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="70">
         <v>44</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="71" t="s">
         <v>187</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="61" t="s">
         <v>70</v>
       </c>
-      <c r="D15" s="38" t="s">
+      <c r="D15" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="39" t="s">
+      <c r="E15" s="72" t="s">
         <v>148</v>
       </c>
-      <c r="F15" s="20" t="s">
+      <c r="F15" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="G15" s="20" t="s">
+      <c r="G15" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="H15" s="20" t="s">
+      <c r="H15" s="61" t="s">
         <v>116</v>
       </c>
-      <c r="I15" s="21">
+      <c r="I15" s="73">
         <v>7290019570868</v>
       </c>
-      <c r="J15" s="52">
+      <c r="J15" s="65">
         <v>104521</v>
       </c>
-      <c r="K15" s="78" t="s">
+      <c r="K15" s="74" t="s">
         <v>131</v>
       </c>
-      <c r="L15" s="62" t="s">
+      <c r="L15" s="65" t="s">
         <v>169</v>
       </c>
-      <c r="M15" s="88">
+      <c r="M15" s="67">
         <v>355</v>
       </c>
-      <c r="N15" s="68" t="s">
+      <c r="N15" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="O15" s="65"/>
-    </row>
-    <row r="16" spans="1:17" s="1" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="O15" s="68"/>
+    </row>
+    <row r="16" spans="1:17" s="69" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="71" t="s">
         <v>187</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="61" t="s">
         <v>72</v>
       </c>
-      <c r="D16" s="36" t="s">
+      <c r="D16" s="61" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="37" t="s">
+      <c r="E16" s="72" t="s">
         <v>149</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="G16" s="14" t="s">
+      <c r="G16" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="H16" s="14"/>
-      <c r="I16" s="15">
+      <c r="H16" s="61"/>
+      <c r="I16" s="73">
         <v>7290019570868</v>
       </c>
-      <c r="J16" s="51">
+      <c r="J16" s="65">
         <v>104522</v>
       </c>
-      <c r="K16" s="76" t="s">
+      <c r="K16" s="74" t="s">
         <v>132</v>
       </c>
-      <c r="L16" s="61" t="s">
+      <c r="L16" s="65" t="s">
         <v>169</v>
       </c>
-      <c r="M16" s="88">
+      <c r="M16" s="67">
         <v>356</v>
       </c>
       <c r="N16" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="O16" s="65"/>
-    </row>
-    <row r="17" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="16">
+      <c r="O16" s="68"/>
+    </row>
+    <row r="17" spans="1:15" s="69" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="70">
         <v>4</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="71" t="s">
         <v>187</v>
       </c>
-      <c r="C17" s="55" t="s">
+      <c r="C17" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="D17" s="36" t="s">
+      <c r="D17" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="37" t="s">
+      <c r="E17" s="72" t="s">
         <v>150</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="F17" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="G17" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="H17" s="14"/>
-      <c r="I17" s="15">
+      <c r="H17" s="61"/>
+      <c r="I17" s="73">
         <v>7290019570868</v>
       </c>
-      <c r="J17" s="51">
+      <c r="J17" s="65">
         <v>104523</v>
       </c>
-      <c r="K17" s="76" t="s">
+      <c r="K17" s="74" t="s">
         <v>133</v>
       </c>
-      <c r="L17" s="61" t="s">
+      <c r="L17" s="65" t="s">
         <v>169</v>
       </c>
-      <c r="M17" s="88">
+      <c r="M17" s="67">
         <v>111</v>
       </c>
       <c r="N17" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="O17" s="65"/>
-    </row>
-    <row r="18" spans="1:15" s="1" customFormat="1" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="18">
+      <c r="O17" s="68"/>
+    </row>
+    <row r="18" spans="1:15" s="69" customFormat="1" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="70">
         <v>55</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="71" t="s">
         <v>187</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="61" t="s">
         <v>74</v>
       </c>
-      <c r="D18" s="38" t="s">
+      <c r="D18" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="E18" s="39" t="s">
+      <c r="E18" s="72" t="s">
         <v>151</v>
       </c>
-      <c r="F18" s="20" t="s">
+      <c r="F18" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="G18" s="20" t="s">
+      <c r="G18" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="H18" s="20" t="s">
+      <c r="H18" s="61" t="s">
         <v>117</v>
       </c>
-      <c r="I18" s="21">
+      <c r="I18" s="73">
         <v>7290019570851</v>
       </c>
-      <c r="J18" s="52">
+      <c r="J18" s="65">
         <v>105521</v>
       </c>
-      <c r="K18" s="78" t="s">
+      <c r="K18" s="74" t="s">
         <v>134</v>
       </c>
-      <c r="L18" s="62" t="s">
+      <c r="L18" s="65" t="s">
         <v>169</v>
       </c>
-      <c r="M18" s="88">
+      <c r="M18" s="67">
         <v>173</v>
       </c>
-      <c r="N18" s="68" t="s">
+      <c r="N18" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="O18" s="65"/>
-    </row>
-    <row r="19" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="13">
+      <c r="O18" s="68"/>
+    </row>
+    <row r="19" spans="1:15" s="69" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="75">
         <v>5</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="61" t="s">
         <v>187</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="61" t="s">
         <v>73</v>
       </c>
-      <c r="D19" s="36" t="s">
+      <c r="D19" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="37" t="s">
+      <c r="E19" s="72" t="s">
         <v>152</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="F19" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="G19" s="14" t="s">
+      <c r="G19" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="H19" s="14"/>
-      <c r="I19" s="15">
+      <c r="H19" s="61"/>
+      <c r="I19" s="73">
         <v>7290019570851</v>
       </c>
-      <c r="J19" s="51">
+      <c r="J19" s="65">
         <v>105522</v>
       </c>
-      <c r="K19" s="79" t="s">
+      <c r="K19" s="76" t="s">
         <v>92</v>
       </c>
-      <c r="L19" s="61" t="s">
+      <c r="L19" s="65" t="s">
         <v>169</v>
       </c>
-      <c r="M19" s="88">
+      <c r="M19" s="67">
         <v>101</v>
       </c>
       <c r="N19" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="O19" s="65"/>
-    </row>
-    <row r="20" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="13">
+      <c r="O19" s="68"/>
+    </row>
+    <row r="20" spans="1:15" s="69" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="75">
         <v>6</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="61" t="s">
         <v>187</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="61" t="s">
         <v>75</v>
       </c>
-      <c r="D20" s="36" t="s">
+      <c r="D20" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="37" t="s">
+      <c r="E20" s="72" t="s">
         <v>152</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="H20" s="14"/>
-      <c r="I20" s="15">
+      <c r="H20" s="61"/>
+      <c r="I20" s="73">
         <v>7290019570844</v>
       </c>
-      <c r="J20" s="51">
+      <c r="J20" s="65">
         <v>106521</v>
       </c>
-      <c r="K20" s="79" t="s">
+      <c r="K20" s="76" t="s">
         <v>93</v>
       </c>
-      <c r="L20" s="61" t="s">
+      <c r="L20" s="65" t="s">
         <v>169</v>
       </c>
-      <c r="M20" s="88">
+      <c r="M20" s="67">
         <v>102</v>
       </c>
       <c r="N20" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="O20" s="65"/>
-    </row>
-    <row r="21" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
+      <c r="O20" s="68"/>
+    </row>
+    <row r="21" spans="1:15" s="69" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="61" t="s">
         <v>187</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="61" t="s">
         <v>76</v>
       </c>
-      <c r="D21" s="36" t="s">
+      <c r="D21" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="E21" s="37" t="s">
+      <c r="E21" s="72" t="s">
         <v>153</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="F21" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="G21" s="14" t="s">
+      <c r="G21" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="H21" s="14"/>
-      <c r="I21" s="15">
+      <c r="H21" s="61"/>
+      <c r="I21" s="73">
         <v>7290019570837</v>
       </c>
-      <c r="J21" s="51">
+      <c r="J21" s="65">
         <v>107521</v>
       </c>
-      <c r="K21" s="79" t="s">
+      <c r="K21" s="76" t="s">
         <v>94</v>
       </c>
-      <c r="L21" s="61" t="s">
+      <c r="L21" s="65" t="s">
         <v>169</v>
       </c>
-      <c r="M21" s="88">
+      <c r="M21" s="67">
         <v>120</v>
       </c>
       <c r="N21" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="O21" s="65"/>
-    </row>
-    <row r="22" spans="1:15" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="13">
+      <c r="O21" s="68"/>
+    </row>
+    <row r="22" spans="1:15" s="69" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="75">
         <v>8</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="61" t="s">
         <v>187</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="61" t="s">
         <v>77</v>
       </c>
-      <c r="D22" s="36" t="s">
+      <c r="D22" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="37" t="s">
+      <c r="E22" s="72" t="s">
         <v>154</v>
       </c>
-      <c r="F22" s="14" t="s">
+      <c r="F22" s="61" t="s">
         <v>112</v>
       </c>
-      <c r="G22" s="14" t="s">
+      <c r="G22" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="H22" s="14" t="s">
+      <c r="H22" s="61" t="s">
         <v>178</v>
       </c>
-      <c r="I22" s="15">
+      <c r="I22" s="73">
         <v>7290019570820</v>
       </c>
-      <c r="J22" s="51">
+      <c r="J22" s="65">
         <v>108521</v>
       </c>
-      <c r="K22" s="79" t="s">
+      <c r="K22" s="76" t="s">
         <v>95</v>
       </c>
-      <c r="L22" s="61" t="s">
+      <c r="L22" s="65" t="s">
         <v>169</v>
       </c>
-      <c r="M22" s="88">
+      <c r="M22" s="67">
         <v>103</v>
       </c>
       <c r="N22" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="O22" s="65"/>
-    </row>
-    <row r="23" spans="1:15" s="1" customFormat="1" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
-      <c r="B23" s="23" t="s">
+      <c r="O22" s="68"/>
+    </row>
+    <row r="23" spans="1:15" s="69" customFormat="1" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="59"/>
+      <c r="B23" s="60" t="s">
         <v>187</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="61" t="s">
         <v>101</v>
       </c>
-      <c r="D23" s="40"/>
-      <c r="E23" s="41" t="s">
+      <c r="D23" s="60"/>
+      <c r="E23" s="63" t="s">
         <v>155</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="F23" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="G23" s="14" t="s">
+      <c r="G23" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="H23" s="14" t="s">
+      <c r="H23" s="61" t="s">
         <v>102</v>
       </c>
-      <c r="I23" s="24">
+      <c r="I23" s="64">
         <v>7290019570813</v>
       </c>
-      <c r="J23" s="51">
+      <c r="J23" s="65">
         <v>108522</v>
       </c>
-      <c r="K23" s="79" t="s">
+      <c r="K23" s="76" t="s">
         <v>96</v>
       </c>
-      <c r="L23" s="61" t="s">
+      <c r="L23" s="65" t="s">
         <v>169</v>
       </c>
-      <c r="M23" s="88">
+      <c r="M23" s="67">
         <v>188</v>
       </c>
       <c r="N23" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="O23" s="65"/>
-    </row>
-    <row r="24" spans="1:15" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="22" t="s">
+      <c r="O23" s="68"/>
+    </row>
+    <row r="24" spans="1:15" s="69" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="60" t="s">
         <v>187</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="61" t="s">
         <v>78</v>
       </c>
-      <c r="D24" s="42" t="s">
+      <c r="D24" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="41" t="s">
+      <c r="E24" s="63" t="s">
         <v>156</v>
       </c>
-      <c r="F24" s="14" t="s">
+      <c r="F24" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="G24" s="14" t="s">
+      <c r="G24" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="H24" s="14" t="s">
+      <c r="H24" s="61" t="s">
         <v>118</v>
       </c>
-      <c r="I24" s="24">
+      <c r="I24" s="64">
         <v>7290019570806</v>
       </c>
-      <c r="J24" s="51">
+      <c r="J24" s="65">
         <v>110531</v>
       </c>
-      <c r="K24" s="80" t="s">
+      <c r="K24" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="L24" s="61" t="s">
+      <c r="L24" s="65" t="s">
         <v>169</v>
       </c>
-      <c r="M24" s="88">
+      <c r="M24" s="67">
         <v>112</v>
       </c>
       <c r="N24" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="O24" s="65"/>
-    </row>
-    <row r="25" spans="1:15" s="1" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="16" t="s">
+      <c r="O24" s="68"/>
+    </row>
+    <row r="25" spans="1:15" s="69" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="71" t="s">
         <v>187</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="61" t="s">
         <v>78</v>
       </c>
-      <c r="D25" s="36" t="s">
+      <c r="D25" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="E25" s="37" t="s">
+      <c r="E25" s="72" t="s">
         <v>157</v>
       </c>
-      <c r="F25" s="14" t="s">
+      <c r="F25" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="G25" s="14" t="s">
+      <c r="G25" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="H25" s="14" t="s">
+      <c r="H25" s="61" t="s">
         <v>176</v>
       </c>
-      <c r="I25" s="15">
+      <c r="I25" s="73">
         <v>7290019570790</v>
       </c>
-      <c r="J25" s="51">
+      <c r="J25" s="65">
         <v>110532</v>
       </c>
-      <c r="K25" s="76" t="s">
+      <c r="K25" s="74" t="s">
         <v>135</v>
       </c>
-      <c r="L25" s="61" t="s">
+      <c r="L25" s="65" t="s">
         <v>173</v>
       </c>
-      <c r="M25" s="88">
+      <c r="M25" s="67">
         <v>357</v>
       </c>
       <c r="N25" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="O25" s="65"/>
-    </row>
-    <row r="26" spans="1:15" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="16">
+      <c r="O25" s="68"/>
+    </row>
+    <row r="26" spans="1:15" s="69" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="70">
         <v>10</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="71" t="s">
         <v>187</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="61" t="s">
         <v>79</v>
       </c>
-      <c r="D26" s="36" t="s">
+      <c r="D26" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="E26" s="37" t="s">
+      <c r="E26" s="72" t="s">
         <v>158</v>
       </c>
-      <c r="F26" s="14" t="s">
+      <c r="F26" s="61" t="s">
         <v>119</v>
       </c>
-      <c r="G26" s="14" t="s">
+      <c r="G26" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="H26" s="14" t="s">
+      <c r="H26" s="61" t="s">
         <v>177</v>
       </c>
-      <c r="I26" s="15">
+      <c r="I26" s="73">
         <v>7290019570790</v>
       </c>
-      <c r="J26" s="51">
+      <c r="J26" s="65">
         <v>110533</v>
       </c>
-      <c r="K26" s="76" t="s">
+      <c r="K26" s="74" t="s">
         <v>136</v>
       </c>
-      <c r="L26" s="61" t="s">
+      <c r="L26" s="65" t="s">
         <v>169</v>
       </c>
-      <c r="M26" s="88">
+      <c r="M26" s="67">
         <v>174</v>
       </c>
-      <c r="N26" s="87" t="s">
+      <c r="N26" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="O26" s="65"/>
-    </row>
-    <row r="27" spans="1:15" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
+      <c r="O26" s="68"/>
+    </row>
+    <row r="27" spans="1:15" s="69" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="61" t="s">
         <v>187</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="61" t="s">
         <v>80</v>
       </c>
-      <c r="D27" s="36" t="s">
+      <c r="D27" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="E27" s="37" t="s">
+      <c r="E27" s="72" t="s">
         <v>159</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F27" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="G27" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="H27" s="14"/>
-      <c r="I27" s="15">
+      <c r="H27" s="61"/>
+      <c r="I27" s="73">
         <v>7290019570783</v>
       </c>
-      <c r="J27" s="51">
+      <c r="J27" s="65">
         <v>170521</v>
       </c>
-      <c r="K27" s="79" t="s">
+      <c r="K27" s="76" t="s">
         <v>98</v>
       </c>
-      <c r="L27" s="61" t="s">
+      <c r="L27" s="65" t="s">
         <v>169</v>
       </c>
-      <c r="M27" s="88">
+      <c r="M27" s="67">
         <v>121</v>
       </c>
       <c r="N27" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="O27" s="65"/>
-    </row>
-    <row r="28" spans="1:15" s="1" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="16">
+      <c r="O27" s="68"/>
+    </row>
+    <row r="28" spans="1:15" s="69" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="70">
         <v>99</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="71" t="s">
         <v>187</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="61" t="s">
         <v>81</v>
       </c>
-      <c r="D28" s="36" t="s">
+      <c r="D28" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="E28" s="37" t="s">
+      <c r="E28" s="72" t="s">
         <v>160</v>
       </c>
-      <c r="F28" s="14" t="s">
+      <c r="F28" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="G28" s="14" t="s">
+      <c r="G28" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="H28" s="14" t="s">
+      <c r="H28" s="61" t="s">
         <v>179</v>
       </c>
-      <c r="I28" s="15">
+      <c r="I28" s="73">
         <v>7290019570776</v>
       </c>
-      <c r="J28" s="51">
+      <c r="J28" s="65">
         <v>109521</v>
       </c>
-      <c r="K28" s="76" t="s">
+      <c r="K28" s="74" t="s">
         <v>137</v>
       </c>
-      <c r="L28" s="61" t="s">
+      <c r="L28" s="65" t="s">
         <v>169</v>
       </c>
-      <c r="M28" s="88">
+      <c r="M28" s="67">
         <v>350</v>
       </c>
       <c r="N28" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="O28" s="65"/>
-    </row>
-    <row r="29" spans="1:15" s="1" customFormat="1" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="13">
+      <c r="O28" s="68"/>
+    </row>
+    <row r="29" spans="1:15" s="69" customFormat="1" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="75">
         <v>9</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="61" t="s">
         <v>187</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="61" t="s">
         <v>81</v>
       </c>
-      <c r="D29" s="36" t="s">
+      <c r="D29" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="E29" s="37" t="s">
+      <c r="E29" s="72" t="s">
         <v>161</v>
       </c>
-      <c r="F29" s="14" t="s">
+      <c r="F29" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="G29" s="14" t="s">
+      <c r="G29" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="H29" s="14"/>
-      <c r="I29" s="15">
+      <c r="H29" s="61"/>
+      <c r="I29" s="73">
         <v>7290019570776</v>
       </c>
-      <c r="J29" s="51">
+      <c r="J29" s="65">
         <v>109522</v>
       </c>
-      <c r="K29" s="79" t="s">
+      <c r="K29" s="76" t="s">
         <v>99</v>
       </c>
-      <c r="L29" s="61" t="s">
+      <c r="L29" s="65" t="s">
         <v>169</v>
       </c>
-      <c r="M29" s="88">
+      <c r="M29" s="67">
         <v>181</v>
       </c>
       <c r="N29" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="O29" s="65"/>
-    </row>
-    <row r="30" spans="1:15" s="1" customFormat="1" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
-      <c r="B30" s="14" t="s">
+      <c r="O29" s="68"/>
+    </row>
+    <row r="30" spans="1:15" s="69" customFormat="1" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="75"/>
+      <c r="B30" s="61" t="s">
         <v>187</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="61" t="s">
         <v>82</v>
       </c>
-      <c r="D30" s="36"/>
-      <c r="E30" s="37" t="s">
+      <c r="D30" s="61"/>
+      <c r="E30" s="72" t="s">
         <v>155</v>
       </c>
-      <c r="F30" s="14" t="s">
+      <c r="F30" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="G30" s="14" t="s">
+      <c r="G30" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="H30" s="14" t="s">
+      <c r="H30" s="61" t="s">
         <v>180</v>
       </c>
-      <c r="I30" s="15">
+      <c r="I30" s="73">
         <v>7290019570769</v>
       </c>
-      <c r="J30" s="51">
+      <c r="J30" s="65">
         <v>109523</v>
       </c>
-      <c r="K30" s="79" t="s">
+      <c r="K30" s="76" t="s">
         <v>100</v>
       </c>
-      <c r="L30" s="61" t="s">
+      <c r="L30" s="65" t="s">
         <v>169</v>
       </c>
-      <c r="M30" s="88">
+      <c r="M30" s="67">
         <v>182</v>
       </c>
       <c r="N30" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="O30" s="65"/>
-    </row>
-    <row r="31" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="13"/>
-      <c r="B31" s="14" t="s">
+      <c r="O30" s="68"/>
+    </row>
+    <row r="31" spans="1:15" s="69" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="75"/>
+      <c r="B31" s="61" t="s">
         <v>187</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="61" t="s">
         <v>120</v>
       </c>
-      <c r="D31" s="36" t="s">
+      <c r="D31" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="E31" s="37" t="s">
+      <c r="E31" s="72" t="s">
         <v>162</v>
       </c>
-      <c r="F31" s="14" t="s">
+      <c r="F31" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="G31" s="14" t="s">
+      <c r="G31" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="H31" s="14"/>
-      <c r="I31" s="15">
+      <c r="H31" s="61"/>
+      <c r="I31" s="73">
         <v>7290019570752</v>
       </c>
-      <c r="J31" s="51">
+      <c r="J31" s="65">
         <v>157521</v>
       </c>
-      <c r="K31" s="79" t="s">
+      <c r="K31" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="L31" s="61" t="s">
+      <c r="L31" s="65" t="s">
         <v>169</v>
       </c>
-      <c r="M31" s="88">
+      <c r="M31" s="67">
         <v>110</v>
       </c>
       <c r="N31" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="O31" s="65"/>
-    </row>
-    <row r="32" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="14" t="s">
+      <c r="O31" s="68"/>
+    </row>
+    <row r="32" spans="1:15" s="85" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B32" s="85" t="s">
         <v>187</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="85" t="s">
         <v>83</v>
       </c>
-      <c r="D32" s="36" t="s">
+      <c r="D32" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="E32" s="37" t="s">
+      <c r="E32" s="85" t="s">
         <v>163</v>
       </c>
-      <c r="F32" s="14" t="s">
+      <c r="F32" s="85" t="s">
         <v>111</v>
       </c>
-      <c r="G32" s="14" t="s">
+      <c r="G32" s="85" t="s">
         <v>108</v>
       </c>
-      <c r="H32" s="14" t="s">
+      <c r="H32" s="85" t="s">
         <v>114</v>
       </c>
-      <c r="I32" s="15">
+      <c r="I32" s="85">
         <v>7290019570745</v>
       </c>
-      <c r="J32" s="51">
+      <c r="J32" s="85">
         <v>109524</v>
       </c>
-      <c r="K32" s="79" t="s">
+      <c r="K32" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="L32" s="61" t="s">
+      <c r="L32" s="85" t="s">
         <v>169</v>
       </c>
-      <c r="M32" s="88">
+      <c r="M32" s="85">
         <v>105</v>
       </c>
-      <c r="N32" s="67" t="s">
+      <c r="N32" s="85" t="s">
         <v>195</v>
       </c>
-      <c r="O32" s="65"/>
-    </row>
-    <row r="33" spans="1:17" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="13"/>
-      <c r="B33" s="14" t="s">
+      <c r="O32" s="85" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" s="69" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="75"/>
+      <c r="B33" s="61" t="s">
         <v>187</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="61" t="s">
         <v>84</v>
       </c>
-      <c r="D33" s="36"/>
-      <c r="E33" s="37" t="s">
+      <c r="D33" s="61"/>
+      <c r="E33" s="72" t="s">
         <v>155</v>
       </c>
-      <c r="F33" s="14" t="s">
+      <c r="F33" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="G33" s="14" t="s">
+      <c r="G33" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="H33" s="14"/>
-      <c r="I33" s="15">
+      <c r="H33" s="61"/>
+      <c r="I33" s="73">
         <v>7290019570738</v>
       </c>
-      <c r="J33" s="51">
+      <c r="J33" s="65">
         <v>109525</v>
       </c>
-      <c r="K33" s="79" t="s">
+      <c r="K33" s="76" t="s">
         <v>53</v>
       </c>
-      <c r="L33" s="61" t="s">
+      <c r="L33" s="65" t="s">
         <v>169</v>
       </c>
-      <c r="M33" s="88">
+      <c r="M33" s="67">
         <v>187</v>
       </c>
       <c r="N33" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="O33" s="65"/>
-    </row>
-    <row r="34" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
-      <c r="B34" s="14" t="s">
+      <c r="O33" s="68"/>
+    </row>
+    <row r="34" spans="1:17" s="69" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="75"/>
+      <c r="B34" s="61" t="s">
         <v>187</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="61" t="s">
         <v>89</v>
       </c>
-      <c r="D34" s="36"/>
-      <c r="E34" s="37" t="s">
+      <c r="D34" s="61"/>
+      <c r="E34" s="72" t="s">
         <v>164</v>
       </c>
-      <c r="F34" s="14" t="s">
+      <c r="F34" s="61" t="s">
         <v>181</v>
       </c>
-      <c r="G34" s="14" t="s">
+      <c r="G34" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="H34" s="14" t="s">
+      <c r="H34" s="61" t="s">
         <v>182</v>
       </c>
-      <c r="I34" s="15">
+      <c r="I34" s="73">
         <v>7290019570684</v>
       </c>
-      <c r="J34" s="51">
+      <c r="J34" s="65">
         <v>155521</v>
       </c>
-      <c r="K34" s="76" t="s">
+      <c r="K34" s="74" t="s">
         <v>56</v>
       </c>
-      <c r="L34" s="61" t="s">
+      <c r="L34" s="65" t="s">
         <v>169</v>
       </c>
-      <c r="M34" s="88">
+      <c r="M34" s="67">
         <v>179</v>
       </c>
       <c r="N34" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="O34" s="65"/>
-    </row>
-    <row r="35" spans="1:17" s="1" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="25"/>
-      <c r="B35" s="26" t="s">
+      <c r="O34" s="68"/>
+    </row>
+    <row r="35" spans="1:17" s="1" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="10"/>
+      <c r="B35" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="C35" s="26" t="s">
+      <c r="C35" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="D35" s="43" t="s">
+      <c r="D35" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="E35" s="44" t="s">
+      <c r="E35" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="F35" s="26" t="s">
+      <c r="F35" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="G35" s="26" t="s">
+      <c r="G35" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="H35" s="26"/>
-      <c r="I35" s="27">
+      <c r="H35" s="11"/>
+      <c r="I35" s="12">
         <v>7290019570721</v>
       </c>
-      <c r="J35" s="53">
+      <c r="J35" s="27">
         <v>153521</v>
       </c>
-      <c r="K35" s="81" t="s">
+      <c r="K35" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="L35" s="63" t="s">
+      <c r="L35" s="33" t="s">
         <v>169</v>
       </c>
-      <c r="M35" s="69">
+      <c r="M35" s="46">
         <v>161</v>
       </c>
-      <c r="N35" s="69" t="s">
+      <c r="N35" s="37" t="s">
         <v>195</v>
       </c>
-      <c r="O35" s="65"/>
-    </row>
-    <row r="36" spans="1:17" s="1" customFormat="1" ht="16.5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="25"/>
-      <c r="B36" s="26" t="s">
+      <c r="O35" s="35"/>
+    </row>
+    <row r="36" spans="1:17" s="1" customFormat="1" ht="16.5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="10"/>
+      <c r="B36" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="C36" s="26" t="s">
+      <c r="C36" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="D36" s="43" t="s">
+      <c r="D36" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="E36" s="44" t="s">
+      <c r="E36" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="F36" s="26" t="s">
+      <c r="F36" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="G36" s="26" t="s">
+      <c r="G36" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="H36" s="26"/>
-      <c r="I36" s="27">
+      <c r="H36" s="11"/>
+      <c r="I36" s="12">
         <v>7290019570714</v>
       </c>
-      <c r="J36" s="53">
+      <c r="J36" s="27">
         <v>150521</v>
       </c>
-      <c r="K36" s="81" t="s">
+      <c r="K36" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="L36" s="63" t="s">
+      <c r="L36" s="33" t="s">
         <v>169</v>
       </c>
-      <c r="M36" s="69">
+      <c r="M36" s="46">
         <v>163</v>
       </c>
-      <c r="N36" s="69" t="s">
+      <c r="N36" s="37" t="s">
         <v>195</v>
       </c>
-      <c r="O36" s="65"/>
-      <c r="P36" s="83" t="s">
+      <c r="O36" s="35"/>
+      <c r="P36" s="42" t="s">
         <v>199</v>
       </c>
-      <c r="Q36" s="84">
+      <c r="Q36" s="43">
         <f>COUNTIF(N4:N38,"CERO")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="16.5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="25"/>
-      <c r="B37" s="26" t="s">
+    <row r="37" spans="1:17" s="69" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="75"/>
+      <c r="B37" s="61" t="s">
         <v>187</v>
       </c>
-      <c r="C37" s="26" t="s">
+      <c r="C37" s="61" t="s">
         <v>87</v>
       </c>
-      <c r="D37" s="43" t="s">
+      <c r="D37" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="E37" s="44" t="s">
+      <c r="E37" s="72" t="s">
         <v>164</v>
       </c>
-      <c r="F37" s="26" t="s">
+      <c r="F37" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="G37" s="26" t="s">
+      <c r="G37" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="H37" s="14" t="s">
+      <c r="H37" s="61" t="s">
         <v>114</v>
       </c>
-      <c r="I37" s="27">
+      <c r="I37" s="73">
         <v>7290019570707</v>
       </c>
-      <c r="J37" s="53">
+      <c r="J37" s="65">
         <v>151521</v>
       </c>
-      <c r="K37" s="82" t="s">
+      <c r="K37" s="74" t="s">
         <v>138</v>
       </c>
-      <c r="L37" s="63" t="s">
+      <c r="L37" s="65" t="s">
         <v>169</v>
       </c>
-      <c r="M37" s="69">
+      <c r="M37" s="67">
         <v>177</v>
       </c>
-      <c r="N37" s="69" t="s">
+      <c r="N37" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="O37" s="65"/>
-      <c r="P37" s="85" t="s">
+      <c r="O37" s="68"/>
+      <c r="P37" s="79" t="s">
         <v>196</v>
       </c>
-      <c r="Q37" s="86">
+      <c r="Q37" s="80">
         <f>COUNTIF(N4:N38,"OK")</f>
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="1" customFormat="1" ht="17.25" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="25"/>
-      <c r="B38" s="26" t="s">
+    <row r="38" spans="1:17" s="1" customFormat="1" ht="17.25" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="10"/>
+      <c r="B38" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="C38" s="26" t="s">
+      <c r="C38" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="D38" s="43" t="s">
+      <c r="D38" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="E38" s="44" t="s">
+      <c r="E38" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="F38" s="26" t="s">
+      <c r="F38" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="G38" s="26" t="s">
+      <c r="G38" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="H38" s="26" t="s">
+      <c r="H38" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="I38" s="27">
+      <c r="I38" s="12">
         <v>7290019570691</v>
       </c>
-      <c r="J38" s="53">
+      <c r="J38" s="27">
         <v>156521</v>
       </c>
-      <c r="K38" s="81" t="s">
+      <c r="K38" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="L38" s="63" t="s">
+      <c r="L38" s="33" t="s">
         <v>169</v>
       </c>
-      <c r="M38" s="70">
+      <c r="M38" s="58">
         <v>162</v>
       </c>
-      <c r="N38" s="70" t="s">
+      <c r="N38" s="38" t="s">
         <v>195</v>
       </c>
-      <c r="O38" s="65"/>
-      <c r="P38" s="83" t="s">
+      <c r="O38" s="35"/>
+      <c r="P38" s="42" t="s">
         <v>197</v>
       </c>
-      <c r="Q38" s="86">
+      <c r="Q38" s="45">
         <f>COUNTIF(N4:N38,"FALTA")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:17" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="28"/>
-      <c r="B39" s="29"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="45"/>
-      <c r="E39" s="46"/>
-      <c r="I39" s="5"/>
-      <c r="J39" s="5"/>
-      <c r="K39" s="71"/>
-      <c r="L39" s="5"/>
-      <c r="M39" s="5"/>
-      <c r="N39" s="5"/>
-      <c r="O39" s="59"/>
-      <c r="P39" s="85" t="s">
+    <row r="39" spans="1:17" s="1" customFormat="1" ht="90" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="98" t="s">
+        <v>203</v>
+      </c>
+      <c r="B39" s="99"/>
+      <c r="C39" s="106" t="s">
+        <v>201</v>
+      </c>
+      <c r="D39" s="100"/>
+      <c r="E39" s="101"/>
+      <c r="F39" s="99"/>
+      <c r="G39" s="99"/>
+      <c r="H39" s="99"/>
+      <c r="I39" s="107">
+        <v>7290019570677</v>
+      </c>
+      <c r="J39" s="102">
+        <v>102534</v>
+      </c>
+      <c r="K39" s="108" t="s">
+        <v>202</v>
+      </c>
+      <c r="L39" s="103"/>
+      <c r="M39" s="104">
+        <v>359</v>
+      </c>
+      <c r="N39" s="103" t="s">
+        <v>204</v>
+      </c>
+      <c r="O39" s="105"/>
+      <c r="P39" s="42"/>
+      <c r="Q39" s="45"/>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40" s="13"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="22"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="39"/>
+      <c r="L40" s="5"/>
+      <c r="M40" s="5"/>
+      <c r="N40" s="5"/>
+      <c r="O40" s="31"/>
+      <c r="P40" s="44" t="s">
         <v>198</v>
       </c>
-      <c r="Q39" s="86">
+      <c r="Q40" s="45">
         <f>COUNTIF(N4:N38,"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" s="45" t="s">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A41" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="B40" s="29"/>
-      <c r="C40" s="30"/>
-      <c r="D40" s="45"/>
-      <c r="E40" s="46"/>
-      <c r="I40" s="5"/>
-      <c r="J40" s="5"/>
-      <c r="K40" s="71"/>
-      <c r="L40" s="5"/>
-      <c r="O40" s="59"/>
-      <c r="P40" s="5"/>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A41" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="B41" s="29"/>
-      <c r="C41" s="30"/>
-      <c r="D41" s="45"/>
-      <c r="E41" s="46"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="22"/>
       <c r="I41" s="5"/>
       <c r="J41" s="5"/>
-      <c r="K41" s="71"/>
+      <c r="K41" s="39"/>
       <c r="L41" s="5"/>
-      <c r="M41" s="5"/>
-      <c r="N41"/>
-      <c r="O41" s="59"/>
+      <c r="O41" s="31"/>
       <c r="P41" s="5"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A42" s="45" t="s">
-        <v>49</v>
-      </c>
-      <c r="B42" s="29"/>
-      <c r="C42" s="30"/>
-      <c r="D42" s="45"/>
-      <c r="E42" s="46"/>
+      <c r="A42" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42" s="14"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="22"/>
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
-      <c r="K42" s="71"/>
+      <c r="K42" s="39"/>
       <c r="L42" s="5"/>
       <c r="M42" s="5"/>
-      <c r="N42" s="5"/>
-      <c r="O42" s="59"/>
+      <c r="N42"/>
+      <c r="O42" s="31"/>
       <c r="P42" s="5"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A43" s="54" t="s">
-        <v>51</v>
-      </c>
-      <c r="B43" s="31"/>
-      <c r="C43" s="32"/>
-      <c r="D43" s="47"/>
-      <c r="E43" s="48"/>
+      <c r="A43" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43" s="14"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="22"/>
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
-      <c r="K43" s="71"/>
+      <c r="K43" s="39"/>
       <c r="L43" s="5"/>
       <c r="M43" s="5"/>
       <c r="N43" s="5"/>
-      <c r="O43" s="59"/>
+      <c r="O43" s="31"/>
       <c r="P43" s="5"/>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A44" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44" s="16"/>
+      <c r="C44" s="17"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="24"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="39"/>
+      <c r="L44" s="5"/>
+      <c r="M44" s="5"/>
+      <c r="N44" s="5"/>
+      <c r="O44" s="31"/>
+      <c r="P44" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -3424,6 +3506,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="מסמך" ma:contentTypeID="0x010100E111FB68E4AB3A458E6F1E68F8888CED" ma:contentTypeVersion="13" ma:contentTypeDescription="צור מסמך חדש." ma:contentTypeScope="" ma:versionID="bfe1cfa8ea064de69b4e2203b8e1e509">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4613b05c-4671-4207-a6b8-e30994dce502" xmlns:ns3="ae89acfa-0242-4570-84ca-e3aafb74daca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b8d078cf0bd54969afc6a4d318ee940" ns2:_="" ns3:_="">
     <xsd:import namespace="4613b05c-4671-4207-a6b8-e30994dce502"/>
@@ -3646,17 +3739,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4613b05c-4671-4207-a6b8-e30994dce502">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="ae89acfa-0242-4570-84ca-e3aafb74daca" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3667,6 +3749,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
+    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
+    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A9BCE7-9EE4-4695-9AF6-872741DC1E3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3685,18 +3779,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cbbec6ca-1437-44ec-b95e-c44e536ab8fc"/>
-    <ds:schemaRef ds:uri="4613b05c-4671-4207-a6b8-e30994dce502"/>
-    <ds:schemaRef ds:uri="ae89acfa-0242-4570-84ca-e3aafb74daca"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
   <ds:schemaRefs>

</xml_diff>